<commit_message>
[05-03-2019] - Operational and comments added
</commit_message>
<xml_diff>
--- a/HAST_Inputs.xlsx
+++ b/HAST_Inputs.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="20730"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C53F86F3-952A-48A3-B886-F6421C380051}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9DE9883F-9F5D-4FBC-801A-D11EC6A0725C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="465" windowWidth="14805" windowHeight="7650" tabRatio="868" firstSheet="1" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="465" windowWidth="14805" windowHeight="7650" tabRatio="868" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cover Sheet" sheetId="10" r:id="rId1"/>
@@ -423,7 +423,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="467" uniqueCount="373">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="349" uniqueCount="301">
   <si>
     <t>Name</t>
   </si>
@@ -1242,264 +1242,21 @@
     <t>220 kV A1</t>
   </si>
   <si>
-    <t>110 kV A1</t>
-  </si>
-  <si>
-    <t>Clonshaugh 110 kV</t>
-  </si>
-  <si>
-    <t>Belcamp 220 kV</t>
-  </si>
-  <si>
-    <t>Belcamp</t>
-  </si>
-  <si>
-    <t>Clonshaugh</t>
-  </si>
-  <si>
-    <t>Finglas</t>
-  </si>
-  <si>
-    <t>Finglas 220 kV</t>
-  </si>
-  <si>
     <t>C:\Users\david\OneDrive - Power Systems Consultants Inc\Projects\PSPF010 - PQ expert\HAST\Working_GIT\</t>
   </si>
   <si>
-    <t>Belcamp 110 kV</t>
-  </si>
-  <si>
-    <t>220 kV B2</t>
-  </si>
-  <si>
     <t>Base_Case</t>
   </si>
   <si>
-    <t>Barnakyle 110 kV</t>
-  </si>
-  <si>
-    <t>Barnakyle</t>
-  </si>
-  <si>
-    <t>Blundelstown 110 kV</t>
-  </si>
-  <si>
-    <t>Corkagh 110 kV</t>
-  </si>
-  <si>
-    <t>Clonfad 110 kV</t>
-  </si>
-  <si>
-    <t>Cloghran 110 kV</t>
-  </si>
-  <si>
     <t>Clonee 220 kV</t>
   </si>
   <si>
-    <t>Derryiron 110 kV</t>
-  </si>
-  <si>
-    <t>Gillinstown 110 kV</t>
-  </si>
-  <si>
-    <t>Gallanstown 110 kV</t>
-  </si>
-  <si>
-    <t>Griffinrath 110 kV</t>
-  </si>
-  <si>
-    <t>Hawkinstown 110 kV</t>
-  </si>
-  <si>
-    <t>Harristown 110 kV</t>
-  </si>
-  <si>
-    <t>Inchicore 220 kV</t>
-  </si>
-  <si>
-    <t>Kilmahud 110 kV</t>
-  </si>
-  <si>
-    <t>Muckerstown 110 kV</t>
-  </si>
-  <si>
-    <t>Platin 110 kV</t>
-  </si>
-  <si>
-    <t>Snugborough 110 kV</t>
-  </si>
-  <si>
-    <t>Timahoe North 110 kV</t>
-  </si>
-  <si>
-    <t>Treascon 110 kV</t>
-  </si>
-  <si>
-    <t>Blundelstown</t>
-  </si>
-  <si>
-    <t>Corkagh</t>
-  </si>
-  <si>
-    <t>Clonfad</t>
-  </si>
-  <si>
-    <t>Cloghran</t>
-  </si>
-  <si>
     <t>Clonee</t>
   </si>
   <si>
-    <t>Cruiserath</t>
-  </si>
-  <si>
-    <t>Derryiron</t>
-  </si>
-  <si>
-    <t>Gillinstown</t>
-  </si>
-  <si>
-    <t>Gallanstown</t>
-  </si>
-  <si>
-    <t>Griffinrath</t>
-  </si>
-  <si>
-    <t>Hawkinstown</t>
-  </si>
-  <si>
-    <t>Harristown</t>
-  </si>
-  <si>
-    <t>Inchicore</t>
-  </si>
-  <si>
-    <t>Kilmahud</t>
-  </si>
-  <si>
-    <t>Muckerstown</t>
-  </si>
-  <si>
-    <t>Platin</t>
-  </si>
-  <si>
-    <t>Snugborough</t>
-  </si>
-  <si>
-    <t>Treascon</t>
-  </si>
-  <si>
-    <t>Timahoe North</t>
-  </si>
-  <si>
-    <t>220 kV B1</t>
-  </si>
-  <si>
-    <t>Cruiserath 220 kV</t>
-  </si>
-  <si>
-    <t>AIM 2017-MODEL-13072018-TAP_Clonshaugh</t>
-  </si>
-  <si>
     <t>Mutual</t>
   </si>
   <si>
-    <t>CDU2_FIN2_ckt1</t>
-  </si>
-  <si>
-    <t>Corduff</t>
-  </si>
-  <si>
-    <t>220 kV Finglas #1 CB</t>
-  </si>
-  <si>
-    <t>Open</t>
-  </si>
-  <si>
-    <t>220 kV Corduff #1 CB</t>
-  </si>
-  <si>
-    <t>NW2_FIN2_ckt1</t>
-  </si>
-  <si>
-    <t>North Wall</t>
-  </si>
-  <si>
-    <t>220 kV Finglas CB</t>
-  </si>
-  <si>
-    <t>220 kV North Wall CB</t>
-  </si>
-  <si>
-    <t>SHL2_FIN2_ckt1</t>
-  </si>
-  <si>
-    <t>Shellybanks</t>
-  </si>
-  <si>
-    <t>220 kV Finglas DL</t>
-  </si>
-  <si>
-    <t>220 kV Shellybanks CB</t>
-  </si>
-  <si>
-    <t>BEL1_CGH1_ckt1</t>
-  </si>
-  <si>
-    <t>110 kV Clonshaugh #1 CB</t>
-  </si>
-  <si>
-    <t>CB1</t>
-  </si>
-  <si>
-    <t>FIN2_BEL2_ckt1</t>
-  </si>
-  <si>
-    <t>220 kV Belcamp CB</t>
-  </si>
-  <si>
-    <t>CB4</t>
-  </si>
-  <si>
-    <t>SHL2_BEL2_ckt1</t>
-  </si>
-  <si>
-    <t>220 kV Belcamp DL</t>
-  </si>
-  <si>
-    <t>CB3</t>
-  </si>
-  <si>
-    <t>BEL2_BEL1_tx1</t>
-  </si>
-  <si>
-    <t>220 kV T1 CB</t>
-  </si>
-  <si>
-    <t>110 kV T1 CB</t>
-  </si>
-  <si>
-    <t>BEL1_NBY1_ckt1</t>
-  </si>
-  <si>
-    <t>110 kV Newbury #1 CB</t>
-  </si>
-  <si>
-    <t>Newbury</t>
-  </si>
-  <si>
-    <t>110 kV Grange CB</t>
-  </si>
-  <si>
-    <t>CGH1_Tap16</t>
-  </si>
-  <si>
-    <t>PBO1_C3T3</t>
-  </si>
-  <si>
-    <t>PBO1_C3</t>
-  </si>
-  <si>
     <t>1) Added in Functionality to run studies with a range of filter options</t>
   </si>
   <si>
@@ -1521,9 +1278,6 @@
     <t>Only a single filter will be included at a time</t>
   </si>
   <si>
-    <t>Result Name</t>
-  </si>
-  <si>
     <t>C-Type</t>
   </si>
   <si>
@@ -1546,6 +1300,36 @@
   </si>
   <si>
     <t>Number of Steps</t>
+  </si>
+  <si>
+    <t>T1</t>
+  </si>
+  <si>
+    <t>AIM 2017-MODEL-07022019-TAP_TEST</t>
+  </si>
+  <si>
+    <t>BC_CustDevs_CLOph3</t>
+  </si>
+  <si>
+    <t>SV 2.5GW E-250 M0 W1350</t>
+  </si>
+  <si>
+    <t>Bracetown 220 kV</t>
+  </si>
+  <si>
+    <t>Bracetown</t>
+  </si>
+  <si>
+    <t>220 kV A2</t>
+  </si>
+  <si>
+    <t>Filter Name</t>
+  </si>
+  <si>
+    <t>Fil_CLO2</t>
+  </si>
+  <si>
+    <t>Fil_BRA2</t>
   </si>
 </sst>
 </file>
@@ -2334,16 +2118,16 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>357</v>
+        <v>276</v>
       </c>
       <c r="B10" s="35" t="s">
-        <v>358</v>
+        <v>277</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>359</v>
+        <v>278</v>
       </c>
       <c r="D10" t="s">
-        <v>360</v>
+        <v>279</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -2365,8 +2149,8 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:F24"/>
   <sheetViews>
-    <sheetView topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2408,7 +2192,7 @@
         <v>33</v>
       </c>
       <c r="B5" s="27" t="s">
-        <v>278</v>
+        <v>271</v>
       </c>
       <c r="C5" s="25" t="s">
         <v>253</v>
@@ -2595,7 +2379,7 @@
         <v>235</v>
       </c>
       <c r="B22" s="22" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C22" s="21" t="s">
         <v>247</v>
@@ -2606,7 +2390,7 @@
         <v>236</v>
       </c>
       <c r="B23" s="22" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C23" s="21" t="s">
         <v>248</v>
@@ -2643,8 +2427,8 @@
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:D22"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2680,16 +2464,16 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>355</v>
+        <v>291</v>
       </c>
       <c r="B5" s="34" t="s">
-        <v>323</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>356</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>354</v>
+        <v>292</v>
+      </c>
+      <c r="C5" s="34" t="s">
+        <v>293</v>
+      </c>
+      <c r="D5" s="34" t="s">
+        <v>294</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -2807,7 +2591,7 @@
   <dimension ref="A1:AB165"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2963,7 +2747,7 @@
     </row>
     <row r="5" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
-        <v>281</v>
+        <v>272</v>
       </c>
       <c r="B5" s="5">
         <v>0</v>
@@ -2996,27 +2780,13 @@
       <c r="AB5" s="3"/>
     </row>
     <row r="6" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A6" s="3" t="s">
-        <v>325</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>326</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>327</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>328</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>276</v>
-      </c>
-      <c r="F6" s="3" t="s">
-        <v>329</v>
-      </c>
-      <c r="G6" s="3" t="s">
-        <v>328</v>
-      </c>
+      <c r="A6" s="3"/>
+      <c r="B6" s="3"/>
+      <c r="C6" s="3"/>
+      <c r="D6" s="3"/>
+      <c r="E6" s="3"/>
+      <c r="F6" s="3"/>
+      <c r="G6" s="3"/>
       <c r="H6" s="28"/>
       <c r="I6" s="28"/>
       <c r="J6" s="28"/>
@@ -3040,27 +2810,13 @@
       <c r="AB6" s="3"/>
     </row>
     <row r="7" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A7" s="3" t="s">
-        <v>330</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>331</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>332</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>328</v>
-      </c>
-      <c r="E7" s="3" t="s">
-        <v>276</v>
-      </c>
-      <c r="F7" s="3" t="s">
-        <v>333</v>
-      </c>
-      <c r="G7" s="3" t="s">
-        <v>328</v>
-      </c>
+      <c r="A7" s="3"/>
+      <c r="B7" s="3"/>
+      <c r="C7" s="3"/>
+      <c r="D7" s="3"/>
+      <c r="E7" s="3"/>
+      <c r="F7" s="3"/>
+      <c r="G7" s="3"/>
       <c r="H7" s="28"/>
       <c r="I7" s="28"/>
       <c r="J7" s="28"/>
@@ -3084,27 +2840,13 @@
       <c r="AB7" s="3"/>
     </row>
     <row r="8" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A8" s="3" t="s">
-        <v>334</v>
-      </c>
-      <c r="B8" s="3" t="s">
-        <v>335</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>336</v>
-      </c>
-      <c r="D8" s="3" t="s">
-        <v>328</v>
-      </c>
-      <c r="E8" s="3" t="s">
-        <v>276</v>
-      </c>
-      <c r="F8" s="3" t="s">
-        <v>337</v>
-      </c>
-      <c r="G8" s="3" t="s">
-        <v>328</v>
-      </c>
+      <c r="A8" s="3"/>
+      <c r="B8" s="3"/>
+      <c r="C8" s="3"/>
+      <c r="D8" s="3"/>
+      <c r="E8" s="3"/>
+      <c r="F8" s="3"/>
+      <c r="G8" s="3"/>
       <c r="H8" s="28"/>
       <c r="I8" s="28"/>
       <c r="J8" s="28"/>
@@ -3128,27 +2870,13 @@
       <c r="AB8" s="3"/>
     </row>
     <row r="9" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A9" s="3" t="s">
-        <v>338</v>
-      </c>
-      <c r="B9" s="3" t="s">
-        <v>274</v>
-      </c>
-      <c r="C9" s="3" t="s">
-        <v>339</v>
-      </c>
-      <c r="D9" s="3" t="s">
-        <v>328</v>
-      </c>
-      <c r="E9" s="3" t="s">
-        <v>275</v>
-      </c>
-      <c r="F9" s="3" t="s">
-        <v>340</v>
-      </c>
-      <c r="G9" s="3" t="s">
-        <v>328</v>
-      </c>
+      <c r="A9" s="3"/>
+      <c r="B9" s="3"/>
+      <c r="C9" s="3"/>
+      <c r="D9" s="3"/>
+      <c r="E9" s="3"/>
+      <c r="F9" s="3"/>
+      <c r="G9" s="3"/>
       <c r="H9" s="28"/>
       <c r="I9" s="28"/>
       <c r="J9" s="28"/>
@@ -3172,27 +2900,13 @@
       <c r="AB9" s="3"/>
     </row>
     <row r="10" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A10" s="3" t="s">
-        <v>341</v>
-      </c>
-      <c r="B10" s="3" t="s">
-        <v>276</v>
-      </c>
-      <c r="C10" s="3" t="s">
-        <v>342</v>
-      </c>
-      <c r="D10" s="3" t="s">
-        <v>328</v>
-      </c>
-      <c r="E10" s="3" t="s">
-        <v>274</v>
-      </c>
-      <c r="F10" s="3" t="s">
-        <v>343</v>
-      </c>
-      <c r="G10" s="3" t="s">
-        <v>328</v>
-      </c>
+      <c r="A10" s="3"/>
+      <c r="B10" s="3"/>
+      <c r="C10" s="3"/>
+      <c r="D10" s="3"/>
+      <c r="E10" s="3"/>
+      <c r="F10" s="3"/>
+      <c r="G10" s="3"/>
       <c r="H10" s="28"/>
       <c r="I10" s="28"/>
       <c r="J10" s="28"/>
@@ -3216,27 +2930,13 @@
       <c r="AB10" s="3"/>
     </row>
     <row r="11" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A11" s="3" t="s">
-        <v>344</v>
-      </c>
-      <c r="B11" s="3" t="s">
-        <v>335</v>
-      </c>
-      <c r="C11" s="3" t="s">
-        <v>345</v>
-      </c>
-      <c r="D11" s="3" t="s">
-        <v>328</v>
-      </c>
-      <c r="E11" s="3" t="s">
-        <v>274</v>
-      </c>
-      <c r="F11" s="3" t="s">
-        <v>346</v>
-      </c>
-      <c r="G11" s="3" t="s">
-        <v>328</v>
-      </c>
+      <c r="A11" s="3"/>
+      <c r="B11" s="3"/>
+      <c r="C11" s="3"/>
+      <c r="D11" s="3"/>
+      <c r="E11" s="3"/>
+      <c r="F11" s="3"/>
+      <c r="G11" s="3"/>
       <c r="H11" s="28"/>
       <c r="I11" s="28"/>
       <c r="J11" s="28"/>
@@ -3260,27 +2960,13 @@
       <c r="AB11" s="3"/>
     </row>
     <row r="12" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A12" s="3" t="s">
-        <v>347</v>
-      </c>
-      <c r="B12" s="3" t="s">
-        <v>274</v>
-      </c>
-      <c r="C12" s="3" t="s">
-        <v>348</v>
-      </c>
-      <c r="D12" s="3" t="s">
-        <v>328</v>
-      </c>
-      <c r="E12" s="3" t="s">
-        <v>274</v>
-      </c>
-      <c r="F12" s="3" t="s">
-        <v>349</v>
-      </c>
-      <c r="G12" s="3" t="s">
-        <v>328</v>
-      </c>
+      <c r="A12" s="3"/>
+      <c r="B12" s="3"/>
+      <c r="C12" s="3"/>
+      <c r="D12" s="3"/>
+      <c r="E12" s="3"/>
+      <c r="F12" s="3"/>
+      <c r="G12" s="3"/>
       <c r="H12" s="28"/>
       <c r="I12" s="28"/>
       <c r="J12" s="28"/>
@@ -3304,27 +2990,13 @@
       <c r="AB12" s="3"/>
     </row>
     <row r="13" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A13" s="3" t="s">
-        <v>350</v>
-      </c>
-      <c r="B13" s="3" t="s">
-        <v>274</v>
-      </c>
-      <c r="C13" s="3" t="s">
-        <v>351</v>
-      </c>
-      <c r="D13" s="3" t="s">
-        <v>328</v>
-      </c>
-      <c r="E13" s="3" t="s">
-        <v>352</v>
-      </c>
-      <c r="F13" s="3" t="s">
-        <v>353</v>
-      </c>
-      <c r="G13" s="3" t="s">
-        <v>328</v>
-      </c>
+      <c r="A13" s="3"/>
+      <c r="B13" s="3"/>
+      <c r="C13" s="3"/>
+      <c r="D13" s="3"/>
+      <c r="E13" s="3"/>
+      <c r="F13" s="3"/>
+      <c r="G13" s="3"/>
       <c r="H13" s="28"/>
       <c r="I13" s="28"/>
       <c r="J13" s="28"/>
@@ -6546,7 +6218,7 @@
   <dimension ref="A1:D103"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6572,25 +6244,25 @@
         <v>21</v>
       </c>
       <c r="D4" s="36" t="s">
-        <v>324</v>
+        <v>275</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>279</v>
+        <v>295</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>274</v>
+        <v>296</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>271</v>
+        <v>297</v>
       </c>
       <c r="D5" s="3" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="28" t="s">
+      <c r="A6" s="3" t="s">
         <v>273</v>
       </c>
       <c r="B6" s="3" t="s">
@@ -6604,312 +6276,136 @@
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="3" t="s">
-        <v>272</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>275</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>271</v>
-      </c>
-      <c r="D7" s="3" t="b">
-        <v>1</v>
-      </c>
+      <c r="A7" s="3"/>
+      <c r="B7" s="3"/>
+      <c r="C7" s="3"/>
+      <c r="D7" s="3"/>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="3" t="s">
-        <v>277</v>
-      </c>
-      <c r="B8" s="3" t="s">
-        <v>276</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>280</v>
-      </c>
-      <c r="D8" s="3" t="b">
-        <v>0</v>
-      </c>
+      <c r="A8" s="3"/>
+      <c r="B8" s="3"/>
+      <c r="C8" s="3"/>
+      <c r="D8" s="3"/>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="3" t="s">
-        <v>282</v>
-      </c>
-      <c r="B9" s="3" t="s">
-        <v>283</v>
-      </c>
-      <c r="C9" s="3" t="s">
-        <v>271</v>
-      </c>
-      <c r="D9" s="3" t="b">
-        <v>0</v>
-      </c>
+      <c r="A9" s="3"/>
+      <c r="B9" s="3"/>
+      <c r="C9" s="3"/>
+      <c r="D9" s="3"/>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="28" t="s">
-        <v>284</v>
-      </c>
-      <c r="B10" s="3" t="s">
-        <v>302</v>
-      </c>
-      <c r="C10" s="3" t="s">
-        <v>271</v>
-      </c>
-      <c r="D10" s="3" t="b">
-        <v>0</v>
-      </c>
+      <c r="A10" s="28"/>
+      <c r="B10" s="3"/>
+      <c r="C10" s="3"/>
+      <c r="D10" s="3"/>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="28" t="s">
-        <v>285</v>
-      </c>
-      <c r="B11" s="3" t="s">
-        <v>303</v>
-      </c>
-      <c r="C11" s="3" t="s">
-        <v>271</v>
-      </c>
-      <c r="D11" s="3" t="b">
-        <v>0</v>
-      </c>
+      <c r="A11" s="28"/>
+      <c r="B11" s="3"/>
+      <c r="C11" s="3"/>
+      <c r="D11" s="3"/>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="3" t="s">
-        <v>286</v>
-      </c>
-      <c r="B12" s="3" t="s">
-        <v>304</v>
-      </c>
-      <c r="C12" s="3" t="s">
-        <v>271</v>
-      </c>
-      <c r="D12" s="3" t="b">
-        <v>0</v>
-      </c>
+      <c r="A12" s="3"/>
+      <c r="B12" s="3"/>
+      <c r="C12" s="3"/>
+      <c r="D12" s="3"/>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="3" t="s">
-        <v>287</v>
-      </c>
-      <c r="B13" s="3" t="s">
-        <v>305</v>
-      </c>
-      <c r="C13" s="3" t="s">
-        <v>271</v>
-      </c>
-      <c r="D13" s="3" t="b">
-        <v>0</v>
-      </c>
+      <c r="A13" s="3"/>
+      <c r="B13" s="3"/>
+      <c r="C13" s="3"/>
+      <c r="D13" s="3"/>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="3" t="s">
-        <v>288</v>
-      </c>
-      <c r="B14" s="3" t="s">
-        <v>306</v>
-      </c>
-      <c r="C14" s="3" t="s">
-        <v>270</v>
-      </c>
-      <c r="D14" s="3" t="b">
-        <v>0</v>
-      </c>
+      <c r="A14" s="3"/>
+      <c r="B14" s="3"/>
+      <c r="C14" s="3"/>
+      <c r="D14" s="3"/>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="3" t="s">
-        <v>322</v>
-      </c>
-      <c r="B15" s="3" t="s">
-        <v>307</v>
-      </c>
-      <c r="C15" s="3" t="s">
-        <v>270</v>
-      </c>
-      <c r="D15" s="3" t="b">
-        <v>0</v>
-      </c>
+      <c r="A15" s="3"/>
+      <c r="B15" s="3"/>
+      <c r="C15" s="3"/>
+      <c r="D15" s="3"/>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="3" t="s">
-        <v>289</v>
-      </c>
-      <c r="B16" s="3" t="s">
-        <v>308</v>
-      </c>
-      <c r="C16" s="3" t="s">
-        <v>271</v>
-      </c>
-      <c r="D16" s="3" t="b">
-        <v>0</v>
-      </c>
+      <c r="A16" s="3"/>
+      <c r="B16" s="3"/>
+      <c r="C16" s="3"/>
+      <c r="D16" s="3"/>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="3" t="s">
-        <v>290</v>
-      </c>
-      <c r="B17" s="3" t="s">
-        <v>309</v>
-      </c>
-      <c r="C17" s="3" t="s">
-        <v>271</v>
-      </c>
-      <c r="D17" s="3" t="b">
-        <v>0</v>
-      </c>
+      <c r="A17" s="3"/>
+      <c r="B17" s="3"/>
+      <c r="C17" s="3"/>
+      <c r="D17" s="3"/>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="3" t="s">
-        <v>291</v>
-      </c>
-      <c r="B18" s="3" t="s">
-        <v>310</v>
-      </c>
-      <c r="C18" s="3" t="s">
-        <v>271</v>
-      </c>
-      <c r="D18" s="3" t="b">
-        <v>0</v>
-      </c>
+      <c r="A18" s="3"/>
+      <c r="B18" s="3"/>
+      <c r="C18" s="3"/>
+      <c r="D18" s="3"/>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="3" t="s">
-        <v>292</v>
-      </c>
-      <c r="B19" s="3" t="s">
-        <v>311</v>
-      </c>
-      <c r="C19" s="3" t="s">
-        <v>271</v>
-      </c>
-      <c r="D19" s="3" t="b">
-        <v>0</v>
-      </c>
+      <c r="A19" s="3"/>
+      <c r="B19" s="3"/>
+      <c r="C19" s="3"/>
+      <c r="D19" s="3"/>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="3" t="s">
-        <v>293</v>
-      </c>
-      <c r="B20" s="3" t="s">
-        <v>312</v>
-      </c>
-      <c r="C20" s="3" t="s">
-        <v>271</v>
-      </c>
-      <c r="D20" s="3" t="b">
-        <v>0</v>
-      </c>
+      <c r="A20" s="3"/>
+      <c r="B20" s="3"/>
+      <c r="C20" s="3"/>
+      <c r="D20" s="3"/>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="28" t="s">
-        <v>294</v>
-      </c>
-      <c r="B21" s="3" t="s">
-        <v>313</v>
-      </c>
-      <c r="C21" s="3" t="s">
-        <v>271</v>
-      </c>
-      <c r="D21" s="3" t="b">
-        <v>0</v>
-      </c>
+      <c r="A21" s="28"/>
+      <c r="B21" s="3"/>
+      <c r="C21" s="3"/>
+      <c r="D21" s="3"/>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="3" t="s">
-        <v>295</v>
-      </c>
-      <c r="B22" s="3" t="s">
-        <v>314</v>
-      </c>
-      <c r="C22" s="3" t="s">
-        <v>321</v>
-      </c>
-      <c r="D22" s="3" t="b">
-        <v>0</v>
-      </c>
+      <c r="A22" s="3"/>
+      <c r="B22" s="3"/>
+      <c r="C22" s="3"/>
+      <c r="D22" s="3"/>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" s="28" t="s">
-        <v>296</v>
-      </c>
-      <c r="B23" s="3" t="s">
-        <v>315</v>
-      </c>
-      <c r="C23" s="3" t="s">
-        <v>271</v>
-      </c>
-      <c r="D23" s="3" t="b">
-        <v>0</v>
-      </c>
+      <c r="A23" s="28"/>
+      <c r="B23" s="3"/>
+      <c r="C23" s="3"/>
+      <c r="D23" s="3"/>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" s="28" t="s">
-        <v>297</v>
-      </c>
-      <c r="B24" s="3" t="s">
-        <v>316</v>
-      </c>
-      <c r="C24" s="3" t="s">
-        <v>271</v>
-      </c>
-      <c r="D24" s="3" t="b">
-        <v>0</v>
-      </c>
+      <c r="A24" s="28"/>
+      <c r="B24" s="3"/>
+      <c r="C24" s="3"/>
+      <c r="D24" s="3"/>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" s="28" t="s">
-        <v>298</v>
-      </c>
-      <c r="B25" s="3" t="s">
-        <v>317</v>
-      </c>
-      <c r="C25" s="3" t="s">
-        <v>271</v>
-      </c>
-      <c r="D25" s="3" t="b">
-        <v>0</v>
-      </c>
+      <c r="A25" s="28"/>
+      <c r="B25" s="3"/>
+      <c r="C25" s="3"/>
+      <c r="D25" s="3"/>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26" s="28" t="s">
-        <v>299</v>
-      </c>
-      <c r="B26" s="3" t="s">
-        <v>318</v>
-      </c>
-      <c r="C26" s="3" t="s">
-        <v>271</v>
-      </c>
-      <c r="D26" s="3" t="b">
-        <v>0</v>
-      </c>
+      <c r="A26" s="28"/>
+      <c r="B26" s="3"/>
+      <c r="C26" s="3"/>
+      <c r="D26" s="3"/>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27" s="3" t="s">
-        <v>300</v>
-      </c>
-      <c r="B27" s="3" t="s">
-        <v>320</v>
-      </c>
-      <c r="C27" s="3" t="s">
-        <v>271</v>
-      </c>
-      <c r="D27" s="3" t="b">
-        <v>0</v>
-      </c>
+      <c r="A27" s="3"/>
+      <c r="B27" s="3"/>
+      <c r="C27" s="3"/>
+      <c r="D27" s="3"/>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A28" s="3" t="s">
-        <v>301</v>
-      </c>
-      <c r="B28" s="3" t="s">
-        <v>319</v>
-      </c>
-      <c r="C28" s="3" t="s">
-        <v>271</v>
-      </c>
-      <c r="D28" s="3" t="b">
-        <v>0</v>
-      </c>
+      <c r="A28" s="3"/>
+      <c r="B28" s="3"/>
+      <c r="C28" s="3"/>
+      <c r="D28" s="3"/>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="3"/>
@@ -7376,8 +6872,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D08D4187-8BE1-4B7A-A634-AC08177090E1}">
   <dimension ref="A1:L103"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L4" sqref="L4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7389,17 +6885,17 @@
   <sheetData>
     <row r="1" spans="1:12" ht="21" x14ac:dyDescent="0.35">
       <c r="A1" s="7" t="s">
-        <v>361</v>
+        <v>280</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>363</v>
+        <v>282</v>
       </c>
     </row>
     <row r="4" spans="1:12" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A4" s="26" t="s">
-        <v>364</v>
+        <v>298</v>
       </c>
       <c r="B4" s="26" t="s">
         <v>19</v>
@@ -7408,45 +6904,45 @@
         <v>21</v>
       </c>
       <c r="D4" s="26" t="s">
-        <v>362</v>
+        <v>281</v>
       </c>
       <c r="E4" s="36" t="s">
-        <v>366</v>
+        <v>284</v>
       </c>
       <c r="F4" s="36" t="s">
-        <v>367</v>
+        <v>285</v>
       </c>
       <c r="G4" s="36" t="s">
-        <v>372</v>
+        <v>290</v>
       </c>
       <c r="H4" s="36" t="s">
-        <v>368</v>
+        <v>286</v>
       </c>
       <c r="I4" s="36" t="s">
-        <v>369</v>
+        <v>287</v>
       </c>
       <c r="J4" s="36" t="s">
-        <v>372</v>
+        <v>290</v>
       </c>
       <c r="K4" s="36" t="s">
-        <v>370</v>
+        <v>288</v>
       </c>
       <c r="L4" s="36" t="s">
-        <v>371</v>
+        <v>289</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>279</v>
+        <v>299</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>274</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="D5" s="37" t="s">
-        <v>365</v>
+        <v>283</v>
       </c>
       <c r="E5" s="3">
         <v>10</v>
@@ -7458,10 +6954,10 @@
         <v>5</v>
       </c>
       <c r="H5" s="3">
-        <v>150</v>
+        <v>450</v>
       </c>
       <c r="I5" s="3">
-        <v>250</v>
+        <v>550</v>
       </c>
       <c r="J5" s="3">
         <v>5</v>
@@ -7470,22 +6966,46 @@
         <v>20</v>
       </c>
       <c r="L5" s="3">
-        <v>150</v>
+        <v>120</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A6" s="28"/>
-      <c r="B6" s="3"/>
-      <c r="C6" s="3"/>
-      <c r="D6" s="3"/>
-      <c r="E6" s="3"/>
-      <c r="F6" s="3"/>
-      <c r="G6" s="3"/>
-      <c r="H6" s="3"/>
-      <c r="I6" s="3"/>
-      <c r="J6" s="3"/>
-      <c r="K6" s="3"/>
-      <c r="L6" s="3"/>
+      <c r="A6" s="3" t="s">
+        <v>300</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>296</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>297</v>
+      </c>
+      <c r="D6" s="37" t="s">
+        <v>283</v>
+      </c>
+      <c r="E6" s="3">
+        <v>10</v>
+      </c>
+      <c r="F6" s="3">
+        <v>50</v>
+      </c>
+      <c r="G6" s="3">
+        <v>5</v>
+      </c>
+      <c r="H6" s="3">
+        <v>450</v>
+      </c>
+      <c r="I6" s="3">
+        <v>550</v>
+      </c>
+      <c r="J6" s="3">
+        <v>5</v>
+      </c>
+      <c r="K6" s="3">
+        <v>20</v>
+      </c>
+      <c r="L6" s="3">
+        <v>120</v>
+      </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="3"/>
@@ -8848,7 +8368,7 @@
   </sheetData>
   <autoFilter ref="A4:E103" xr:uid="{00000000-0009-0000-0000-000004000000}"/>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D5" xr:uid="{BEBEE289-74B6-45AF-B472-6AAD4F987537}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D5:D6" xr:uid="{BEBEE289-74B6-45AF-B472-6AAD4F987537}">
       <formula1>"C-Type, Single"</formula1>
     </dataValidation>
   </dataValidations>
@@ -9601,7 +9121,7 @@
   <dimension ref="A1:D20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9646,7 +9166,7 @@
         <v>166</v>
       </c>
       <c r="D6" s="14">
-        <v>3025</v>
+        <v>2000</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -9683,7 +9203,7 @@
       </c>
       <c r="D9">
         <f>D6</f>
-        <v>3025</v>
+        <v>2000</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -9695,7 +9215,7 @@
         <v>170</v>
       </c>
       <c r="D10">
-        <v>5</v>
+        <v>50</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -9733,7 +9253,7 @@
       </c>
       <c r="D13">
         <f>D6</f>
-        <v>3025</v>
+        <v>2000</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
@@ -9746,7 +9266,7 @@
       </c>
       <c r="D14">
         <f>D6/D5</f>
-        <v>60.5</v>
+        <v>40</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
@@ -10061,26 +9581,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
-  <documentManagement>
-    <iab7cdb7554d4997ae876b11632fa575 xmlns="3cada6dc-2705-46ed-bab2-0b2cd6d935ca">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </iab7cdb7554d4997ae876b11632fa575>
-    <TaxCatchAll xmlns="3cada6dc-2705-46ed-bab2-0b2cd6d935ca"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100C9B3B8AC64AC88418540180D602CE6AB" ma:contentTypeVersion="4" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="c03373d3e8f67dac2598d545e73c3e0f">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="3cada6dc-2705-46ed-bab2-0b2cd6d935ca" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="f693bfc3a603cfa0c3f0b58e702f3d19" ns2:_="">
     <xsd:import namespace="3cada6dc-2705-46ed-bab2-0b2cd6d935ca"/>
@@ -10232,7 +9732,45 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
+  <documentManagement>
+    <iab7cdb7554d4997ae876b11632fa575 xmlns="3cada6dc-2705-46ed-bab2-0b2cd6d935ca">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </iab7cdb7554d4997ae876b11632fa575>
+    <TaxCatchAll xmlns="3cada6dc-2705-46ed-bab2-0b2cd6d935ca"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2A5E1C23-6545-45A2-BF0C-826678B16173}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="3cada6dc-2705-46ed-bab2-0b2cd6d935ca"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FCC61AA8-C35E-4598-8617-08B80F018AC2}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
@@ -10248,28 +9786,10 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7B5D7682-109C-47ED-9D9D-D061E76CCAD3}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2A5E1C23-6545-45A2-BF0C-826678B16173}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="3cada6dc-2705-46ed-bab2-0b2cd6d935ca"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
[11-03-2019] - Minor tuning and improvements to log error reporting <pf.py> - Attempted script to control max no. processes but needs further development.
</commit_message>
<xml_diff>
--- a/HAST_Inputs.xlsx
+++ b/HAST_Inputs.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="20730"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9DE9883F-9F5D-4FBC-801A-D11EC6A0725C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0EC77AC-0B3E-4E7D-80D8-E188CACA070D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="465" windowWidth="14805" windowHeight="7650" tabRatio="868" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="465" windowWidth="14805" windowHeight="7650" tabRatio="868" firstSheet="1" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cover Sheet" sheetId="10" r:id="rId1"/>
@@ -277,7 +277,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 If set to TRUE then mutual impedance will be calculated from this node to other nodes.  Helps to improve study speed by setting to False</t>
@@ -411,7 +411,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 If set to TRUE then mutual impedance will be calculated from this node to other nodes.  Helps to improve study speed by setting to False</t>
@@ -423,7 +423,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="349" uniqueCount="301">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="373" uniqueCount="316">
   <si>
     <t>Name</t>
   </si>
@@ -1242,9 +1242,6 @@
     <t>220 kV A1</t>
   </si>
   <si>
-    <t>C:\Users\david\OneDrive - Power Systems Consultants Inc\Projects\PSPF010 - PQ expert\HAST\Working_GIT\</t>
-  </si>
-  <si>
     <t>Base_Case</t>
   </si>
   <si>
@@ -1302,12 +1299,6 @@
     <t>Number of Steps</t>
   </si>
   <si>
-    <t>T1</t>
-  </si>
-  <si>
-    <t>AIM 2017-MODEL-07022019-TAP_TEST</t>
-  </si>
-  <si>
     <t>BC_CustDevs_CLOph3</t>
   </si>
   <si>
@@ -1329,14 +1320,68 @@
     <t>Fil_CLO2</t>
   </si>
   <si>
-    <t>Fil_BRA2</t>
+    <t>SC1</t>
+  </si>
+  <si>
+    <t>AIM 2017-MODEL-07022019-TAP_CloneePh3</t>
+  </si>
+  <si>
+    <t>C:\Users\david\Desktop\</t>
+  </si>
+  <si>
+    <t>CLO2-CDU2-ckt1</t>
+  </si>
+  <si>
+    <t>220 kV Corduff CB</t>
+  </si>
+  <si>
+    <t>Open</t>
+  </si>
+  <si>
+    <t>Corduff</t>
+  </si>
+  <si>
+    <t>220 kV Clonee CB</t>
+  </si>
+  <si>
+    <t>WOO2-CDU2-ckt1</t>
+  </si>
+  <si>
+    <t>Woodland</t>
+  </si>
+  <si>
+    <t>220 kV Corduff #3 CB</t>
+  </si>
+  <si>
+    <t>220 kV Woodland #3 CB</t>
+  </si>
+  <si>
+    <t>WOO4_T4204</t>
+  </si>
+  <si>
+    <t>400 kV T4204 CB</t>
+  </si>
+  <si>
+    <t>220 kV T4204 CB</t>
+  </si>
+  <si>
+    <t>CDU2-CRU2-ckt1</t>
+  </si>
+  <si>
+    <t>220 kV Cruiserath #1 CB</t>
+  </si>
+  <si>
+    <t>Cruiserath</t>
+  </si>
+  <si>
+    <t>CB1</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1414,12 +1459,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <charset val="1"/>
     </font>
   </fonts>
   <fills count="3">
@@ -2118,16 +2157,16 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
+        <v>275</v>
+      </c>
+      <c r="B10" s="35" t="s">
         <v>276</v>
       </c>
-      <c r="B10" s="35" t="s">
+      <c r="C10" s="4" t="s">
         <v>277</v>
       </c>
-      <c r="C10" s="4" t="s">
+      <c r="D10" t="s">
         <v>278</v>
-      </c>
-      <c r="D10" t="s">
-        <v>279</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -2149,8 +2188,8 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:F24"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2192,7 +2231,7 @@
         <v>33</v>
       </c>
       <c r="B5" s="27" t="s">
-        <v>271</v>
+        <v>299</v>
       </c>
       <c r="C5" s="25" t="s">
         <v>253</v>
@@ -2427,8 +2466,8 @@
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:D22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B30" sqref="B30"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2464,16 +2503,16 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
+        <v>297</v>
+      </c>
+      <c r="B5" s="34" t="s">
+        <v>298</v>
+      </c>
+      <c r="C5" s="34" t="s">
+        <v>290</v>
+      </c>
+      <c r="D5" s="34" t="s">
         <v>291</v>
-      </c>
-      <c r="B5" s="34" t="s">
-        <v>292</v>
-      </c>
-      <c r="C5" s="34" t="s">
-        <v>293</v>
-      </c>
-      <c r="D5" s="34" t="s">
-        <v>294</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -2591,7 +2630,7 @@
   <dimension ref="A1:AB165"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2747,7 +2786,7 @@
     </row>
     <row r="5" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="B5" s="5">
         <v>0</v>
@@ -2780,13 +2819,27 @@
       <c r="AB5" s="3"/>
     </row>
     <row r="6" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A6" s="3"/>
-      <c r="B6" s="3"/>
-      <c r="C6" s="3"/>
-      <c r="D6" s="3"/>
-      <c r="E6" s="3"/>
-      <c r="F6" s="3"/>
-      <c r="G6" s="3"/>
+      <c r="A6" s="3" t="s">
+        <v>300</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>273</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>301</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>302</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>303</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>304</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>302</v>
+      </c>
       <c r="H6" s="28"/>
       <c r="I6" s="28"/>
       <c r="J6" s="28"/>
@@ -2810,13 +2863,27 @@
       <c r="AB6" s="3"/>
     </row>
     <row r="7" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A7" s="3"/>
-      <c r="B7" s="3"/>
-      <c r="C7" s="3"/>
-      <c r="D7" s="3"/>
-      <c r="E7" s="3"/>
-      <c r="F7" s="3"/>
-      <c r="G7" s="3"/>
+      <c r="A7" s="3" t="s">
+        <v>305</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>306</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>307</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>302</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>303</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>308</v>
+      </c>
+      <c r="G7" s="3" t="s">
+        <v>302</v>
+      </c>
       <c r="H7" s="28"/>
       <c r="I7" s="28"/>
       <c r="J7" s="28"/>
@@ -2840,13 +2907,27 @@
       <c r="AB7" s="3"/>
     </row>
     <row r="8" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A8" s="3"/>
-      <c r="B8" s="3"/>
-      <c r="C8" s="3"/>
-      <c r="D8" s="3"/>
-      <c r="E8" s="3"/>
-      <c r="F8" s="3"/>
-      <c r="G8" s="3"/>
+      <c r="A8" s="3" t="s">
+        <v>309</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>306</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>310</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>302</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>306</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>311</v>
+      </c>
+      <c r="G8" s="3" t="s">
+        <v>302</v>
+      </c>
       <c r="H8" s="28"/>
       <c r="I8" s="28"/>
       <c r="J8" s="28"/>
@@ -2870,13 +2951,27 @@
       <c r="AB8" s="3"/>
     </row>
     <row r="9" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A9" s="3"/>
-      <c r="B9" s="3"/>
-      <c r="C9" s="3"/>
-      <c r="D9" s="3"/>
-      <c r="E9" s="3"/>
-      <c r="F9" s="3"/>
-      <c r="G9" s="3"/>
+      <c r="A9" s="3" t="s">
+        <v>312</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>303</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>313</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>302</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>314</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>315</v>
+      </c>
+      <c r="G9" s="3" t="s">
+        <v>302</v>
+      </c>
       <c r="H9" s="28"/>
       <c r="I9" s="28"/>
       <c r="J9" s="28"/>
@@ -6218,7 +6313,7 @@
   <dimension ref="A1:D103"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="P13" sqref="P13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6244,18 +6339,18 @@
         <v>21</v>
       </c>
       <c r="D4" s="36" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>296</v>
+        <v>293</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
       <c r="D5" s="3" t="b">
         <v>1</v>
@@ -6263,10 +6358,10 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
+        <v>272</v>
+      </c>
+      <c r="B6" s="3" t="s">
         <v>273</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>274</v>
       </c>
       <c r="C6" s="3" t="s">
         <v>270</v>
@@ -6872,8 +6967,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D08D4187-8BE1-4B7A-A634-AC08177090E1}">
   <dimension ref="A1:L103"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J6" sqref="J6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6885,17 +6980,17 @@
   <sheetData>
     <row r="1" spans="1:12" ht="21" x14ac:dyDescent="0.35">
       <c r="A1" s="7" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
     </row>
     <row r="4" spans="1:12" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A4" s="26" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
       <c r="B4" s="26" t="s">
         <v>19</v>
@@ -6904,63 +6999,63 @@
         <v>21</v>
       </c>
       <c r="D4" s="26" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="E4" s="36" t="s">
+        <v>283</v>
+      </c>
+      <c r="F4" s="36" t="s">
         <v>284</v>
       </c>
-      <c r="F4" s="36" t="s">
+      <c r="G4" s="36" t="s">
+        <v>289</v>
+      </c>
+      <c r="H4" s="36" t="s">
         <v>285</v>
       </c>
-      <c r="G4" s="36" t="s">
-        <v>290</v>
-      </c>
-      <c r="H4" s="36" t="s">
+      <c r="I4" s="36" t="s">
         <v>286</v>
       </c>
-      <c r="I4" s="36" t="s">
+      <c r="J4" s="36" t="s">
+        <v>289</v>
+      </c>
+      <c r="K4" s="36" t="s">
         <v>287</v>
       </c>
-      <c r="J4" s="36" t="s">
-        <v>290</v>
-      </c>
-      <c r="K4" s="36" t="s">
+      <c r="L4" s="36" t="s">
         <v>288</v>
-      </c>
-      <c r="L4" s="36" t="s">
-        <v>289</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>299</v>
+        <v>296</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>270</v>
       </c>
       <c r="D5" s="37" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="E5" s="3">
-        <v>10</v>
+        <v>30</v>
       </c>
       <c r="F5" s="3">
-        <v>50</v>
+        <v>80</v>
       </c>
       <c r="G5" s="3">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H5" s="3">
-        <v>450</v>
+        <v>400</v>
       </c>
       <c r="I5" s="3">
-        <v>550</v>
+        <v>800</v>
       </c>
       <c r="J5" s="3">
-        <v>5</v>
+        <v>17</v>
       </c>
       <c r="K5" s="3">
         <v>20</v>
@@ -6970,42 +7065,18 @@
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A6" s="3" t="s">
-        <v>300</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>296</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>297</v>
-      </c>
-      <c r="D6" s="37" t="s">
-        <v>283</v>
-      </c>
-      <c r="E6" s="3">
-        <v>10</v>
-      </c>
-      <c r="F6" s="3">
-        <v>50</v>
-      </c>
-      <c r="G6" s="3">
-        <v>5</v>
-      </c>
-      <c r="H6" s="3">
-        <v>450</v>
-      </c>
-      <c r="I6" s="3">
-        <v>550</v>
-      </c>
-      <c r="J6" s="3">
-        <v>5</v>
-      </c>
-      <c r="K6" s="3">
-        <v>20</v>
-      </c>
-      <c r="L6" s="3">
-        <v>120</v>
-      </c>
+      <c r="A6" s="3"/>
+      <c r="B6" s="3"/>
+      <c r="C6" s="3"/>
+      <c r="D6" s="37"/>
+      <c r="E6" s="3"/>
+      <c r="F6" s="3"/>
+      <c r="G6" s="3"/>
+      <c r="H6" s="3"/>
+      <c r="I6" s="3"/>
+      <c r="J6" s="3"/>
+      <c r="K6" s="3"/>
+      <c r="L6" s="3"/>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="3"/>
@@ -9121,7 +9192,7 @@
   <dimension ref="A1:D20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9190,7 +9261,7 @@
         <v>168</v>
       </c>
       <c r="D8" s="14">
-        <v>50</v>
+        <v>100</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -9202,7 +9273,6 @@
         <v>169</v>
       </c>
       <c r="D9">
-        <f>D6</f>
         <v>2000</v>
       </c>
     </row>
@@ -9581,6 +9651,26 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
+  <documentManagement>
+    <iab7cdb7554d4997ae876b11632fa575 xmlns="3cada6dc-2705-46ed-bab2-0b2cd6d935ca">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </iab7cdb7554d4997ae876b11632fa575>
+    <TaxCatchAll xmlns="3cada6dc-2705-46ed-bab2-0b2cd6d935ca"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100C9B3B8AC64AC88418540180D602CE6AB" ma:contentTypeVersion="4" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="c03373d3e8f67dac2598d545e73c3e0f">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="3cada6dc-2705-46ed-bab2-0b2cd6d935ca" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="f693bfc3a603cfa0c3f0b58e702f3d19" ns2:_="">
     <xsd:import namespace="3cada6dc-2705-46ed-bab2-0b2cd6d935ca"/>
@@ -9732,27 +9822,31 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
-  <documentManagement>
-    <iab7cdb7554d4997ae876b11632fa575 xmlns="3cada6dc-2705-46ed-bab2-0b2cd6d935ca">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </iab7cdb7554d4997ae876b11632fa575>
-    <TaxCatchAll xmlns="3cada6dc-2705-46ed-bab2-0b2cd6d935ca"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7B5D7682-109C-47ED-9D9D-D061E76CCAD3}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FCC61AA8-C35E-4598-8617-08B80F018AC2}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="3cada6dc-2705-46ed-bab2-0b2cd6d935ca"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2A5E1C23-6545-45A2-BF0C-826678B16173}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -9768,28 +9862,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FCC61AA8-C35E-4598-8617-08B80F018AC2}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="3cada6dc-2705-46ed-bab2-0b2cd6d935ca"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7B5D7682-109C-47ED-9D9D-D061E76CCAD3}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
[14-03-2019] - Fine tuned results processing to include more detail
</commit_message>
<xml_diff>
--- a/HAST_Inputs.xlsx
+++ b/HAST_Inputs.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="20730"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0EC77AC-0B3E-4E7D-80D8-E188CACA070D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8663C527-8152-41F1-81B5-98141A2E4710}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="465" windowWidth="14805" windowHeight="7650" tabRatio="868" firstSheet="1" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="465" windowWidth="14805" windowHeight="7650" tabRatio="868" firstSheet="1" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cover Sheet" sheetId="10" r:id="rId1"/>
@@ -423,7 +423,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="373" uniqueCount="316">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="348" uniqueCount="303">
   <si>
     <t>Name</t>
   </si>
@@ -1275,9 +1275,6 @@
     <t>Only a single filter will be included at a time</t>
   </si>
   <si>
-    <t>C-Type</t>
-  </si>
-  <si>
     <t>Reactive Power Start</t>
   </si>
   <si>
@@ -1317,9 +1314,6 @@
     <t>Filter Name</t>
   </si>
   <si>
-    <t>Fil_CLO2</t>
-  </si>
-  <si>
     <t>SC1</t>
   </si>
   <si>
@@ -1342,39 +1336,6 @@
   </si>
   <si>
     <t>220 kV Clonee CB</t>
-  </si>
-  <si>
-    <t>WOO2-CDU2-ckt1</t>
-  </si>
-  <si>
-    <t>Woodland</t>
-  </si>
-  <si>
-    <t>220 kV Corduff #3 CB</t>
-  </si>
-  <si>
-    <t>220 kV Woodland #3 CB</t>
-  </si>
-  <si>
-    <t>WOO4_T4204</t>
-  </si>
-  <si>
-    <t>400 kV T4204 CB</t>
-  </si>
-  <si>
-    <t>220 kV T4204 CB</t>
-  </si>
-  <si>
-    <t>CDU2-CRU2-ckt1</t>
-  </si>
-  <si>
-    <t>220 kV Cruiserath #1 CB</t>
-  </si>
-  <si>
-    <t>Cruiserath</t>
-  </si>
-  <si>
-    <t>CB1</t>
   </si>
 </sst>
 </file>
@@ -2231,7 +2192,7 @@
         <v>33</v>
       </c>
       <c r="B5" s="27" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="C5" s="25" t="s">
         <v>253</v>
@@ -2467,7 +2428,7 @@
   <dimension ref="A1:D22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2503,16 +2464,16 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="B5" s="34" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="C5" s="34" t="s">
+        <v>289</v>
+      </c>
+      <c r="D5" s="34" t="s">
         <v>290</v>
-      </c>
-      <c r="D5" s="34" t="s">
-        <v>291</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -2630,7 +2591,7 @@
   <dimension ref="A1:AB165"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="A7" sqref="A7:G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2820,25 +2781,25 @@
     </row>
     <row r="6" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>273</v>
       </c>
       <c r="C6" s="3" t="s">
+        <v>299</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>300</v>
+      </c>
+      <c r="E6" s="3" t="s">
         <v>301</v>
       </c>
-      <c r="D6" s="3" t="s">
+      <c r="F6" s="3" t="s">
         <v>302</v>
       </c>
-      <c r="E6" s="3" t="s">
-        <v>303</v>
-      </c>
-      <c r="F6" s="3" t="s">
-        <v>304</v>
-      </c>
       <c r="G6" s="3" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="H6" s="28"/>
       <c r="I6" s="28"/>
@@ -2863,27 +2824,13 @@
       <c r="AB6" s="3"/>
     </row>
     <row r="7" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A7" s="3" t="s">
-        <v>305</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>306</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>307</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>302</v>
-      </c>
-      <c r="E7" s="3" t="s">
-        <v>303</v>
-      </c>
-      <c r="F7" s="3" t="s">
-        <v>308</v>
-      </c>
-      <c r="G7" s="3" t="s">
-        <v>302</v>
-      </c>
+      <c r="A7" s="3"/>
+      <c r="B7" s="3"/>
+      <c r="C7" s="3"/>
+      <c r="D7" s="3"/>
+      <c r="E7" s="3"/>
+      <c r="F7" s="3"/>
+      <c r="G7" s="3"/>
       <c r="H7" s="28"/>
       <c r="I7" s="28"/>
       <c r="J7" s="28"/>
@@ -2907,27 +2854,13 @@
       <c r="AB7" s="3"/>
     </row>
     <row r="8" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A8" s="3" t="s">
-        <v>309</v>
-      </c>
-      <c r="B8" s="3" t="s">
-        <v>306</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>310</v>
-      </c>
-      <c r="D8" s="3" t="s">
-        <v>302</v>
-      </c>
-      <c r="E8" s="3" t="s">
-        <v>306</v>
-      </c>
-      <c r="F8" s="3" t="s">
-        <v>311</v>
-      </c>
-      <c r="G8" s="3" t="s">
-        <v>302</v>
-      </c>
+      <c r="A8" s="3"/>
+      <c r="B8" s="3"/>
+      <c r="C8" s="3"/>
+      <c r="D8" s="3"/>
+      <c r="E8" s="3"/>
+      <c r="F8" s="3"/>
+      <c r="G8" s="3"/>
       <c r="H8" s="28"/>
       <c r="I8" s="28"/>
       <c r="J8" s="28"/>
@@ -2951,27 +2884,13 @@
       <c r="AB8" s="3"/>
     </row>
     <row r="9" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A9" s="3" t="s">
-        <v>312</v>
-      </c>
-      <c r="B9" s="3" t="s">
-        <v>303</v>
-      </c>
-      <c r="C9" s="3" t="s">
-        <v>313</v>
-      </c>
-      <c r="D9" s="3" t="s">
-        <v>302</v>
-      </c>
-      <c r="E9" s="3" t="s">
-        <v>314</v>
-      </c>
-      <c r="F9" s="3" t="s">
-        <v>315</v>
-      </c>
-      <c r="G9" s="3" t="s">
-        <v>302</v>
-      </c>
+      <c r="A9" s="3"/>
+      <c r="B9" s="3"/>
+      <c r="C9" s="3"/>
+      <c r="D9" s="3"/>
+      <c r="E9" s="3"/>
+      <c r="F9" s="3"/>
+      <c r="G9" s="3"/>
       <c r="H9" s="28"/>
       <c r="I9" s="28"/>
       <c r="J9" s="28"/>
@@ -6344,13 +6263,13 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
+        <v>291</v>
+      </c>
+      <c r="B5" s="3" t="s">
         <v>292</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="C5" s="3" t="s">
         <v>293</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>294</v>
       </c>
       <c r="D5" s="3" t="b">
         <v>1</v>
@@ -6967,8 +6886,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D08D4187-8BE1-4B7A-A634-AC08177090E1}">
   <dimension ref="A1:L103"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J6" sqref="J6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A5" sqref="A5:L5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6990,7 +6909,7 @@
     </row>
     <row r="4" spans="1:12" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A4" s="26" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="B4" s="26" t="s">
         <v>19</v>
@@ -7002,67 +6921,43 @@
         <v>280</v>
       </c>
       <c r="E4" s="36" t="s">
+        <v>282</v>
+      </c>
+      <c r="F4" s="36" t="s">
         <v>283</v>
       </c>
-      <c r="F4" s="36" t="s">
+      <c r="G4" s="36" t="s">
+        <v>288</v>
+      </c>
+      <c r="H4" s="36" t="s">
         <v>284</v>
       </c>
-      <c r="G4" s="36" t="s">
-        <v>289</v>
-      </c>
-      <c r="H4" s="36" t="s">
+      <c r="I4" s="36" t="s">
         <v>285</v>
       </c>
-      <c r="I4" s="36" t="s">
+      <c r="J4" s="36" t="s">
+        <v>288</v>
+      </c>
+      <c r="K4" s="36" t="s">
         <v>286</v>
       </c>
-      <c r="J4" s="36" t="s">
-        <v>289</v>
-      </c>
-      <c r="K4" s="36" t="s">
+      <c r="L4" s="36" t="s">
         <v>287</v>
       </c>
-      <c r="L4" s="36" t="s">
-        <v>288</v>
-      </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A5" s="3" t="s">
-        <v>296</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>273</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>270</v>
-      </c>
-      <c r="D5" s="37" t="s">
-        <v>282</v>
-      </c>
-      <c r="E5" s="3">
-        <v>30</v>
-      </c>
-      <c r="F5" s="3">
-        <v>80</v>
-      </c>
-      <c r="G5" s="3">
-        <v>6</v>
-      </c>
-      <c r="H5" s="3">
-        <v>400</v>
-      </c>
-      <c r="I5" s="3">
-        <v>800</v>
-      </c>
-      <c r="J5" s="3">
-        <v>17</v>
-      </c>
-      <c r="K5" s="3">
-        <v>20</v>
-      </c>
-      <c r="L5" s="3">
-        <v>120</v>
-      </c>
+      <c r="A5" s="3"/>
+      <c r="B5" s="3"/>
+      <c r="C5" s="3"/>
+      <c r="D5" s="37"/>
+      <c r="E5" s="3"/>
+      <c r="F5" s="3"/>
+      <c r="G5" s="3"/>
+      <c r="H5" s="3"/>
+      <c r="I5" s="3"/>
+      <c r="J5" s="3"/>
+      <c r="K5" s="3"/>
+      <c r="L5" s="3"/>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="3"/>
@@ -8454,8 +8349,8 @@
   <sheetPr codeName="Sheet6"/>
   <dimension ref="A1:G59"/>
   <sheetViews>
-    <sheetView topLeftCell="A28" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B51" sqref="B51"/>
+    <sheetView tabSelected="1" topLeftCell="A25" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D40" sqref="D40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9192,7 +9087,7 @@
   <dimension ref="A1:D20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9660,17 +9555,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
-  <documentManagement>
-    <iab7cdb7554d4997ae876b11632fa575 xmlns="3cada6dc-2705-46ed-bab2-0b2cd6d935ca">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </iab7cdb7554d4997ae876b11632fa575>
-    <TaxCatchAll xmlns="3cada6dc-2705-46ed-bab2-0b2cd6d935ca"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100C9B3B8AC64AC88418540180D602CE6AB" ma:contentTypeVersion="4" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="c03373d3e8f67dac2598d545e73c3e0f">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="3cada6dc-2705-46ed-bab2-0b2cd6d935ca" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="f693bfc3a603cfa0c3f0b58e702f3d19" ns2:_="">
     <xsd:import namespace="3cada6dc-2705-46ed-bab2-0b2cd6d935ca"/>
@@ -9822,6 +9706,17 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
+  <documentManagement>
+    <iab7cdb7554d4997ae876b11632fa575 xmlns="3cada6dc-2705-46ed-bab2-0b2cd6d935ca">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </iab7cdb7554d4997ae876b11632fa575>
+    <TaxCatchAll xmlns="3cada6dc-2705-46ed-bab2-0b2cd6d935ca"/>
+  </documentManagement>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7B5D7682-109C-47ED-9D9D-D061E76CCAD3}">
   <ds:schemaRefs>
@@ -9831,22 +9726,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FCC61AA8-C35E-4598-8617-08B80F018AC2}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="3cada6dc-2705-46ed-bab2-0b2cd6d935ca"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2A5E1C23-6545-45A2-BF0C-826678B16173}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -9862,4 +9741,20 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FCC61AA8-C35E-4598-8617-08B80F018AC2}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="3cada6dc-2705-46ed-bab2-0b2cd6d935ca"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
[19-03-2019] - Major changes to improve study case creation and processing speed [19-03-2019] - Running successfully for frequency sweep with Z1 and Z12 impedance but to run with Z12 needs to be run from PowerFactory
TODO: Develop to allow Z12 to be run from console.
</commit_message>
<xml_diff>
--- a/HAST_Inputs.xlsx
+++ b/HAST_Inputs.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="20730"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8663C527-8152-41F1-81B5-98141A2E4710}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23A3EFA6-2236-4963-A6EB-E4B7006F9201}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="465" windowWidth="14805" windowHeight="7650" tabRatio="868" firstSheet="1" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="465" windowWidth="14805" windowHeight="7650" tabRatio="868" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cover Sheet" sheetId="10" r:id="rId1"/>
@@ -2149,8 +2149,8 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:F24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2324,7 +2324,7 @@
         <v>232</v>
       </c>
       <c r="B17" s="22" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C17" s="21" t="s">
         <v>242</v>
@@ -2390,7 +2390,7 @@
         <v>236</v>
       </c>
       <c r="B23" s="22" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C23" s="21" t="s">
         <v>248</v>
@@ -8349,7 +8349,7 @@
   <sheetPr codeName="Sheet6"/>
   <dimension ref="A1:G59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="D40" sqref="D40"/>
     </sheetView>
   </sheetViews>
@@ -9087,7 +9087,7 @@
   <dimension ref="A1:D20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9546,15 +9546,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100C9B3B8AC64AC88418540180D602CE6AB" ma:contentTypeVersion="4" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="c03373d3e8f67dac2598d545e73c3e0f">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="3cada6dc-2705-46ed-bab2-0b2cd6d935ca" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="f693bfc3a603cfa0c3f0b58e702f3d19" ns2:_="">
     <xsd:import namespace="3cada6dc-2705-46ed-bab2-0b2cd6d935ca"/>
@@ -9706,7 +9697,7 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
   <documentManagement>
     <iab7cdb7554d4997ae876b11632fa575 xmlns="3cada6dc-2705-46ed-bab2-0b2cd6d935ca">
@@ -9717,15 +9708,16 @@
 </p:properties>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7B5D7682-109C-47ED-9D9D-D061E76CCAD3}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2A5E1C23-6545-45A2-BF0C-826678B16173}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -9743,7 +9735,7 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FCC61AA8-C35E-4598-8617-08B80F018AC2}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
@@ -9757,4 +9749,12 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7B5D7682-109C-47ED-9D9D-D061E76CCAD3}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
[01-04-2019] - Processing of results into DataFrame completed, now need to deal with extract. Main Task: - Adjust layout to align with HAST and inserting of graphs. - Need to consider how to deal with different data availability and produce some unit-test code
</commit_message>
<xml_diff>
--- a/HAST_Inputs.xlsx
+++ b/HAST_Inputs.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="20730"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23A3EFA6-2236-4963-A6EB-E4B7006F9201}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB8783B7-3AD6-42CB-B300-7498688340C3}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="465" windowWidth="14805" windowHeight="7650" tabRatio="868" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="465" windowWidth="14805" windowHeight="7650" tabRatio="868" firstSheet="1" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cover Sheet" sheetId="10" r:id="rId1"/>
@@ -1317,9 +1317,6 @@
     <t>SC1</t>
   </si>
   <si>
-    <t>AIM 2017-MODEL-07022019-TAP_CloneePh3</t>
-  </si>
-  <si>
     <t>C:\Users\david\Desktop\</t>
   </si>
   <si>
@@ -1336,6 +1333,9 @@
   </si>
   <si>
     <t>220 kV Clonee CB</t>
+  </si>
+  <si>
+    <t>AIM 2017-MODEL-07022019-TAP_TEST</t>
   </si>
 </sst>
 </file>
@@ -2149,7 +2149,7 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:F24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
@@ -2192,7 +2192,7 @@
         <v>33</v>
       </c>
       <c r="B5" s="27" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="C5" s="25" t="s">
         <v>253</v>
@@ -2324,7 +2324,7 @@
         <v>232</v>
       </c>
       <c r="B17" s="22" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C17" s="21" t="s">
         <v>242</v>
@@ -2428,7 +2428,7 @@
   <dimension ref="A1:D22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2467,7 +2467,7 @@
         <v>295</v>
       </c>
       <c r="B5" s="34" t="s">
-        <v>296</v>
+        <v>302</v>
       </c>
       <c r="C5" s="34" t="s">
         <v>289</v>
@@ -2591,7 +2591,7 @@
   <dimension ref="A1:AB165"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7:G9"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2781,25 +2781,25 @@
     </row>
     <row r="6" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>273</v>
       </c>
       <c r="C6" s="3" t="s">
+        <v>298</v>
+      </c>
+      <c r="D6" s="3" t="s">
         <v>299</v>
       </c>
-      <c r="D6" s="3" t="s">
+      <c r="E6" s="3" t="s">
         <v>300</v>
       </c>
-      <c r="E6" s="3" t="s">
+      <c r="F6" s="3" t="s">
         <v>301</v>
       </c>
-      <c r="F6" s="3" t="s">
-        <v>302</v>
-      </c>
       <c r="G6" s="3" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="H6" s="28"/>
       <c r="I6" s="28"/>
@@ -8350,7 +8350,7 @@
   <dimension ref="A1:G59"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D40" sqref="D40"/>
+      <selection activeCell="F25" sqref="F25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9086,8 +9086,8 @@
   <sheetPr codeName="Sheet7"/>
   <dimension ref="A1:D20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9156,7 +9156,7 @@
         <v>168</v>
       </c>
       <c r="D8" s="14">
-        <v>100</v>
+        <v>50</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -9168,7 +9168,7 @@
         <v>169</v>
       </c>
       <c r="D9">
-        <v>2000</v>
+        <v>2025</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -9180,7 +9180,7 @@
         <v>170</v>
       </c>
       <c r="D10">
-        <v>50</v>
+        <v>5</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -9329,7 +9329,7 @@
   <dimension ref="A1:D19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
[11-04-2019] - Updated to ensure that multiple study cases can be handled when producing frequency scan results
</commit_message>
<xml_diff>
--- a/HAST_Inputs.xlsx
+++ b/HAST_Inputs.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="20730"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB8783B7-3AD6-42CB-B300-7498688340C3}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA2FB174-B75D-469A-887C-E8056A7616AB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="465" windowWidth="14805" windowHeight="7650" tabRatio="868" firstSheet="1" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="465" windowWidth="14805" windowHeight="7650" tabRatio="868" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cover Sheet" sheetId="10" r:id="rId1"/>
@@ -423,7 +423,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="348" uniqueCount="303">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="352" uniqueCount="305">
   <si>
     <t>Name</t>
   </si>
@@ -1336,6 +1336,12 @@
   </si>
   <si>
     <t>AIM 2017-MODEL-07022019-TAP_TEST</t>
+  </si>
+  <si>
+    <t>SC2</t>
+  </si>
+  <si>
+    <t>WP 6.7GW E150 M0 W0</t>
   </si>
 </sst>
 </file>
@@ -2149,8 +2155,8 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:F24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2324,7 +2330,7 @@
         <v>232</v>
       </c>
       <c r="B17" s="22" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C17" s="21" t="s">
         <v>242</v>
@@ -2428,7 +2434,7 @@
   <dimension ref="A1:D22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2477,10 +2483,18 @@
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="3"/>
-      <c r="B6" s="34"/>
-      <c r="C6" s="3"/>
-      <c r="D6" s="3"/>
+      <c r="A6" s="3" t="s">
+        <v>303</v>
+      </c>
+      <c r="B6" s="34" t="s">
+        <v>302</v>
+      </c>
+      <c r="C6" s="34" t="s">
+        <v>289</v>
+      </c>
+      <c r="D6" s="34" t="s">
+        <v>304</v>
+      </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="3"/>
@@ -2590,8 +2604,8 @@
   <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:AB165"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="E37" sqref="E37:E39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9086,8 +9100,8 @@
   <sheetPr codeName="Sheet7"/>
   <dimension ref="A1:D20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9132,7 +9146,7 @@
         <v>166</v>
       </c>
       <c r="D6" s="14">
-        <v>2000</v>
+        <v>1025</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -9168,7 +9182,8 @@
         <v>169</v>
       </c>
       <c r="D9">
-        <v>2025</v>
+        <f>D6</f>
+        <v>1025</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -9218,7 +9233,7 @@
       </c>
       <c r="D13">
         <f>D6</f>
-        <v>2000</v>
+        <v>1025</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
@@ -9231,7 +9246,7 @@
       </c>
       <c r="D14">
         <f>D6/D5</f>
-        <v>40</v>
+        <v>20.5</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
[26-04-2019] - Updated to better handle long names for terminals
</commit_message>
<xml_diff>
--- a/HAST_Inputs.xlsx
+++ b/HAST_Inputs.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="20730"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9F21FB0-DCC3-448E-81E5-47D3523E15E1}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{752EE76F-2F52-4041-97C2-FF8EC6960087}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="465" windowWidth="14805" windowHeight="7650" tabRatio="868" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="465" windowWidth="14805" windowHeight="7650" tabRatio="868" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cover Sheet" sheetId="10" r:id="rId1"/>
@@ -206,7 +206,7 @@
           </rPr>
           <t xml:space="preserve">
 Name of the station 
-Must be unique in the column</t>
+Must be unique in the column and have total length less than 19 characters</t>
         </r>
       </text>
     </comment>
@@ -423,7 +423,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="356" uniqueCount="307">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="389" uniqueCount="307">
   <si>
     <t>Name</t>
   </si>
@@ -1434,7 +1434,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1444,6 +1444,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1616,7 +1622,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1701,13 +1707,46 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="4">
+    <dxf>
+      <font>
+        <color theme="6"/>
+      </font>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="6"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -2161,7 +2200,7 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:F24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
@@ -6259,8 +6298,8 @@
   <sheetPr codeName="Sheet5"/>
   <dimension ref="A1:D103"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="P13" sqref="P13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6275,6 +6314,12 @@
         <v>24</v>
       </c>
     </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="46" t="str">
+        <f t="array" ref="A3">IF(LEN(A5:A103)&gt;19,"NAME LONG", "NAMES OKAY")</f>
+        <v>NAMES OKAY</v>
+      </c>
+    </row>
     <row r="4" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A4" s="26" t="s">
         <v>0</v>
@@ -6904,6 +6949,16 @@
   <sortState ref="A5:A8">
     <sortCondition ref="A5:A8"/>
   </sortState>
+  <conditionalFormatting sqref="A5:A103">
+    <cfRule type="expression" dxfId="3" priority="3">
+      <formula>LEN(A5)&gt;19</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A3">
+    <cfRule type="expression" dxfId="2" priority="1">
+      <formula>A3="NAMES OKAY"</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <legacyDrawing r:id="rId2"/>
@@ -9575,6 +9630,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100C9B3B8AC64AC88418540180D602CE6AB" ma:contentTypeVersion="4" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="c03373d3e8f67dac2598d545e73c3e0f">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="3cada6dc-2705-46ed-bab2-0b2cd6d935ca" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="f693bfc3a603cfa0c3f0b58e702f3d19" ns2:_="">
     <xsd:import namespace="3cada6dc-2705-46ed-bab2-0b2cd6d935ca"/>
@@ -9726,15 +9790,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
   <documentManagement>
@@ -9747,6 +9802,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7B5D7682-109C-47ED-9D9D-D061E76CCAD3}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2A5E1C23-6545-45A2-BF0C-826678B16173}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -9760,14 +9823,6 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7B5D7682-109C-47ED-9D9D-D061E76CCAD3}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
Added ability to create a folder somewhere else if issues creating results folder in target location
</commit_message>
<xml_diff>
--- a/HAST_Inputs.xlsx
+++ b/HAST_Inputs.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="20730"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{752EE76F-2F52-4041-97C2-FF8EC6960087}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8113F58-57B1-4C91-BEB2-DCA0952F6AC8}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="465" windowWidth="14805" windowHeight="7650" tabRatio="868" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="465" windowWidth="14805" windowHeight="7650" tabRatio="868" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cover Sheet" sheetId="10" r:id="rId1"/>
@@ -423,7 +423,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="389" uniqueCount="307">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="356" uniqueCount="307">
   <si>
     <t>Name</t>
   </si>
@@ -1317,9 +1317,6 @@
     <t>SC1</t>
   </si>
   <si>
-    <t>C:\Users\david\Desktop\</t>
-  </si>
-  <si>
     <t>CLO2-CDU2-ckt1</t>
   </si>
   <si>
@@ -1348,6 +1345,9 @@
   </si>
   <si>
     <t>AIM 2017-MODEL-07022019-TAP_TEST2</t>
+  </si>
+  <si>
+    <t>D:\Users\david\Desktop\</t>
   </si>
 </sst>
 </file>
@@ -1683,6 +1683,9 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="2"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1707,28 +1710,13 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
   </cellStyles>
-  <dxfs count="4">
-    <dxf>
-      <font>
-        <color theme="6"/>
-      </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="2">
     <dxf>
       <font>
         <color theme="6"/>
@@ -2200,8 +2188,8 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:F24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2221,11 +2209,11 @@
       <c r="A2" s="7"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="D3" s="38" t="s">
+      <c r="D3" s="39" t="s">
         <v>227</v>
       </c>
-      <c r="E3" s="38"/>
-      <c r="F3" s="38"/>
+      <c r="E3" s="39"/>
+      <c r="F3" s="39"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D4" t="s">
@@ -2243,7 +2231,7 @@
         <v>33</v>
       </c>
       <c r="B5" s="27" t="s">
-        <v>296</v>
+        <v>306</v>
       </c>
       <c r="C5" s="25" t="s">
         <v>253</v>
@@ -2518,7 +2506,7 @@
         <v>295</v>
       </c>
       <c r="B5" s="34" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="C5" s="34" t="s">
         <v>289</v>
@@ -2529,24 +2517,24 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="B6" s="34" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="C6" s="34" t="s">
         <v>289</v>
       </c>
       <c r="D6" s="34" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
+        <v>304</v>
+      </c>
+      <c r="B7" s="34" t="s">
         <v>305</v>
-      </c>
-      <c r="B7" s="34" t="s">
-        <v>306</v>
       </c>
       <c r="C7" s="34" t="s">
         <v>289</v>
@@ -2680,51 +2668,51 @@
     </row>
     <row r="2" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="3" spans="1:28" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="42" t="s">
+      <c r="B3" s="43" t="s">
         <v>10</v>
       </c>
-      <c r="C3" s="43"/>
-      <c r="D3" s="44"/>
-      <c r="E3" s="39" t="s">
+      <c r="C3" s="44"/>
+      <c r="D3" s="45"/>
+      <c r="E3" s="40" t="s">
         <v>11</v>
       </c>
-      <c r="F3" s="40"/>
-      <c r="G3" s="41"/>
-      <c r="H3" s="39" t="s">
+      <c r="F3" s="41"/>
+      <c r="G3" s="42"/>
+      <c r="H3" s="40" t="s">
         <v>12</v>
       </c>
-      <c r="I3" s="40"/>
-      <c r="J3" s="41"/>
-      <c r="K3" s="39" t="s">
+      <c r="I3" s="41"/>
+      <c r="J3" s="42"/>
+      <c r="K3" s="40" t="s">
         <v>13</v>
       </c>
-      <c r="L3" s="40"/>
-      <c r="M3" s="41"/>
-      <c r="N3" s="39" t="s">
+      <c r="L3" s="41"/>
+      <c r="M3" s="42"/>
+      <c r="N3" s="40" t="s">
         <v>14</v>
       </c>
-      <c r="O3" s="40"/>
-      <c r="P3" s="41"/>
-      <c r="Q3" s="39" t="s">
+      <c r="O3" s="41"/>
+      <c r="P3" s="42"/>
+      <c r="Q3" s="40" t="s">
         <v>15</v>
       </c>
-      <c r="R3" s="40"/>
-      <c r="S3" s="41"/>
-      <c r="T3" s="39" t="s">
+      <c r="R3" s="41"/>
+      <c r="S3" s="42"/>
+      <c r="T3" s="40" t="s">
         <v>16</v>
       </c>
-      <c r="U3" s="40"/>
-      <c r="V3" s="41"/>
-      <c r="W3" s="39" t="s">
+      <c r="U3" s="41"/>
+      <c r="V3" s="42"/>
+      <c r="W3" s="40" t="s">
         <v>17</v>
       </c>
-      <c r="X3" s="40"/>
-      <c r="Y3" s="41"/>
-      <c r="Z3" s="39" t="s">
+      <c r="X3" s="41"/>
+      <c r="Y3" s="42"/>
+      <c r="Z3" s="40" t="s">
         <v>18</v>
       </c>
-      <c r="AA3" s="40"/>
-      <c r="AB3" s="41"/>
+      <c r="AA3" s="41"/>
+      <c r="AB3" s="42"/>
     </row>
     <row r="4" spans="1:28" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="6" t="s">
@@ -2848,25 +2836,25 @@
     </row>
     <row r="6" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>273</v>
       </c>
       <c r="C6" s="3" t="s">
+        <v>297</v>
+      </c>
+      <c r="D6" s="3" t="s">
         <v>298</v>
       </c>
-      <c r="D6" s="3" t="s">
+      <c r="E6" s="3" t="s">
         <v>299</v>
       </c>
-      <c r="E6" s="3" t="s">
+      <c r="F6" s="3" t="s">
         <v>300</v>
       </c>
-      <c r="F6" s="3" t="s">
-        <v>301</v>
-      </c>
       <c r="G6" s="3" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="H6" s="28"/>
       <c r="I6" s="28"/>
@@ -6298,7 +6286,7 @@
   <sheetPr codeName="Sheet5"/>
   <dimension ref="A1:D103"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
@@ -6315,7 +6303,7 @@
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="46" t="str">
+      <c r="A3" s="38" t="str">
         <f t="array" ref="A3">IF(LEN(A5:A103)&gt;19,"NAME LONG", "NAMES OKAY")</f>
         <v>NAMES OKAY</v>
       </c>
@@ -6950,12 +6938,12 @@
     <sortCondition ref="A5:A8"/>
   </sortState>
   <conditionalFormatting sqref="A5:A103">
-    <cfRule type="expression" dxfId="3" priority="3">
+    <cfRule type="expression" dxfId="1" priority="3">
       <formula>LEN(A5)&gt;19</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A3">
-    <cfRule type="expression" dxfId="2" priority="1">
+    <cfRule type="expression" dxfId="0" priority="1">
       <formula>A3="NAMES OKAY"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -8465,7 +8453,7 @@
       <c r="G4" s="1"/>
     </row>
     <row r="5" spans="1:7" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="45" t="s">
+      <c r="A5" s="46" t="s">
         <v>153</v>
       </c>
       <c r="B5" s="12" t="s">
@@ -8479,7 +8467,7 @@
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="45"/>
+      <c r="A6" s="46"/>
       <c r="B6" s="12" t="s">
         <v>98</v>
       </c>
@@ -8491,7 +8479,7 @@
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="45"/>
+      <c r="A7" s="46"/>
       <c r="B7" s="12" t="s">
         <v>107</v>
       </c>
@@ -8503,7 +8491,7 @@
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="45"/>
+      <c r="A8" s="46"/>
       <c r="B8" s="12" t="s">
         <v>99</v>
       </c>
@@ -8515,7 +8503,7 @@
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="45"/>
+      <c r="A9" s="46"/>
       <c r="B9" s="12" t="s">
         <v>100</v>
       </c>
@@ -8527,7 +8515,7 @@
       </c>
     </row>
     <row r="10" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A10" s="45"/>
+      <c r="A10" s="46"/>
       <c r="B10" s="12" t="s">
         <v>108</v>
       </c>
@@ -8539,7 +8527,7 @@
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="45"/>
+      <c r="A11" s="46"/>
       <c r="B11" s="12" t="s">
         <v>101</v>
       </c>
@@ -8551,7 +8539,7 @@
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="45"/>
+      <c r="A12" s="46"/>
       <c r="B12" s="12" t="s">
         <v>102</v>
       </c>
@@ -8563,7 +8551,7 @@
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" s="45"/>
+      <c r="A13" s="46"/>
       <c r="B13" s="12" t="s">
         <v>103</v>
       </c>
@@ -8575,7 +8563,7 @@
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" s="45"/>
+      <c r="A14" s="46"/>
       <c r="B14" s="12" t="s">
         <v>104</v>
       </c>
@@ -8587,7 +8575,7 @@
       </c>
     </row>
     <row r="15" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A15" s="45" t="s">
+      <c r="A15" s="46" t="s">
         <v>154</v>
       </c>
       <c r="B15" s="12" t="s">
@@ -8601,7 +8589,7 @@
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" s="45"/>
+      <c r="A16" s="46"/>
       <c r="B16" s="12" t="s">
         <v>109</v>
       </c>
@@ -8613,7 +8601,7 @@
       </c>
     </row>
     <row r="17" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A17" s="45"/>
+      <c r="A17" s="46"/>
       <c r="B17" s="12" t="s">
         <v>110</v>
       </c>
@@ -8625,7 +8613,7 @@
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="45"/>
+      <c r="A18" s="46"/>
       <c r="B18" s="16" t="s">
         <v>111</v>
       </c>
@@ -8637,7 +8625,7 @@
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="45"/>
+      <c r="A19" s="46"/>
       <c r="B19" s="12" t="s">
         <v>112</v>
       </c>
@@ -8649,7 +8637,7 @@
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="45" t="s">
+      <c r="A20" s="46" t="s">
         <v>155</v>
       </c>
       <c r="B20" s="12" t="s">
@@ -8663,7 +8651,7 @@
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="45"/>
+      <c r="A21" s="46"/>
       <c r="B21" s="12" t="s">
         <v>114</v>
       </c>
@@ -8675,7 +8663,7 @@
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="45"/>
+      <c r="A22" s="46"/>
       <c r="B22" s="12" t="s">
         <v>115</v>
       </c>
@@ -8687,7 +8675,7 @@
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" s="45"/>
+      <c r="A23" s="46"/>
       <c r="B23" s="12" t="s">
         <v>116</v>
       </c>
@@ -8699,7 +8687,7 @@
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" s="45"/>
+      <c r="A24" s="46"/>
       <c r="B24" s="12" t="s">
         <v>117</v>
       </c>
@@ -8711,7 +8699,7 @@
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" s="45"/>
+      <c r="A25" s="46"/>
       <c r="B25" s="12" t="s">
         <v>118</v>
       </c>
@@ -8723,7 +8711,7 @@
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26" s="45"/>
+      <c r="A26" s="46"/>
       <c r="B26" s="12" t="s">
         <v>119</v>
       </c>
@@ -8735,7 +8723,7 @@
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27" s="45"/>
+      <c r="A27" s="46"/>
       <c r="B27" s="12" t="s">
         <v>120</v>
       </c>
@@ -8747,7 +8735,7 @@
       </c>
     </row>
     <row r="28" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A28" s="45"/>
+      <c r="A28" s="46"/>
       <c r="B28" s="12" t="s">
         <v>121</v>
       </c>
@@ -8759,7 +8747,7 @@
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A29" s="45"/>
+      <c r="A29" s="46"/>
       <c r="B29" s="12" t="s">
         <v>122</v>
       </c>
@@ -8771,7 +8759,7 @@
       </c>
     </row>
     <row r="30" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A30" s="45"/>
+      <c r="A30" s="46"/>
       <c r="B30" s="12" t="s">
         <v>123</v>
       </c>
@@ -8783,7 +8771,7 @@
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31" s="45" t="s">
+      <c r="A31" s="46" t="s">
         <v>156</v>
       </c>
       <c r="B31" s="12" t="s">
@@ -8797,7 +8785,7 @@
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A32" s="45"/>
+      <c r="A32" s="46"/>
       <c r="B32" s="12" t="s">
         <v>125</v>
       </c>
@@ -8809,7 +8797,7 @@
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A33" s="45"/>
+      <c r="A33" s="46"/>
       <c r="B33" s="12" t="s">
         <v>126</v>
       </c>
@@ -8821,7 +8809,7 @@
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A34" s="45"/>
+      <c r="A34" s="46"/>
       <c r="B34" s="12" t="s">
         <v>127</v>
       </c>
@@ -8833,7 +8821,7 @@
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A35" s="45"/>
+      <c r="A35" s="46"/>
       <c r="B35" s="12" t="s">
         <v>128</v>
       </c>
@@ -8845,7 +8833,7 @@
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A36" s="45"/>
+      <c r="A36" s="46"/>
       <c r="B36" s="12" t="s">
         <v>129</v>
       </c>
@@ -8857,7 +8845,7 @@
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A37" s="45"/>
+      <c r="A37" s="46"/>
       <c r="B37" s="12" t="s">
         <v>130</v>
       </c>
@@ -8869,7 +8857,7 @@
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A38" s="45"/>
+      <c r="A38" s="46"/>
       <c r="B38" s="12" t="s">
         <v>131</v>
       </c>
@@ -8881,7 +8869,7 @@
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A39" s="45" t="s">
+      <c r="A39" s="46" t="s">
         <v>157</v>
       </c>
       <c r="B39" s="12" t="s">
@@ -8895,7 +8883,7 @@
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A40" s="45"/>
+      <c r="A40" s="46"/>
       <c r="B40" s="12" t="s">
         <v>133</v>
       </c>
@@ -8907,7 +8895,7 @@
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A41" s="45"/>
+      <c r="A41" s="46"/>
       <c r="B41" s="12" t="s">
         <v>134</v>
       </c>
@@ -8919,7 +8907,7 @@
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A42" s="45"/>
+      <c r="A42" s="46"/>
       <c r="B42" s="12" t="s">
         <v>135</v>
       </c>
@@ -8931,7 +8919,7 @@
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A43" s="45"/>
+      <c r="A43" s="46"/>
       <c r="B43" s="12" t="s">
         <v>136</v>
       </c>
@@ -8943,7 +8931,7 @@
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A44" s="45"/>
+      <c r="A44" s="46"/>
       <c r="B44" s="12" t="s">
         <v>137</v>
       </c>
@@ -8955,7 +8943,7 @@
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A45" s="45"/>
+      <c r="A45" s="46"/>
       <c r="B45" s="12" t="s">
         <v>138</v>
       </c>
@@ -8967,7 +8955,7 @@
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A46" s="45"/>
+      <c r="A46" s="46"/>
       <c r="B46" s="16" t="s">
         <v>139</v>
       </c>
@@ -8979,7 +8967,7 @@
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A47" s="45"/>
+      <c r="A47" s="46"/>
       <c r="B47" s="12" t="s">
         <v>140</v>
       </c>
@@ -8991,7 +8979,7 @@
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A48" s="45"/>
+      <c r="A48" s="46"/>
       <c r="B48" s="16" t="s">
         <v>141</v>
       </c>
@@ -9003,7 +8991,7 @@
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A49" s="45" t="s">
+      <c r="A49" s="46" t="s">
         <v>158</v>
       </c>
       <c r="B49" s="12" t="s">
@@ -9017,7 +9005,7 @@
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A50" s="45"/>
+      <c r="A50" s="46"/>
       <c r="B50" s="12" t="s">
         <v>143</v>
       </c>
@@ -9029,7 +9017,7 @@
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A51" s="45"/>
+      <c r="A51" s="46"/>
       <c r="B51" s="12" t="s">
         <v>144</v>
       </c>
@@ -9041,7 +9029,7 @@
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A52" s="45" t="s">
+      <c r="A52" s="46" t="s">
         <v>159</v>
       </c>
       <c r="B52" s="12" t="s">
@@ -9055,7 +9043,7 @@
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A53" s="45"/>
+      <c r="A53" s="46"/>
       <c r="B53" s="12" t="s">
         <v>146</v>
       </c>
@@ -9067,7 +9055,7 @@
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A54" s="45"/>
+      <c r="A54" s="46"/>
       <c r="B54" s="12" t="s">
         <v>147</v>
       </c>
@@ -9079,7 +9067,7 @@
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A55" s="45"/>
+      <c r="A55" s="46"/>
       <c r="B55" s="12" t="s">
         <v>148</v>
       </c>
@@ -9091,7 +9079,7 @@
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A56" s="45"/>
+      <c r="A56" s="46"/>
       <c r="B56" s="12" t="s">
         <v>149</v>
       </c>
@@ -9103,7 +9091,7 @@
       </c>
     </row>
     <row r="57" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A57" s="45"/>
+      <c r="A57" s="46"/>
       <c r="B57" s="12" t="s">
         <v>150</v>
       </c>
@@ -9115,7 +9103,7 @@
       </c>
     </row>
     <row r="58" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A58" s="45" t="s">
+      <c r="A58" s="46" t="s">
         <v>160</v>
       </c>
       <c r="B58" s="12" t="s">
@@ -9129,7 +9117,7 @@
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A59" s="45"/>
+      <c r="A59" s="46"/>
       <c r="B59" s="12" t="s">
         <v>152</v>
       </c>
@@ -9193,7 +9181,7 @@
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="45" t="s">
+      <c r="A5" s="46" t="s">
         <v>163</v>
       </c>
       <c r="B5" s="12" t="s">
@@ -9207,7 +9195,7 @@
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="45"/>
+      <c r="A6" s="46"/>
       <c r="B6" s="12" t="s">
         <v>200</v>
       </c>
@@ -9219,7 +9207,7 @@
       </c>
     </row>
     <row r="7" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A7" s="45"/>
+      <c r="A7" s="46"/>
       <c r="B7" s="12" t="s">
         <v>201</v>
       </c>
@@ -9231,7 +9219,7 @@
       </c>
     </row>
     <row r="8" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A8" s="45"/>
+      <c r="A8" s="46"/>
       <c r="B8" s="12" t="s">
         <v>202</v>
       </c>
@@ -9243,7 +9231,7 @@
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="45"/>
+      <c r="A9" s="46"/>
       <c r="B9" s="12" t="s">
         <v>203</v>
       </c>
@@ -9256,7 +9244,7 @@
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="45"/>
+      <c r="A10" s="46"/>
       <c r="B10" s="12" t="s">
         <v>204</v>
       </c>
@@ -9268,7 +9256,7 @@
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="45"/>
+      <c r="A11" s="46"/>
       <c r="B11" s="12" t="s">
         <v>205</v>
       </c>
@@ -9280,7 +9268,7 @@
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="45"/>
+      <c r="A12" s="46"/>
       <c r="B12" s="12" t="s">
         <v>199</v>
       </c>
@@ -9293,7 +9281,7 @@
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="45"/>
+      <c r="A13" s="46"/>
       <c r="B13" s="12" t="s">
         <v>206</v>
       </c>
@@ -9306,7 +9294,7 @@
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="45"/>
+      <c r="A14" s="46"/>
       <c r="B14" s="12" t="s">
         <v>207</v>
       </c>
@@ -9319,7 +9307,7 @@
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="45"/>
+      <c r="A15" s="46"/>
       <c r="B15" s="16" t="s">
         <v>208</v>
       </c>
@@ -9331,7 +9319,7 @@
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="45"/>
+      <c r="A16" s="46"/>
       <c r="B16" s="16" t="s">
         <v>209</v>
       </c>
@@ -9343,7 +9331,7 @@
       </c>
     </row>
     <row r="17" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A17" s="45" t="s">
+      <c r="A17" s="46" t="s">
         <v>164</v>
       </c>
       <c r="B17" s="12" t="s">
@@ -9357,7 +9345,7 @@
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="45"/>
+      <c r="A18" s="46"/>
       <c r="B18" s="12" t="s">
         <v>211</v>
       </c>
@@ -9369,7 +9357,7 @@
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="45"/>
+      <c r="A19" s="46"/>
       <c r="B19" s="12" t="s">
         <v>212</v>
       </c>
@@ -9381,7 +9369,7 @@
       </c>
     </row>
     <row r="20" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A20" s="45"/>
+      <c r="A20" s="46"/>
       <c r="B20" s="12" t="s">
         <v>213</v>
       </c>
@@ -9431,7 +9419,7 @@
       <c r="B1" s="7"/>
     </row>
     <row r="5" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A5" s="45"/>
+      <c r="A5" s="46"/>
       <c r="B5" s="12" t="s">
         <v>252</v>
       </c>
@@ -9443,7 +9431,7 @@
       </c>
     </row>
     <row r="6" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A6" s="45"/>
+      <c r="A6" s="46"/>
       <c r="B6" s="12" t="s">
         <v>214</v>
       </c>
@@ -9455,7 +9443,7 @@
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="45"/>
+      <c r="A7" s="46"/>
       <c r="B7" s="12" t="s">
         <v>215</v>
       </c>
@@ -9467,7 +9455,7 @@
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="45"/>
+      <c r="A8" s="46"/>
       <c r="B8" s="12" t="s">
         <v>216</v>
       </c>
@@ -9479,7 +9467,7 @@
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="45"/>
+      <c r="A9" s="46"/>
       <c r="B9" s="12" t="s">
         <v>199</v>
       </c>
@@ -9491,7 +9479,7 @@
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="45"/>
+      <c r="A10" s="46"/>
       <c r="B10" s="12" t="s">
         <v>206</v>
       </c>
@@ -9503,7 +9491,7 @@
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="45"/>
+      <c r="A11" s="46"/>
       <c r="B11" s="12" t="s">
         <v>207</v>
       </c>
@@ -9516,7 +9504,7 @@
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="45"/>
+      <c r="A12" s="46"/>
       <c r="B12" s="16" t="s">
         <v>208</v>
       </c>
@@ -9528,7 +9516,7 @@
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="45"/>
+      <c r="A13" s="46"/>
       <c r="B13" s="16" t="s">
         <v>209</v>
       </c>
@@ -9554,7 +9542,7 @@
       </c>
     </row>
     <row r="15" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A15" s="45" t="s">
+      <c r="A15" s="46" t="s">
         <v>197</v>
       </c>
       <c r="B15" s="12" t="s">
@@ -9568,7 +9556,7 @@
       </c>
     </row>
     <row r="16" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A16" s="45"/>
+      <c r="A16" s="46"/>
       <c r="B16" s="12" t="s">
         <v>219</v>
       </c>
@@ -9580,7 +9568,7 @@
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="45"/>
+      <c r="A17" s="46"/>
       <c r="B17" s="12" t="s">
         <v>220</v>
       </c>
@@ -9592,7 +9580,7 @@
       </c>
     </row>
     <row r="18" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A18" s="45"/>
+      <c r="A18" s="46"/>
       <c r="B18" s="12" t="s">
         <v>213</v>
       </c>
@@ -9604,7 +9592,7 @@
       </c>
     </row>
     <row r="19" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A19" s="45"/>
+      <c r="A19" s="46"/>
       <c r="B19" s="12" t="s">
         <v>221</v>
       </c>
@@ -9639,6 +9627,17 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
+  <documentManagement>
+    <iab7cdb7554d4997ae876b11632fa575 xmlns="3cada6dc-2705-46ed-bab2-0b2cd6d935ca">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </iab7cdb7554d4997ae876b11632fa575>
+    <TaxCatchAll xmlns="3cada6dc-2705-46ed-bab2-0b2cd6d935ca"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100C9B3B8AC64AC88418540180D602CE6AB" ma:contentTypeVersion="4" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="c03373d3e8f67dac2598d545e73c3e0f">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="3cada6dc-2705-46ed-bab2-0b2cd6d935ca" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="f693bfc3a603cfa0c3f0b58e702f3d19" ns2:_="">
     <xsd:import namespace="3cada6dc-2705-46ed-bab2-0b2cd6d935ca"/>
@@ -9790,17 +9789,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
-  <documentManagement>
-    <iab7cdb7554d4997ae876b11632fa575 xmlns="3cada6dc-2705-46ed-bab2-0b2cd6d935ca">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </iab7cdb7554d4997ae876b11632fa575>
-    <TaxCatchAll xmlns="3cada6dc-2705-46ed-bab2-0b2cd6d935ca"/>
-  </documentManagement>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7B5D7682-109C-47ED-9D9D-D061E76CCAD3}">
   <ds:schemaRefs>
@@ -9810,6 +9798,22 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FCC61AA8-C35E-4598-8617-08B80F018AC2}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="3cada6dc-2705-46ed-bab2-0b2cd6d935ca"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2A5E1C23-6545-45A2-BF0C-826678B16173}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -9825,20 +9829,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FCC61AA8-C35E-4598-8617-08B80F018AC2}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="3cada6dc-2705-46ed-bab2-0b2cd6d935ca"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Added to include High Pass filter as an option
</commit_message>
<xml_diff>
--- a/HAST_Inputs.xlsx
+++ b/HAST_Inputs.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="20730"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8113F58-57B1-4C91-BEB2-DCA0952F6AC8}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1418E31-363F-41D6-A35B-F11FD743D99D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="465" windowWidth="14805" windowHeight="7650" tabRatio="868" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="465" windowWidth="14805" windowHeight="7650" tabRatio="868" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cover Sheet" sheetId="10" r:id="rId1"/>
@@ -2188,7 +2188,7 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:F24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
@@ -6957,8 +6957,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D08D4187-8BE1-4B7A-A634-AC08177090E1}">
   <dimension ref="A1:L103"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5:L5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7048,7 +7048,7 @@
       <c r="A7" s="3"/>
       <c r="B7" s="3"/>
       <c r="C7" s="3"/>
-      <c r="D7" s="3"/>
+      <c r="D7" s="37"/>
       <c r="E7" s="3"/>
       <c r="F7" s="3"/>
       <c r="G7" s="3"/>
@@ -7062,7 +7062,7 @@
       <c r="A8" s="3"/>
       <c r="B8" s="3"/>
       <c r="C8" s="3"/>
-      <c r="D8" s="3"/>
+      <c r="D8" s="37"/>
       <c r="E8" s="3"/>
       <c r="F8" s="3"/>
       <c r="G8" s="3"/>
@@ -7076,7 +7076,7 @@
       <c r="A9" s="3"/>
       <c r="B9" s="3"/>
       <c r="C9" s="3"/>
-      <c r="D9" s="3"/>
+      <c r="D9" s="37"/>
       <c r="E9" s="3"/>
       <c r="F9" s="3"/>
       <c r="G9" s="3"/>
@@ -7090,7 +7090,7 @@
       <c r="A10" s="28"/>
       <c r="B10" s="3"/>
       <c r="C10" s="3"/>
-      <c r="D10" s="3"/>
+      <c r="D10" s="37"/>
       <c r="E10" s="3"/>
       <c r="F10" s="3"/>
       <c r="G10" s="3"/>
@@ -7104,7 +7104,7 @@
       <c r="A11" s="28"/>
       <c r="B11" s="3"/>
       <c r="C11" s="3"/>
-      <c r="D11" s="3"/>
+      <c r="D11" s="37"/>
       <c r="E11" s="3"/>
       <c r="F11" s="3"/>
       <c r="G11" s="3"/>
@@ -7118,7 +7118,7 @@
       <c r="A12" s="3"/>
       <c r="B12" s="3"/>
       <c r="C12" s="3"/>
-      <c r="D12" s="3"/>
+      <c r="D12" s="37"/>
       <c r="E12" s="3"/>
       <c r="F12" s="3"/>
       <c r="G12" s="3"/>
@@ -7132,7 +7132,7 @@
       <c r="A13" s="3"/>
       <c r="B13" s="3"/>
       <c r="C13" s="3"/>
-      <c r="D13" s="3"/>
+      <c r="D13" s="37"/>
       <c r="E13" s="3"/>
       <c r="F13" s="3"/>
       <c r="G13" s="3"/>
@@ -7146,7 +7146,7 @@
       <c r="A14" s="3"/>
       <c r="B14" s="3"/>
       <c r="C14" s="3"/>
-      <c r="D14" s="3"/>
+      <c r="D14" s="37"/>
       <c r="E14" s="3"/>
       <c r="F14" s="3"/>
       <c r="G14" s="3"/>
@@ -7160,7 +7160,7 @@
       <c r="A15" s="3"/>
       <c r="B15" s="3"/>
       <c r="C15" s="3"/>
-      <c r="D15" s="3"/>
+      <c r="D15" s="37"/>
       <c r="E15" s="3"/>
       <c r="F15" s="3"/>
       <c r="G15" s="3"/>
@@ -7174,7 +7174,7 @@
       <c r="A16" s="3"/>
       <c r="B16" s="3"/>
       <c r="C16" s="3"/>
-      <c r="D16" s="3"/>
+      <c r="D16" s="37"/>
       <c r="E16" s="3"/>
       <c r="F16" s="3"/>
       <c r="G16" s="3"/>
@@ -7188,7 +7188,7 @@
       <c r="A17" s="3"/>
       <c r="B17" s="3"/>
       <c r="C17" s="3"/>
-      <c r="D17" s="3"/>
+      <c r="D17" s="37"/>
       <c r="E17" s="3"/>
       <c r="F17" s="3"/>
       <c r="G17" s="3"/>
@@ -7202,7 +7202,7 @@
       <c r="A18" s="3"/>
       <c r="B18" s="3"/>
       <c r="C18" s="3"/>
-      <c r="D18" s="3"/>
+      <c r="D18" s="37"/>
       <c r="E18" s="3"/>
       <c r="F18" s="3"/>
       <c r="G18" s="3"/>
@@ -7216,7 +7216,7 @@
       <c r="A19" s="3"/>
       <c r="B19" s="3"/>
       <c r="C19" s="3"/>
-      <c r="D19" s="3"/>
+      <c r="D19" s="37"/>
       <c r="E19" s="3"/>
       <c r="F19" s="3"/>
       <c r="G19" s="3"/>
@@ -7230,7 +7230,7 @@
       <c r="A20" s="3"/>
       <c r="B20" s="3"/>
       <c r="C20" s="3"/>
-      <c r="D20" s="3"/>
+      <c r="D20" s="37"/>
       <c r="E20" s="3"/>
       <c r="F20" s="3"/>
       <c r="G20" s="3"/>
@@ -7244,7 +7244,7 @@
       <c r="A21" s="28"/>
       <c r="B21" s="3"/>
       <c r="C21" s="3"/>
-      <c r="D21" s="3"/>
+      <c r="D21" s="37"/>
       <c r="E21" s="3"/>
       <c r="F21" s="3"/>
       <c r="G21" s="3"/>
@@ -7258,7 +7258,7 @@
       <c r="A22" s="3"/>
       <c r="B22" s="3"/>
       <c r="C22" s="3"/>
-      <c r="D22" s="3"/>
+      <c r="D22" s="37"/>
       <c r="E22" s="3"/>
       <c r="F22" s="3"/>
       <c r="G22" s="3"/>
@@ -7272,7 +7272,7 @@
       <c r="A23" s="28"/>
       <c r="B23" s="3"/>
       <c r="C23" s="3"/>
-      <c r="D23" s="3"/>
+      <c r="D23" s="37"/>
       <c r="E23" s="3"/>
       <c r="F23" s="3"/>
       <c r="G23" s="3"/>
@@ -7286,7 +7286,7 @@
       <c r="A24" s="28"/>
       <c r="B24" s="3"/>
       <c r="C24" s="3"/>
-      <c r="D24" s="3"/>
+      <c r="D24" s="37"/>
       <c r="E24" s="3"/>
       <c r="F24" s="3"/>
       <c r="G24" s="3"/>
@@ -7300,7 +7300,7 @@
       <c r="A25" s="28"/>
       <c r="B25" s="3"/>
       <c r="C25" s="3"/>
-      <c r="D25" s="3"/>
+      <c r="D25" s="37"/>
       <c r="E25" s="3"/>
       <c r="F25" s="3"/>
       <c r="G25" s="3"/>
@@ -7314,7 +7314,7 @@
       <c r="A26" s="28"/>
       <c r="B26" s="3"/>
       <c r="C26" s="3"/>
-      <c r="D26" s="3"/>
+      <c r="D26" s="37"/>
       <c r="E26" s="3"/>
       <c r="F26" s="3"/>
       <c r="G26" s="3"/>
@@ -7328,7 +7328,7 @@
       <c r="A27" s="3"/>
       <c r="B27" s="3"/>
       <c r="C27" s="3"/>
-      <c r="D27" s="3"/>
+      <c r="D27" s="37"/>
       <c r="E27" s="3"/>
       <c r="F27" s="3"/>
       <c r="G27" s="3"/>
@@ -7342,7 +7342,7 @@
       <c r="A28" s="3"/>
       <c r="B28" s="3"/>
       <c r="C28" s="3"/>
-      <c r="D28" s="3"/>
+      <c r="D28" s="37"/>
       <c r="E28" s="3"/>
       <c r="F28" s="3"/>
       <c r="G28" s="3"/>
@@ -7356,7 +7356,7 @@
       <c r="A29" s="3"/>
       <c r="B29" s="3"/>
       <c r="C29" s="3"/>
-      <c r="D29" s="3"/>
+      <c r="D29" s="37"/>
       <c r="E29" s="3"/>
       <c r="F29" s="3"/>
       <c r="G29" s="3"/>
@@ -7370,7 +7370,7 @@
       <c r="A30" s="3"/>
       <c r="B30" s="3"/>
       <c r="C30" s="3"/>
-      <c r="D30" s="3"/>
+      <c r="D30" s="37"/>
       <c r="E30" s="3"/>
       <c r="F30" s="3"/>
       <c r="G30" s="3"/>
@@ -7384,7 +7384,7 @@
       <c r="A31" s="3"/>
       <c r="B31" s="3"/>
       <c r="C31" s="3"/>
-      <c r="D31" s="3"/>
+      <c r="D31" s="37"/>
       <c r="E31" s="3"/>
       <c r="F31" s="3"/>
       <c r="G31" s="3"/>
@@ -7398,7 +7398,7 @@
       <c r="A32" s="28"/>
       <c r="B32" s="3"/>
       <c r="C32" s="3"/>
-      <c r="D32" s="3"/>
+      <c r="D32" s="37"/>
       <c r="E32" s="3"/>
       <c r="F32" s="3"/>
       <c r="G32" s="3"/>
@@ -7412,7 +7412,7 @@
       <c r="A33" s="28"/>
       <c r="B33" s="3"/>
       <c r="C33" s="3"/>
-      <c r="D33" s="3"/>
+      <c r="D33" s="37"/>
       <c r="E33" s="3"/>
       <c r="F33" s="3"/>
       <c r="G33" s="3"/>
@@ -7426,7 +7426,7 @@
       <c r="A34" s="3"/>
       <c r="B34" s="3"/>
       <c r="C34" s="3"/>
-      <c r="D34" s="3"/>
+      <c r="D34" s="37"/>
       <c r="E34" s="3"/>
       <c r="F34" s="3"/>
       <c r="G34" s="3"/>
@@ -7440,7 +7440,7 @@
       <c r="A35" s="3"/>
       <c r="B35" s="3"/>
       <c r="C35" s="3"/>
-      <c r="D35" s="3"/>
+      <c r="D35" s="37"/>
       <c r="E35" s="3"/>
       <c r="F35" s="3"/>
       <c r="G35" s="3"/>
@@ -7454,7 +7454,7 @@
       <c r="A36" s="3"/>
       <c r="B36" s="3"/>
       <c r="C36" s="3"/>
-      <c r="D36" s="3"/>
+      <c r="D36" s="37"/>
       <c r="E36" s="3"/>
       <c r="F36" s="3"/>
       <c r="G36" s="3"/>
@@ -7468,7 +7468,7 @@
       <c r="A37" s="3"/>
       <c r="B37" s="3"/>
       <c r="C37" s="3"/>
-      <c r="D37" s="3"/>
+      <c r="D37" s="37"/>
       <c r="E37" s="3"/>
       <c r="F37" s="3"/>
       <c r="G37" s="3"/>
@@ -7482,7 +7482,7 @@
       <c r="A38" s="28"/>
       <c r="B38" s="3"/>
       <c r="C38" s="3"/>
-      <c r="D38" s="3"/>
+      <c r="D38" s="37"/>
       <c r="E38" s="3"/>
       <c r="F38" s="3"/>
       <c r="G38" s="3"/>
@@ -7496,7 +7496,7 @@
       <c r="A39" s="3"/>
       <c r="B39" s="3"/>
       <c r="C39" s="3"/>
-      <c r="D39" s="3"/>
+      <c r="D39" s="37"/>
       <c r="E39" s="3"/>
       <c r="F39" s="3"/>
       <c r="G39" s="3"/>
@@ -7510,7 +7510,7 @@
       <c r="A40" s="3"/>
       <c r="B40" s="3"/>
       <c r="C40" s="3"/>
-      <c r="D40" s="3"/>
+      <c r="D40" s="37"/>
       <c r="E40" s="3"/>
       <c r="F40" s="3"/>
       <c r="G40" s="3"/>
@@ -7524,7 +7524,7 @@
       <c r="A41" s="28"/>
       <c r="B41" s="3"/>
       <c r="C41" s="3"/>
-      <c r="D41" s="3"/>
+      <c r="D41" s="37"/>
       <c r="E41" s="3"/>
       <c r="F41" s="3"/>
       <c r="G41" s="3"/>
@@ -7538,7 +7538,7 @@
       <c r="A42" s="3"/>
       <c r="B42" s="3"/>
       <c r="C42" s="3"/>
-      <c r="D42" s="3"/>
+      <c r="D42" s="37"/>
       <c r="E42" s="3"/>
       <c r="F42" s="3"/>
       <c r="G42" s="3"/>
@@ -7552,7 +7552,7 @@
       <c r="A43" s="28"/>
       <c r="B43" s="3"/>
       <c r="C43" s="3"/>
-      <c r="D43" s="3"/>
+      <c r="D43" s="37"/>
       <c r="E43" s="3"/>
       <c r="F43" s="3"/>
       <c r="G43" s="3"/>
@@ -7566,7 +7566,7 @@
       <c r="A44" s="3"/>
       <c r="B44" s="3"/>
       <c r="C44" s="3"/>
-      <c r="D44" s="3"/>
+      <c r="D44" s="37"/>
       <c r="E44" s="3"/>
       <c r="F44" s="3"/>
       <c r="G44" s="3"/>
@@ -7580,7 +7580,7 @@
       <c r="A45" s="3"/>
       <c r="B45" s="3"/>
       <c r="C45" s="3"/>
-      <c r="D45" s="3"/>
+      <c r="D45" s="37"/>
       <c r="E45" s="3"/>
       <c r="F45" s="3"/>
       <c r="G45" s="3"/>
@@ -7594,7 +7594,7 @@
       <c r="A46" s="28"/>
       <c r="B46" s="3"/>
       <c r="C46" s="3"/>
-      <c r="D46" s="3"/>
+      <c r="D46" s="37"/>
       <c r="E46" s="3"/>
       <c r="F46" s="3"/>
       <c r="G46" s="3"/>
@@ -7608,7 +7608,7 @@
       <c r="A47" s="3"/>
       <c r="B47" s="3"/>
       <c r="C47" s="3"/>
-      <c r="D47" s="3"/>
+      <c r="D47" s="37"/>
       <c r="E47" s="3"/>
       <c r="F47" s="3"/>
       <c r="G47" s="3"/>
@@ -7622,7 +7622,7 @@
       <c r="A48" s="28"/>
       <c r="B48" s="3"/>
       <c r="C48" s="3"/>
-      <c r="D48" s="3"/>
+      <c r="D48" s="37"/>
       <c r="E48" s="3"/>
       <c r="F48" s="3"/>
       <c r="G48" s="3"/>
@@ -7636,7 +7636,7 @@
       <c r="A49" s="28"/>
       <c r="B49" s="3"/>
       <c r="C49" s="3"/>
-      <c r="D49" s="3"/>
+      <c r="D49" s="37"/>
       <c r="E49" s="3"/>
       <c r="F49" s="3"/>
       <c r="G49" s="3"/>
@@ -7650,7 +7650,7 @@
       <c r="A50" s="3"/>
       <c r="B50" s="3"/>
       <c r="C50" s="3"/>
-      <c r="D50" s="3"/>
+      <c r="D50" s="37"/>
       <c r="E50" s="3"/>
       <c r="F50" s="3"/>
       <c r="G50" s="3"/>
@@ -7664,7 +7664,7 @@
       <c r="A51" s="28"/>
       <c r="B51" s="3"/>
       <c r="C51" s="3"/>
-      <c r="D51" s="3"/>
+      <c r="D51" s="37"/>
       <c r="E51" s="3"/>
       <c r="F51" s="3"/>
       <c r="G51" s="3"/>
@@ -7678,7 +7678,7 @@
       <c r="A52" s="28"/>
       <c r="B52" s="3"/>
       <c r="C52" s="3"/>
-      <c r="D52" s="3"/>
+      <c r="D52" s="37"/>
       <c r="E52" s="3"/>
       <c r="F52" s="3"/>
       <c r="G52" s="3"/>
@@ -7692,7 +7692,7 @@
       <c r="A53" s="28"/>
       <c r="B53" s="3"/>
       <c r="C53" s="3"/>
-      <c r="D53" s="3"/>
+      <c r="D53" s="37"/>
       <c r="E53" s="3"/>
       <c r="F53" s="3"/>
       <c r="G53" s="3"/>
@@ -7706,7 +7706,7 @@
       <c r="A54" s="3"/>
       <c r="B54" s="3"/>
       <c r="C54" s="3"/>
-      <c r="D54" s="3"/>
+      <c r="D54" s="37"/>
       <c r="E54" s="3"/>
       <c r="F54" s="3"/>
       <c r="G54" s="3"/>
@@ -7720,7 +7720,7 @@
       <c r="A55" s="3"/>
       <c r="B55" s="3"/>
       <c r="C55" s="3"/>
-      <c r="D55" s="3"/>
+      <c r="D55" s="37"/>
       <c r="E55" s="3"/>
       <c r="F55" s="3"/>
       <c r="G55" s="3"/>
@@ -7734,7 +7734,7 @@
       <c r="A56" s="3"/>
       <c r="B56" s="3"/>
       <c r="C56" s="3"/>
-      <c r="D56" s="3"/>
+      <c r="D56" s="37"/>
       <c r="E56" s="3"/>
       <c r="F56" s="3"/>
       <c r="G56" s="3"/>
@@ -7748,7 +7748,7 @@
       <c r="A57" s="28"/>
       <c r="B57" s="3"/>
       <c r="C57" s="3"/>
-      <c r="D57" s="3"/>
+      <c r="D57" s="37"/>
       <c r="E57" s="3"/>
       <c r="F57" s="3"/>
       <c r="G57" s="3"/>
@@ -7762,7 +7762,7 @@
       <c r="A58" s="3"/>
       <c r="B58" s="3"/>
       <c r="C58" s="3"/>
-      <c r="D58" s="3"/>
+      <c r="D58" s="37"/>
       <c r="E58" s="3"/>
       <c r="F58" s="3"/>
       <c r="G58" s="3"/>
@@ -7776,7 +7776,7 @@
       <c r="A59" s="3"/>
       <c r="B59" s="3"/>
       <c r="C59" s="3"/>
-      <c r="D59" s="3"/>
+      <c r="D59" s="37"/>
       <c r="E59" s="3"/>
       <c r="F59" s="3"/>
       <c r="G59" s="3"/>
@@ -7790,7 +7790,7 @@
       <c r="A60" s="28"/>
       <c r="B60" s="3"/>
       <c r="C60" s="3"/>
-      <c r="D60" s="3"/>
+      <c r="D60" s="37"/>
       <c r="E60" s="3"/>
       <c r="F60" s="3"/>
       <c r="G60" s="3"/>
@@ -7804,7 +7804,7 @@
       <c r="A61" s="3"/>
       <c r="B61" s="3"/>
       <c r="C61" s="3"/>
-      <c r="D61" s="3"/>
+      <c r="D61" s="37"/>
       <c r="E61" s="3"/>
       <c r="F61" s="3"/>
       <c r="G61" s="3"/>
@@ -7818,7 +7818,7 @@
       <c r="A62" s="3"/>
       <c r="B62" s="3"/>
       <c r="C62" s="3"/>
-      <c r="D62" s="3"/>
+      <c r="D62" s="37"/>
       <c r="E62" s="3"/>
       <c r="F62" s="3"/>
       <c r="G62" s="3"/>
@@ -7832,7 +7832,7 @@
       <c r="A63" s="28"/>
       <c r="B63" s="3"/>
       <c r="C63" s="3"/>
-      <c r="D63" s="3"/>
+      <c r="D63" s="37"/>
       <c r="E63" s="3"/>
       <c r="F63" s="3"/>
       <c r="G63" s="3"/>
@@ -7846,7 +7846,7 @@
       <c r="A64" s="3"/>
       <c r="B64" s="3"/>
       <c r="C64" s="3"/>
-      <c r="D64" s="3"/>
+      <c r="D64" s="37"/>
       <c r="E64" s="3"/>
       <c r="F64" s="3"/>
       <c r="G64" s="3"/>
@@ -7860,7 +7860,7 @@
       <c r="A65" s="3"/>
       <c r="B65" s="3"/>
       <c r="C65" s="3"/>
-      <c r="D65" s="3"/>
+      <c r="D65" s="37"/>
       <c r="E65" s="3"/>
       <c r="F65" s="3"/>
       <c r="G65" s="3"/>
@@ -7874,7 +7874,7 @@
       <c r="A66" s="3"/>
       <c r="B66" s="3"/>
       <c r="C66" s="3"/>
-      <c r="D66" s="3"/>
+      <c r="D66" s="37"/>
       <c r="E66" s="3"/>
       <c r="F66" s="3"/>
       <c r="G66" s="3"/>
@@ -7888,7 +7888,7 @@
       <c r="A67" s="3"/>
       <c r="B67" s="3"/>
       <c r="C67" s="3"/>
-      <c r="D67" s="3"/>
+      <c r="D67" s="37"/>
       <c r="E67" s="3"/>
       <c r="F67" s="3"/>
       <c r="G67" s="3"/>
@@ -7902,7 +7902,7 @@
       <c r="A68" s="3"/>
       <c r="B68" s="3"/>
       <c r="C68" s="3"/>
-      <c r="D68" s="3"/>
+      <c r="D68" s="37"/>
       <c r="E68" s="3"/>
       <c r="F68" s="3"/>
       <c r="G68" s="3"/>
@@ -7916,7 +7916,7 @@
       <c r="A69" s="3"/>
       <c r="B69" s="3"/>
       <c r="C69" s="3"/>
-      <c r="D69" s="3"/>
+      <c r="D69" s="37"/>
       <c r="E69" s="3"/>
       <c r="F69" s="3"/>
       <c r="G69" s="3"/>
@@ -7930,7 +7930,7 @@
       <c r="A70" s="3"/>
       <c r="B70" s="3"/>
       <c r="C70" s="3"/>
-      <c r="D70" s="3"/>
+      <c r="D70" s="37"/>
       <c r="E70" s="3"/>
       <c r="F70" s="3"/>
       <c r="G70" s="3"/>
@@ -7944,7 +7944,7 @@
       <c r="A71" s="28"/>
       <c r="B71" s="3"/>
       <c r="C71" s="3"/>
-      <c r="D71" s="3"/>
+      <c r="D71" s="37"/>
       <c r="E71" s="3"/>
       <c r="F71" s="3"/>
       <c r="G71" s="3"/>
@@ -7958,7 +7958,7 @@
       <c r="A72" s="28"/>
       <c r="B72" s="3"/>
       <c r="C72" s="3"/>
-      <c r="D72" s="3"/>
+      <c r="D72" s="37"/>
       <c r="E72" s="3"/>
       <c r="F72" s="3"/>
       <c r="G72" s="3"/>
@@ -7972,7 +7972,7 @@
       <c r="A73" s="28"/>
       <c r="B73" s="3"/>
       <c r="C73" s="3"/>
-      <c r="D73" s="3"/>
+      <c r="D73" s="37"/>
       <c r="E73" s="3"/>
       <c r="F73" s="3"/>
       <c r="G73" s="3"/>
@@ -7986,7 +7986,7 @@
       <c r="A74" s="3"/>
       <c r="B74" s="3"/>
       <c r="C74" s="3"/>
-      <c r="D74" s="3"/>
+      <c r="D74" s="37"/>
       <c r="E74" s="3"/>
       <c r="F74" s="3"/>
       <c r="G74" s="3"/>
@@ -8000,7 +8000,7 @@
       <c r="A75" s="3"/>
       <c r="B75" s="3"/>
       <c r="C75" s="3"/>
-      <c r="D75" s="3"/>
+      <c r="D75" s="37"/>
       <c r="E75" s="3"/>
       <c r="F75" s="3"/>
       <c r="G75" s="3"/>
@@ -8014,7 +8014,7 @@
       <c r="A76" s="3"/>
       <c r="B76" s="3"/>
       <c r="C76" s="3"/>
-      <c r="D76" s="3"/>
+      <c r="D76" s="37"/>
       <c r="E76" s="3"/>
       <c r="F76" s="3"/>
       <c r="G76" s="3"/>
@@ -8028,7 +8028,7 @@
       <c r="A77" s="3"/>
       <c r="B77" s="3"/>
       <c r="C77" s="3"/>
-      <c r="D77" s="3"/>
+      <c r="D77" s="37"/>
       <c r="E77" s="3"/>
       <c r="F77" s="3"/>
       <c r="G77" s="3"/>
@@ -8042,7 +8042,7 @@
       <c r="A78" s="28"/>
       <c r="B78" s="3"/>
       <c r="C78" s="3"/>
-      <c r="D78" s="3"/>
+      <c r="D78" s="37"/>
       <c r="E78" s="3"/>
       <c r="F78" s="3"/>
       <c r="G78" s="3"/>
@@ -8056,7 +8056,7 @@
       <c r="A79" s="3"/>
       <c r="B79" s="3"/>
       <c r="C79" s="3"/>
-      <c r="D79" s="3"/>
+      <c r="D79" s="37"/>
       <c r="E79" s="3"/>
       <c r="F79" s="3"/>
       <c r="G79" s="3"/>
@@ -8070,7 +8070,7 @@
       <c r="A80" s="28"/>
       <c r="B80" s="3"/>
       <c r="C80" s="3"/>
-      <c r="D80" s="3"/>
+      <c r="D80" s="37"/>
       <c r="E80" s="3"/>
       <c r="F80" s="3"/>
       <c r="G80" s="3"/>
@@ -8084,7 +8084,7 @@
       <c r="A81" s="3"/>
       <c r="B81" s="3"/>
       <c r="C81" s="3"/>
-      <c r="D81" s="3"/>
+      <c r="D81" s="37"/>
       <c r="E81" s="3"/>
       <c r="F81" s="3"/>
       <c r="G81" s="3"/>
@@ -8098,7 +8098,7 @@
       <c r="A82" s="28"/>
       <c r="B82" s="3"/>
       <c r="C82" s="3"/>
-      <c r="D82" s="3"/>
+      <c r="D82" s="37"/>
       <c r="E82" s="3"/>
       <c r="F82" s="3"/>
       <c r="G82" s="3"/>
@@ -8112,7 +8112,7 @@
       <c r="A83" s="3"/>
       <c r="B83" s="3"/>
       <c r="C83" s="3"/>
-      <c r="D83" s="3"/>
+      <c r="D83" s="37"/>
       <c r="E83" s="3"/>
       <c r="F83" s="3"/>
       <c r="G83" s="3"/>
@@ -8126,7 +8126,7 @@
       <c r="A84" s="3"/>
       <c r="B84" s="3"/>
       <c r="C84" s="3"/>
-      <c r="D84" s="3"/>
+      <c r="D84" s="37"/>
       <c r="E84" s="3"/>
       <c r="F84" s="3"/>
       <c r="G84" s="3"/>
@@ -8140,7 +8140,7 @@
       <c r="A85" s="3"/>
       <c r="B85" s="3"/>
       <c r="C85" s="3"/>
-      <c r="D85" s="3"/>
+      <c r="D85" s="37"/>
       <c r="E85" s="3"/>
       <c r="F85" s="3"/>
       <c r="G85" s="3"/>
@@ -8154,7 +8154,7 @@
       <c r="A86" s="28"/>
       <c r="B86" s="3"/>
       <c r="C86" s="3"/>
-      <c r="D86" s="3"/>
+      <c r="D86" s="37"/>
       <c r="E86" s="3"/>
       <c r="F86" s="3"/>
       <c r="G86" s="3"/>
@@ -8168,7 +8168,7 @@
       <c r="A87" s="3"/>
       <c r="B87" s="3"/>
       <c r="C87" s="3"/>
-      <c r="D87" s="3"/>
+      <c r="D87" s="37"/>
       <c r="E87" s="3"/>
       <c r="F87" s="3"/>
       <c r="G87" s="3"/>
@@ -8182,7 +8182,7 @@
       <c r="A88" s="3"/>
       <c r="B88" s="3"/>
       <c r="C88" s="3"/>
-      <c r="D88" s="3"/>
+      <c r="D88" s="37"/>
       <c r="E88" s="3"/>
       <c r="F88" s="3"/>
       <c r="G88" s="3"/>
@@ -8196,7 +8196,7 @@
       <c r="A89" s="28"/>
       <c r="B89" s="3"/>
       <c r="C89" s="3"/>
-      <c r="D89" s="3"/>
+      <c r="D89" s="37"/>
       <c r="E89" s="3"/>
       <c r="F89" s="3"/>
       <c r="G89" s="3"/>
@@ -8210,7 +8210,7 @@
       <c r="A90" s="3"/>
       <c r="B90" s="3"/>
       <c r="C90" s="3"/>
-      <c r="D90" s="3"/>
+      <c r="D90" s="37"/>
       <c r="E90" s="3"/>
       <c r="F90" s="3"/>
       <c r="G90" s="3"/>
@@ -8224,7 +8224,7 @@
       <c r="A91" s="3"/>
       <c r="B91" s="3"/>
       <c r="C91" s="3"/>
-      <c r="D91" s="3"/>
+      <c r="D91" s="37"/>
       <c r="E91" s="3"/>
       <c r="F91" s="3"/>
       <c r="G91" s="3"/>
@@ -8238,7 +8238,7 @@
       <c r="A92" s="3"/>
       <c r="B92" s="3"/>
       <c r="C92" s="3"/>
-      <c r="D92" s="3"/>
+      <c r="D92" s="37"/>
       <c r="E92" s="3"/>
       <c r="F92" s="3"/>
       <c r="G92" s="3"/>
@@ -8252,7 +8252,7 @@
       <c r="A93" s="28"/>
       <c r="B93" s="3"/>
       <c r="C93" s="3"/>
-      <c r="D93" s="3"/>
+      <c r="D93" s="37"/>
       <c r="E93" s="3"/>
       <c r="F93" s="3"/>
       <c r="G93" s="3"/>
@@ -8266,7 +8266,7 @@
       <c r="A94" s="28"/>
       <c r="B94" s="3"/>
       <c r="C94" s="3"/>
-      <c r="D94" s="28"/>
+      <c r="D94" s="37"/>
       <c r="E94" s="3"/>
       <c r="F94" s="3"/>
       <c r="G94" s="3"/>
@@ -8280,7 +8280,7 @@
       <c r="A95" s="3"/>
       <c r="B95" s="3"/>
       <c r="C95" s="3"/>
-      <c r="D95" s="3"/>
+      <c r="D95" s="37"/>
       <c r="E95" s="3"/>
       <c r="F95" s="3"/>
       <c r="G95" s="3"/>
@@ -8294,7 +8294,7 @@
       <c r="A96" s="3"/>
       <c r="B96" s="3"/>
       <c r="C96" s="3"/>
-      <c r="D96" s="3"/>
+      <c r="D96" s="37"/>
       <c r="E96" s="3"/>
       <c r="F96" s="3"/>
       <c r="G96" s="3"/>
@@ -8308,7 +8308,7 @@
       <c r="A97" s="28"/>
       <c r="B97" s="3"/>
       <c r="C97" s="3"/>
-      <c r="D97" s="3"/>
+      <c r="D97" s="37"/>
       <c r="E97" s="3"/>
       <c r="F97" s="3"/>
       <c r="G97" s="3"/>
@@ -8322,7 +8322,7 @@
       <c r="A98" s="3"/>
       <c r="B98" s="3"/>
       <c r="C98" s="3"/>
-      <c r="D98" s="3"/>
+      <c r="D98" s="37"/>
       <c r="E98" s="3"/>
       <c r="F98" s="3"/>
       <c r="G98" s="3"/>
@@ -8336,7 +8336,7 @@
       <c r="A99" s="28"/>
       <c r="B99" s="3"/>
       <c r="C99" s="3"/>
-      <c r="D99" s="3"/>
+      <c r="D99" s="37"/>
       <c r="E99" s="3"/>
       <c r="F99" s="3"/>
       <c r="G99" s="3"/>
@@ -8350,7 +8350,7 @@
       <c r="A100" s="28"/>
       <c r="B100" s="3"/>
       <c r="C100" s="3"/>
-      <c r="D100" s="3"/>
+      <c r="D100" s="37"/>
       <c r="E100" s="3"/>
       <c r="F100" s="3"/>
       <c r="G100" s="3"/>
@@ -8364,7 +8364,7 @@
       <c r="A101" s="28"/>
       <c r="B101" s="3"/>
       <c r="C101" s="3"/>
-      <c r="D101" s="3"/>
+      <c r="D101" s="37"/>
       <c r="E101" s="3"/>
       <c r="F101" s="3"/>
       <c r="G101" s="3"/>
@@ -8378,7 +8378,7 @@
       <c r="A102" s="28"/>
       <c r="B102" s="3"/>
       <c r="C102" s="3"/>
-      <c r="D102" s="3"/>
+      <c r="D102" s="37"/>
       <c r="E102" s="3"/>
       <c r="F102" s="3"/>
       <c r="G102" s="3"/>
@@ -8392,7 +8392,7 @@
       <c r="A103" s="28"/>
       <c r="B103" s="3"/>
       <c r="C103" s="3"/>
-      <c r="D103" s="3"/>
+      <c r="D103" s="37"/>
       <c r="E103" s="3"/>
       <c r="F103" s="3"/>
       <c r="G103" s="3"/>
@@ -8405,8 +8405,8 @@
   </sheetData>
   <autoFilter ref="A4:E103" xr:uid="{00000000-0009-0000-0000-000004000000}"/>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D5:D6" xr:uid="{BEBEE289-74B6-45AF-B472-6AAD4F987537}">
-      <formula1>"C-Type, Single"</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D5:D103" xr:uid="{BEBEE289-74B6-45AF-B472-6AAD4F987537}">
+      <formula1>"C-Type, Single, High Pass"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -9618,26 +9618,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
-  <documentManagement>
-    <iab7cdb7554d4997ae876b11632fa575 xmlns="3cada6dc-2705-46ed-bab2-0b2cd6d935ca">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </iab7cdb7554d4997ae876b11632fa575>
-    <TaxCatchAll xmlns="3cada6dc-2705-46ed-bab2-0b2cd6d935ca"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100C9B3B8AC64AC88418540180D602CE6AB" ma:contentTypeVersion="4" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="c03373d3e8f67dac2598d545e73c3e0f">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="3cada6dc-2705-46ed-bab2-0b2cd6d935ca" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="f693bfc3a603cfa0c3f0b58e702f3d19" ns2:_="">
     <xsd:import namespace="3cada6dc-2705-46ed-bab2-0b2cd6d935ca"/>
@@ -9789,10 +9769,40 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
+  <documentManagement>
+    <iab7cdb7554d4997ae876b11632fa575 xmlns="3cada6dc-2705-46ed-bab2-0b2cd6d935ca">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </iab7cdb7554d4997ae876b11632fa575>
+    <TaxCatchAll xmlns="3cada6dc-2705-46ed-bab2-0b2cd6d935ca"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7B5D7682-109C-47ED-9D9D-D061E76CCAD3}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2A5E1C23-6545-45A2-BF0C-826678B16173}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="3cada6dc-2705-46ed-bab2-0b2cd6d935ca"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -9814,19 +9824,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2A5E1C23-6545-45A2-BF0C-826678B16173}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7B5D7682-109C-47ED-9D9D-D061E76CCAD3}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="3cada6dc-2705-46ed-bab2-0b2cd6d935ca"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Minor changes to code and update to HAST_Inputs.xlsx
</commit_message>
<xml_diff>
--- a/HAST_Inputs.xlsx
+++ b/HAST_Inputs.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="20730"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1418E31-363F-41D6-A35B-F11FD743D99D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43538348-FE84-4DD1-A7F8-373B9775FDCF}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="465" windowWidth="14805" windowHeight="7650" tabRatio="868" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="465" windowWidth="14805" windowHeight="7650" tabRatio="868" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cover Sheet" sheetId="10" r:id="rId1"/>
@@ -423,7 +423,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="356" uniqueCount="307">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="465" uniqueCount="309">
   <si>
     <t>Name</t>
   </si>
@@ -506,9 +506,6 @@
     <t>Frequency Sweep Settings</t>
   </si>
   <si>
-    <t>Harmonic Loadflow Settings</t>
-  </si>
-  <si>
     <t>Studycase (.IntCase)</t>
   </si>
   <si>
@@ -1142,9 +1139,6 @@
     <t>True = Carries out a full check of the supplied cases and runs N-1 to see if they all solve in loadflow</t>
   </si>
   <si>
-    <t>True = Carries out the Harmonic Load flow</t>
-  </si>
-  <si>
     <t xml:space="preserve">True = Carries out the frequency sweep </t>
   </si>
   <si>
@@ -1154,25 +1148,13 @@
     <t>True = Deletes the 3 created folder after 1) Results under studcases, 2)Operation Scenarios, 3) Mutual Element Folder under network elements</t>
   </si>
   <si>
-    <t>True = Export the results to Excel</t>
-  </si>
-  <si>
-    <t>True = Makes Excel Visible while plotting. Can be annoying if you are doing other work as if you click the excel screen it stops the simulation</t>
-  </si>
-  <si>
     <t>True = Exports the R &amp; X data</t>
   </si>
   <si>
-    <t>True = Calculates the Convex Hull of the RX points and exports the data and adds it to the graph</t>
-  </si>
-  <si>
     <t>True = Exports the Self Impedance to excel</t>
   </si>
   <si>
     <t>True = Exports the Mutual Impedance to excel</t>
-  </si>
-  <si>
-    <t>True = Export Mutual Impedances to excel</t>
   </si>
   <si>
     <t>Stage 2</t>
@@ -1349,12 +1331,85 @@
   <si>
     <t>D:\Users\david\Desktop\</t>
   </si>
+  <si>
+    <r>
+      <t xml:space="preserve">True = Calculates the Convex Hull of the RX points and exports the data and adds it to the graph </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(This no longer does anything in HAST v2.1.4 since it is done separately)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">True = Carries out the Harmonic Load flow </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(This no longer does anything in HAST v2.1.4 since it is done separately)</t>
+    </r>
+  </si>
+  <si>
+    <t>True = Export the results to Excel (Can be done later)</t>
+  </si>
+  <si>
+    <t>This doesn't do anything</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">True = Export the HRM result to excel </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(This no longer does anything in HAST v2.1.4 since it is done separately)</t>
+    </r>
+  </si>
+  <si>
+    <t>1) Development of code to improve processing and allow multiple results to be exported</t>
+  </si>
+  <si>
+    <t>V2.1.4</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Harmonic Loadflow Settings </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="16"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(This sheet is no longer used)</t>
+    </r>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1429,6 +1484,21 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="16"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0" tint="-0.499984740745262"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1622,7 +1692,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="47">
+  <cellXfs count="48">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1709,6 +1779,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -2073,8 +2146,8 @@
   </sheetPr>
   <dimension ref="A1:D12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2086,7 +2159,7 @@
   <sheetData>
     <row r="1" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
-        <v>263</v>
+        <v>257</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -2096,7 +2169,7 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -2129,7 +2202,7 @@
     </row>
     <row r="8" spans="1:4" ht="75" x14ac:dyDescent="0.25">
       <c r="A8" s="12" t="s">
-        <v>265</v>
+        <v>259</v>
       </c>
       <c r="B8" t="s">
         <v>7</v>
@@ -2138,12 +2211,12 @@
         <v>42725</v>
       </c>
       <c r="D8" t="s">
-        <v>264</v>
+        <v>258</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>267</v>
+        <v>261</v>
       </c>
       <c r="B9" t="s">
         <v>7</v>
@@ -2152,25 +2225,36 @@
         <v>42849</v>
       </c>
       <c r="D9" t="s">
-        <v>268</v>
+        <v>262</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>275</v>
+        <v>269</v>
       </c>
       <c r="B10" s="35" t="s">
-        <v>276</v>
+        <v>270</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>277</v>
+        <v>271</v>
       </c>
       <c r="D10" t="s">
-        <v>278</v>
+        <v>272</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C11" s="4"/>
+      <c r="A11" t="s">
+        <v>306</v>
+      </c>
+      <c r="B11" s="35" t="s">
+        <v>270</v>
+      </c>
+      <c r="C11" s="4">
+        <v>43640</v>
+      </c>
+      <c r="D11" t="s">
+        <v>307</v>
+      </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C12" s="4"/>
@@ -2178,6 +2262,7 @@
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B10" r:id="rId1" xr:uid="{CC8536B1-0BA0-4FAD-8288-D1AF894BCD4C}"/>
+    <hyperlink ref="B11" r:id="rId2" xr:uid="{F4137E57-A552-4C8E-8A40-95C82D83748B}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2188,8 +2273,8 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:F24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2202,7 +2287,7 @@
   <sheetData>
     <row r="1" spans="1:6" ht="21" x14ac:dyDescent="0.35">
       <c r="A1" s="7" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="21" x14ac:dyDescent="0.35">
@@ -2210,240 +2295,240 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D3" s="39" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="E3" s="39"/>
       <c r="F3" s="39"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D4" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="E4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F4" t="s">
-        <v>250</v>
+        <v>244</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="23" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B5" s="27" t="s">
-        <v>306</v>
+        <v>300</v>
       </c>
       <c r="C5" s="25" t="s">
-        <v>253</v>
+        <v>247</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="23" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B6" s="20" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C6" s="25" t="s">
-        <v>254</v>
+        <v>248</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="23" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B7" s="20" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="C7" s="25" t="s">
-        <v>255</v>
+        <v>249</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="23" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B8" s="20" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="C8" s="25" t="s">
-        <v>256</v>
+        <v>250</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="23" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B9" s="20" t="s">
-        <v>269</v>
+        <v>263</v>
       </c>
       <c r="C9" s="25" t="s">
-        <v>257</v>
+        <v>251</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="23" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B10" s="20" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C10" s="25" t="s">
-        <v>258</v>
+        <v>252</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="23" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B11" s="20" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C11" s="25" t="s">
-        <v>259</v>
+        <v>253</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="23" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B12" s="20" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C12" s="25" t="s">
-        <v>260</v>
+        <v>254</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="23" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="B13" s="22" t="b">
         <v>1</v>
       </c>
       <c r="C13" s="21" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="23" t="s">
-        <v>261</v>
+        <v>255</v>
       </c>
       <c r="B14" s="22" t="b">
         <v>1</v>
       </c>
       <c r="C14" s="21" t="s">
-        <v>240</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" s="23" t="s">
-        <v>262</v>
-      </c>
-      <c r="B15" s="22" t="b">
+        <v>256</v>
+      </c>
+      <c r="B15" s="47" t="b">
         <v>0</v>
       </c>
       <c r="C15" s="21" t="s">
-        <v>239</v>
+        <v>302</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="23" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="B16" s="22" t="b">
         <v>0</v>
       </c>
       <c r="C16" s="21" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A17" s="23" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="B17" s="22" t="b">
         <v>1</v>
       </c>
       <c r="C17" s="21" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="23" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B18" s="22" t="b">
         <v>1</v>
       </c>
       <c r="C18" s="21" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="23" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B19" s="22" t="b">
         <v>0</v>
       </c>
       <c r="C19" s="21" t="s">
-        <v>244</v>
+        <v>304</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="B20" s="22" t="b">
         <v>1</v>
       </c>
       <c r="C20" s="21" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>234</v>
-      </c>
-      <c r="B21" s="22" t="b">
+        <v>233</v>
+      </c>
+      <c r="B21" s="47" t="b">
         <v>0</v>
       </c>
       <c r="C21" s="21" t="s">
-        <v>246</v>
+        <v>301</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="23" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B22" s="22" t="b">
         <v>1</v>
       </c>
       <c r="C22" s="21" t="s">
-        <v>247</v>
+        <v>242</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="23" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="B23" s="22" t="b">
         <v>1</v>
       </c>
       <c r="C23" s="21" t="s">
-        <v>248</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A24" s="23" t="s">
-        <v>237</v>
-      </c>
-      <c r="B24" s="22" t="b">
+        <v>236</v>
+      </c>
+      <c r="B24" s="47" t="b">
         <v>0</v>
       </c>
       <c r="C24" s="21" t="s">
-        <v>249</v>
+        <v>305</v>
       </c>
     </row>
   </sheetData>
@@ -2495,52 +2580,52 @@
         <v>9</v>
       </c>
       <c r="C4" s="32" t="s">
+        <v>27</v>
+      </c>
+      <c r="D4" s="33" t="s">
         <v>28</v>
-      </c>
-      <c r="D4" s="33" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
+        <v>289</v>
+      </c>
+      <c r="B5" s="34" t="s">
         <v>295</v>
       </c>
-      <c r="B5" s="34" t="s">
-        <v>301</v>
-      </c>
       <c r="C5" s="34" t="s">
-        <v>289</v>
+        <v>283</v>
       </c>
       <c r="D5" s="34" t="s">
-        <v>290</v>
+        <v>284</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>302</v>
+        <v>296</v>
       </c>
       <c r="B6" s="34" t="s">
-        <v>301</v>
+        <v>295</v>
       </c>
       <c r="C6" s="34" t="s">
-        <v>289</v>
+        <v>283</v>
       </c>
       <c r="D6" s="34" t="s">
-        <v>303</v>
+        <v>297</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>304</v>
+        <v>298</v>
       </c>
       <c r="B7" s="34" t="s">
-        <v>305</v>
+        <v>299</v>
       </c>
       <c r="C7" s="34" t="s">
-        <v>289</v>
+        <v>283</v>
       </c>
       <c r="D7" s="34" t="s">
-        <v>290</v>
+        <v>284</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -2725,7 +2810,7 @@
         <v>20</v>
       </c>
       <c r="D4" s="9" t="s">
-        <v>266</v>
+        <v>260</v>
       </c>
       <c r="E4" s="11" t="s">
         <v>19</v>
@@ -2734,7 +2819,7 @@
         <v>20</v>
       </c>
       <c r="G4" s="9" t="s">
-        <v>266</v>
+        <v>260</v>
       </c>
       <c r="H4" s="11" t="s">
         <v>19</v>
@@ -2743,7 +2828,7 @@
         <v>20</v>
       </c>
       <c r="J4" s="9" t="s">
-        <v>266</v>
+        <v>260</v>
       </c>
       <c r="K4" s="11" t="s">
         <v>19</v>
@@ -2752,7 +2837,7 @@
         <v>20</v>
       </c>
       <c r="M4" s="9" t="s">
-        <v>266</v>
+        <v>260</v>
       </c>
       <c r="N4" s="11" t="s">
         <v>19</v>
@@ -2761,7 +2846,7 @@
         <v>20</v>
       </c>
       <c r="P4" s="9" t="s">
-        <v>266</v>
+        <v>260</v>
       </c>
       <c r="Q4" s="11" t="s">
         <v>19</v>
@@ -2770,7 +2855,7 @@
         <v>20</v>
       </c>
       <c r="S4" s="9" t="s">
-        <v>266</v>
+        <v>260</v>
       </c>
       <c r="T4" s="11" t="s">
         <v>19</v>
@@ -2779,7 +2864,7 @@
         <v>20</v>
       </c>
       <c r="V4" s="9" t="s">
-        <v>266</v>
+        <v>260</v>
       </c>
       <c r="W4" s="11" t="s">
         <v>19</v>
@@ -2788,7 +2873,7 @@
         <v>20</v>
       </c>
       <c r="Y4" s="9" t="s">
-        <v>266</v>
+        <v>260</v>
       </c>
       <c r="Z4" s="11" t="s">
         <v>19</v>
@@ -2797,12 +2882,12 @@
         <v>20</v>
       </c>
       <c r="AB4" s="9" t="s">
-        <v>266</v>
+        <v>260</v>
       </c>
     </row>
     <row r="5" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
-        <v>271</v>
+        <v>265</v>
       </c>
       <c r="B5" s="5">
         <v>0</v>
@@ -2836,25 +2921,25 @@
     </row>
     <row r="6" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>296</v>
+        <v>290</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>273</v>
+        <v>267</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>297</v>
+        <v>291</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>298</v>
+        <v>292</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>299</v>
+        <v>293</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>300</v>
+        <v>294</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>298</v>
+        <v>292</v>
       </c>
       <c r="H6" s="28"/>
       <c r="I6" s="28"/>
@@ -6319,18 +6404,18 @@
         <v>21</v>
       </c>
       <c r="D4" s="36" t="s">
-        <v>274</v>
+        <v>268</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>291</v>
+        <v>285</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>292</v>
+        <v>286</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>293</v>
+        <v>287</v>
       </c>
       <c r="D5" s="3" t="b">
         <v>1</v>
@@ -6338,13 +6423,13 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>272</v>
+        <v>266</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>273</v>
+        <v>267</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>270</v>
+        <v>264</v>
       </c>
       <c r="D6" s="3" t="b">
         <v>1</v>
@@ -6957,7 +7042,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D08D4187-8BE1-4B7A-A634-AC08177090E1}">
   <dimension ref="A1:L103"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
@@ -6970,17 +7055,17 @@
   <sheetData>
     <row r="1" spans="1:12" ht="21" x14ac:dyDescent="0.35">
       <c r="A1" s="7" t="s">
-        <v>279</v>
+        <v>273</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>281</v>
+        <v>275</v>
       </c>
     </row>
     <row r="4" spans="1:12" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A4" s="26" t="s">
-        <v>294</v>
+        <v>288</v>
       </c>
       <c r="B4" s="26" t="s">
         <v>19</v>
@@ -6989,31 +7074,31 @@
         <v>21</v>
       </c>
       <c r="D4" s="26" t="s">
+        <v>274</v>
+      </c>
+      <c r="E4" s="36" t="s">
+        <v>276</v>
+      </c>
+      <c r="F4" s="36" t="s">
+        <v>277</v>
+      </c>
+      <c r="G4" s="36" t="s">
+        <v>282</v>
+      </c>
+      <c r="H4" s="36" t="s">
+        <v>278</v>
+      </c>
+      <c r="I4" s="36" t="s">
+        <v>279</v>
+      </c>
+      <c r="J4" s="36" t="s">
+        <v>282</v>
+      </c>
+      <c r="K4" s="36" t="s">
         <v>280</v>
       </c>
-      <c r="E4" s="36" t="s">
-        <v>282</v>
-      </c>
-      <c r="F4" s="36" t="s">
-        <v>283</v>
-      </c>
-      <c r="G4" s="36" t="s">
-        <v>288</v>
-      </c>
-      <c r="H4" s="36" t="s">
-        <v>284</v>
-      </c>
-      <c r="I4" s="36" t="s">
-        <v>285</v>
-      </c>
-      <c r="J4" s="36" t="s">
-        <v>288</v>
-      </c>
-      <c r="K4" s="36" t="s">
-        <v>286</v>
-      </c>
       <c r="L4" s="36" t="s">
-        <v>287</v>
+        <v>281</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
@@ -8454,13 +8539,13 @@
     </row>
     <row r="5" spans="1:7" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="46" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B5" s="12" t="s">
-        <v>251</v>
+        <v>245</v>
       </c>
       <c r="C5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D5">
         <v>0</v>
@@ -8469,10 +8554,10 @@
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="46"/>
       <c r="B6" s="12" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C6" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D6">
         <v>1</v>
@@ -8481,10 +8566,10 @@
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="46"/>
       <c r="B7" s="12" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C7" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D7">
         <v>1</v>
@@ -8493,10 +8578,10 @@
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="46"/>
       <c r="B8" s="12" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C8" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D8">
         <v>1</v>
@@ -8505,10 +8590,10 @@
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="46"/>
       <c r="B9" s="12" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C9" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D9">
         <v>1</v>
@@ -8517,10 +8602,10 @@
     <row r="10" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="46"/>
       <c r="B10" s="12" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C10" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D10">
         <v>0</v>
@@ -8529,10 +8614,10 @@
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="46"/>
       <c r="B11" s="12" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C11" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D11">
         <v>1</v>
@@ -8541,10 +8626,10 @@
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="46"/>
       <c r="B12" s="12" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C12" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D12">
         <v>1</v>
@@ -8553,10 +8638,10 @@
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="46"/>
       <c r="B13" s="12" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C13" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D13">
         <v>0</v>
@@ -8565,10 +8650,10 @@
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="46"/>
       <c r="B14" s="12" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C14" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D14">
         <v>100</v>
@@ -8576,13 +8661,13 @@
     </row>
     <row r="15" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A15" s="46" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B15" s="12" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C15" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D15">
         <v>1</v>
@@ -8591,10 +8676,10 @@
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="46"/>
       <c r="B16" s="12" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C16" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D16">
         <v>1</v>
@@ -8603,10 +8688,10 @@
     <row r="17" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A17" s="46"/>
       <c r="B17" s="12" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C17" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D17">
         <v>0</v>
@@ -8615,22 +8700,22 @@
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="46"/>
       <c r="B18" s="16" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C18" s="19" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="D18" s="18" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="46"/>
       <c r="B19" s="12" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C19" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D19">
         <v>0</v>
@@ -8638,13 +8723,13 @@
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="46" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B20" s="12" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C20" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D20">
         <v>0</v>
@@ -8653,10 +8738,10 @@
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="46"/>
       <c r="B21" s="12" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C21" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D21">
         <v>0</v>
@@ -8665,10 +8750,10 @@
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="46"/>
       <c r="B22" s="12" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C22" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D22">
         <v>0</v>
@@ -8677,10 +8762,10 @@
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="46"/>
       <c r="B23" s="12" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C23" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D23">
         <v>1</v>
@@ -8689,10 +8774,10 @@
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="46"/>
       <c r="B24" s="12" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C24" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D24">
         <v>20</v>
@@ -8701,10 +8786,10 @@
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="46"/>
       <c r="B25" s="12" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C25" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D25">
         <v>0</v>
@@ -8713,10 +8798,10 @@
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="46"/>
       <c r="B26" s="12" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C26" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D26">
         <v>1</v>
@@ -8725,10 +8810,10 @@
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="46"/>
       <c r="B27" s="12" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C27" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D27">
         <v>0</v>
@@ -8737,10 +8822,10 @@
     <row r="28" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A28" s="46"/>
       <c r="B28" s="12" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C28" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D28">
         <v>2</v>
@@ -8749,10 +8834,10 @@
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="46"/>
       <c r="B29" s="12" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C29" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D29">
         <v>0</v>
@@ -8761,10 +8846,10 @@
     <row r="30" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A30" s="46"/>
       <c r="B30" s="12" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C30" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D30">
         <v>0</v>
@@ -8772,13 +8857,13 @@
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" s="46" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B31" s="12" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C31" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D31">
         <v>100</v>
@@ -8787,10 +8872,10 @@
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" s="46"/>
       <c r="B32" s="12" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C32" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D32">
         <v>80</v>
@@ -8799,10 +8884,10 @@
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="46"/>
       <c r="B33" s="12" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C33" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D33">
         <v>5</v>
@@ -8811,10 +8896,10 @@
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" s="46"/>
       <c r="B34" s="12" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C34" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D34">
         <v>10000</v>
@@ -8823,10 +8908,10 @@
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" s="46"/>
       <c r="B35" s="12" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C35" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D35">
         <v>10</v>
@@ -8835,10 +8920,10 @@
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" s="46"/>
       <c r="B36" s="12" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C36" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D36">
         <v>1</v>
@@ -8847,10 +8932,10 @@
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" s="46"/>
       <c r="B37" s="12" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C37" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D37">
         <v>1</v>
@@ -8859,10 +8944,10 @@
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" s="46"/>
       <c r="B38" s="12" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C38" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D38">
         <v>1</v>
@@ -8870,13 +8955,13 @@
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" s="46" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B39" s="12" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C39" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D39">
         <v>0</v>
@@ -8885,10 +8970,10 @@
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" s="46"/>
       <c r="B40" s="12" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C40" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D40">
         <v>1</v>
@@ -8897,10 +8982,10 @@
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" s="46"/>
       <c r="B41" s="12" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C41" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D41">
         <v>2</v>
@@ -8909,10 +8994,10 @@
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" s="46"/>
       <c r="B42" s="12" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C42" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D42">
         <v>1</v>
@@ -8921,10 +9006,10 @@
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" s="46"/>
       <c r="B43" s="12" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C43" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D43">
         <v>110</v>
@@ -8933,10 +9018,10 @@
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" s="46"/>
       <c r="B44" s="12" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C44" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D44">
         <v>0.9</v>
@@ -8945,10 +9030,10 @@
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" s="46"/>
       <c r="B45" s="12" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C45" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D45">
         <v>1.1200000000000001</v>
@@ -8957,22 +9042,22 @@
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" s="46"/>
       <c r="B46" s="16" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C46" s="19" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D46" s="18" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" s="46"/>
       <c r="B47" s="12" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C47" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D47">
         <v>1</v>
@@ -8981,24 +9066,24 @@
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" s="46"/>
       <c r="B48" s="16" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C48" s="19" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D48" s="18" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" s="46" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B49" s="12" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C49" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D49">
         <v>100</v>
@@ -9007,10 +9092,10 @@
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" s="46"/>
       <c r="B50" s="12" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C50" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D50">
         <v>100</v>
@@ -9019,10 +9104,10 @@
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" s="46"/>
       <c r="B51" s="12" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C51" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D51">
         <v>100</v>
@@ -9030,13 +9115,13 @@
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" s="46" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B52" s="12" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C52" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D52">
         <v>0</v>
@@ -9045,10 +9130,10 @@
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" s="46"/>
       <c r="B53" s="12" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C53" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D53">
         <v>0.9</v>
@@ -9057,10 +9142,10 @@
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" s="46"/>
       <c r="B54" s="12" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C54" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D54">
         <v>12</v>
@@ -9069,10 +9154,10 @@
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" s="46"/>
       <c r="B55" s="12" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C55" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D55">
         <v>0.95</v>
@@ -9081,10 +9166,10 @@
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" s="46"/>
       <c r="B56" s="12" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C56" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D56">
         <v>0.1</v>
@@ -9093,10 +9178,10 @@
     <row r="57" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A57" s="46"/>
       <c r="B57" s="12" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C57" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D57">
         <v>1</v>
@@ -9104,13 +9189,13 @@
     </row>
     <row r="58" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A58" s="46" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B58" s="12" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C58" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D58">
         <v>1</v>
@@ -9119,10 +9204,10 @@
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59" s="46"/>
       <c r="B59" s="12" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C59" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D59">
         <v>1</v>
@@ -9177,18 +9262,18 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="46" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B5" s="12" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="C5" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="D5" s="14">
         <v>50</v>
@@ -9197,10 +9282,10 @@
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="46"/>
       <c r="B6" s="12" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="C6" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="D6" s="14">
         <v>1025</v>
@@ -9209,10 +9294,10 @@
     <row r="7" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="46"/>
       <c r="B7" s="12" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C7" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="D7">
         <v>0</v>
@@ -9221,10 +9306,10 @@
     <row r="8" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="46"/>
       <c r="B8" s="12" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C8" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="D8" s="14">
         <v>50</v>
@@ -9233,10 +9318,10 @@
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="46"/>
       <c r="B9" s="12" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="C9" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="D9">
         <f>D6</f>
@@ -9246,10 +9331,10 @@
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="46"/>
       <c r="B10" s="12" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="C10" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="D10">
         <v>5</v>
@@ -9258,10 +9343,10 @@
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="46"/>
       <c r="B11" s="12" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="C11" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="D11">
         <v>0</v>
@@ -9270,10 +9355,10 @@
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="46"/>
       <c r="B12" s="12" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="C12" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="D12">
         <f>D5</f>
@@ -9283,10 +9368,10 @@
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="46"/>
       <c r="B13" s="12" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="C13" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="D13">
         <f>D6</f>
@@ -9296,10 +9381,10 @@
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="46"/>
       <c r="B14" s="12" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="C14" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="D14">
         <f>D6/D5</f>
@@ -9309,36 +9394,36 @@
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="46"/>
       <c r="B15" s="16" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C15" s="17" t="s">
+        <v>174</v>
+      </c>
+      <c r="D15" s="18" t="s">
         <v>175</v>
-      </c>
-      <c r="D15" s="18" t="s">
-        <v>176</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="46"/>
       <c r="B16" s="16" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C16" s="17" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="D16" s="18" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A17" s="46" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B17" s="12" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="C17" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="D17">
         <v>0.01</v>
@@ -9347,10 +9432,10 @@
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="46"/>
       <c r="B18" s="12" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C18" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D18">
         <v>5.0000000000000001E-3</v>
@@ -9359,10 +9444,10 @@
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="46"/>
       <c r="B19" s="12" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C19" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="D19">
         <v>10</v>
@@ -9371,10 +9456,10 @@
     <row r="20" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A20" s="46"/>
       <c r="B20" s="12" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="C20" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="D20">
         <v>0</v>
@@ -9401,7 +9486,7 @@
   <dimension ref="A1:D19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9414,17 +9499,17 @@
   <sheetData>
     <row r="1" spans="1:4" ht="21" x14ac:dyDescent="0.35">
       <c r="A1" s="7" t="s">
-        <v>27</v>
+        <v>308</v>
       </c>
       <c r="B1" s="7"/>
     </row>
     <row r="5" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="46"/>
       <c r="B5" s="12" t="s">
-        <v>252</v>
+        <v>246</v>
       </c>
       <c r="C5" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="D5">
         <v>0</v>
@@ -9433,10 +9518,10 @@
     <row r="6" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="46"/>
       <c r="B6" s="12" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="C6" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="D6" s="14">
         <v>1</v>
@@ -9445,10 +9530,10 @@
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="46"/>
       <c r="B7" s="12" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="C7" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="D7">
         <v>0</v>
@@ -9457,10 +9542,10 @@
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="46"/>
       <c r="B8" s="12" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C8" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="D8">
         <v>0</v>
@@ -9469,10 +9554,10 @@
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="46"/>
       <c r="B9" s="12" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="C9" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="D9" s="24">
         <v>50</v>
@@ -9481,10 +9566,10 @@
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="46"/>
       <c r="B10" s="12" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="C10" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="D10" s="14">
         <v>150</v>
@@ -9493,10 +9578,10 @@
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="46"/>
       <c r="B11" s="12" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="C11" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="D11">
         <f>D10/D9</f>
@@ -9506,36 +9591,36 @@
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="46"/>
       <c r="B12" s="16" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C12" s="19" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="D12" s="18" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="46"/>
       <c r="B13" s="16" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C13" s="19" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="D13" s="18" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A14" s="15" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="B14" s="12" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C14" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="D14">
         <v>0</v>
@@ -9543,13 +9628,13 @@
     </row>
     <row r="15" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A15" s="46" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B15" s="12" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="C15" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="D15">
         <v>0</v>
@@ -9558,10 +9643,10 @@
     <row r="16" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A16" s="46"/>
       <c r="B16" s="12" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="C16" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="D16">
         <v>3</v>
@@ -9570,10 +9655,10 @@
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="46"/>
       <c r="B17" s="12" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="C17" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="D17">
         <v>0</v>
@@ -9582,10 +9667,10 @@
     <row r="18" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A18" s="46"/>
       <c r="B18" s="12" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="C18" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="D18">
         <v>0</v>
@@ -9594,10 +9679,10 @@
     <row r="19" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A19" s="46"/>
       <c r="B19" s="12" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="C19" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="D19">
         <v>1.6</v>
@@ -9770,6 +9855,15 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
   <documentManagement>
     <iab7cdb7554d4997ae876b11632fa575 xmlns="3cada6dc-2705-46ed-bab2-0b2cd6d935ca">
@@ -9778,15 +9872,6 @@
     <TaxCatchAll xmlns="3cada6dc-2705-46ed-bab2-0b2cd6d935ca"/>
   </documentManagement>
 </p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -9808,6 +9893,14 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7B5D7682-109C-47ED-9D9D-D061E76CCAD3}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FCC61AA8-C35E-4598-8617-08B80F018AC2}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
@@ -9821,12 +9914,4 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7B5D7682-109C-47ED-9D9D-D061E76CCAD3}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Resolved issues with study running in PF 2019
</commit_message>
<xml_diff>
--- a/HAST_Inputs.xlsx
+++ b/HAST_Inputs.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="20730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21328"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43538348-FE84-4DD1-A7F8-373B9775FDCF}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65E45D54-9CB5-46F8-B382-FCFF1BCD4C4E}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="465" windowWidth="14805" windowHeight="7650" tabRatio="868" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="868" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cover Sheet" sheetId="10" r:id="rId1"/>
@@ -28,6 +28,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -423,7 +424,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="465" uniqueCount="309">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="344" uniqueCount="297">
   <si>
     <t>Name</t>
   </si>
@@ -755,9 +756,6 @@
     <t>(0 Ref Machine, 1 Load, Static Gen, Dist slack by loads, Dist slack by Sync,</t>
   </si>
   <si>
-    <t>Reference Busbar</t>
-  </si>
-  <si>
     <t>Angle</t>
   </si>
   <si>
@@ -1092,9 +1090,6 @@
   </si>
   <si>
     <t>ldf</t>
-  </si>
-  <si>
-    <t>EIRGRID\Turlough Hill\220 kV T2001/2 TCB.ElmTerm</t>
   </si>
   <si>
     <t>harm</t>
@@ -1227,12 +1222,6 @@
     <t>Base_Case</t>
   </si>
   <si>
-    <t>Clonee 220 kV</t>
-  </si>
-  <si>
-    <t>Clonee</t>
-  </si>
-  <si>
     <t>Mutual</t>
   </si>
   <si>
@@ -1278,55 +1267,7 @@
     <t>Number of Steps</t>
   </si>
   <si>
-    <t>BC_CustDevs_CLOph3</t>
-  </si>
-  <si>
-    <t>SV 2.5GW E-250 M0 W1350</t>
-  </si>
-  <si>
-    <t>Bracetown 220 kV</t>
-  </si>
-  <si>
-    <t>Bracetown</t>
-  </si>
-  <si>
-    <t>220 kV A2</t>
-  </si>
-  <si>
     <t>Filter Name</t>
-  </si>
-  <si>
-    <t>SC1</t>
-  </si>
-  <si>
-    <t>CLO2-CDU2-ckt1</t>
-  </si>
-  <si>
-    <t>220 kV Corduff CB</t>
-  </si>
-  <si>
-    <t>Open</t>
-  </si>
-  <si>
-    <t>Corduff</t>
-  </si>
-  <si>
-    <t>220 kV Clonee CB</t>
-  </si>
-  <si>
-    <t>AIM 2017-MODEL-07022019-TAP_TEST</t>
-  </si>
-  <si>
-    <t>SC2</t>
-  </si>
-  <si>
-    <t>WP 6.7GW E150 M0 W0</t>
-  </si>
-  <si>
-    <t>SC3</t>
-  </si>
-  <si>
-    <t>AIM 2017-MODEL-07022019-TAP_TEST2</t>
   </si>
   <si>
     <t>D:\Users\david\Desktop\</t>
@@ -1403,6 +1344,30 @@
       </rPr>
       <t>(This sheet is no longer used)</t>
     </r>
+  </si>
+  <si>
+    <t>BASE</t>
+  </si>
+  <si>
+    <t>AIM 2019-MODEL-RELEASE v1.0(JI7867)</t>
+  </si>
+  <si>
+    <t>CP966</t>
+  </si>
+  <si>
+    <t>SV-HW</t>
+  </si>
+  <si>
+    <t>EirGrid\Turlough Hill\220 kV T2001/2 TCB</t>
+  </si>
+  <si>
+    <t>Reference Busbar (NetElements\Substation\Terminal)</t>
+  </si>
+  <si>
+    <t>Woodland</t>
+  </si>
+  <si>
+    <t>Dunstown</t>
   </si>
 </sst>
 </file>
@@ -1756,6 +1721,9 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1779,9 +1747,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -2146,7 +2111,7 @@
   </sheetPr>
   <dimension ref="A1:D12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
@@ -2159,7 +2124,7 @@
   <sheetData>
     <row r="1" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -2202,7 +2167,7 @@
     </row>
     <row r="8" spans="1:4" ht="75" x14ac:dyDescent="0.25">
       <c r="A8" s="12" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="B8" t="s">
         <v>7</v>
@@ -2211,12 +2176,12 @@
         <v>42725</v>
       </c>
       <c r="D8" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="B9" t="s">
         <v>7</v>
@@ -2225,35 +2190,35 @@
         <v>42849</v>
       </c>
       <c r="D9" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
       <c r="B10" s="35" t="s">
-        <v>270</v>
+        <v>266</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>271</v>
+        <v>267</v>
       </c>
       <c r="D10" t="s">
-        <v>272</v>
+        <v>268</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>306</v>
+        <v>286</v>
       </c>
       <c r="B11" s="35" t="s">
-        <v>270</v>
+        <v>266</v>
       </c>
       <c r="C11" s="4">
         <v>43640</v>
       </c>
       <c r="D11" t="s">
-        <v>307</v>
+        <v>287</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -2274,7 +2239,7 @@
   <dimension ref="A1:F24"/>
   <sheetViews>
     <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2294,21 +2259,21 @@
       <c r="A2" s="7"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="D3" s="39" t="s">
-        <v>226</v>
-      </c>
-      <c r="E3" s="39"/>
-      <c r="F3" s="39"/>
+      <c r="D3" s="40" t="s">
+        <v>224</v>
+      </c>
+      <c r="E3" s="40"/>
+      <c r="F3" s="40"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D4" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="E4" t="s">
         <v>44</v>
       </c>
       <c r="F4" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -2316,10 +2281,10 @@
         <v>32</v>
       </c>
       <c r="B5" s="27" t="s">
-        <v>300</v>
+        <v>280</v>
       </c>
       <c r="C5" s="25" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -2330,7 +2295,7 @@
         <v>42</v>
       </c>
       <c r="C6" s="25" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
@@ -2338,10 +2303,10 @@
         <v>34</v>
       </c>
       <c r="B7" s="20" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="C7" s="25" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -2349,10 +2314,10 @@
         <v>35</v>
       </c>
       <c r="B8" s="20" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="C8" s="25" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -2360,10 +2325,10 @@
         <v>36</v>
       </c>
       <c r="B9" s="20" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="C9" s="25" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -2374,7 +2339,7 @@
         <v>41</v>
       </c>
       <c r="C10" s="25" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -2385,7 +2350,7 @@
         <v>42</v>
       </c>
       <c r="C11" s="25" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -2396,62 +2361,62 @@
         <v>43</v>
       </c>
       <c r="C12" s="25" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="23" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="B13" s="22" t="b">
         <v>1</v>
       </c>
       <c r="C13" s="21" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="23" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="B14" s="22" t="b">
         <v>1</v>
       </c>
       <c r="C14" s="21" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" s="23" t="s">
-        <v>256</v>
-      </c>
-      <c r="B15" s="47" t="b">
+        <v>254</v>
+      </c>
+      <c r="B15" s="39" t="b">
         <v>0</v>
       </c>
       <c r="C15" s="21" t="s">
-        <v>302</v>
+        <v>282</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="23" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="B16" s="22" t="b">
         <v>0</v>
       </c>
       <c r="C16" s="21" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A17" s="23" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="B17" s="22" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C17" s="21" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
@@ -2462,7 +2427,7 @@
         <v>1</v>
       </c>
       <c r="C18" s="21" t="s">
-        <v>303</v>
+        <v>283</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
@@ -2473,62 +2438,62 @@
         <v>0</v>
       </c>
       <c r="C19" s="21" t="s">
-        <v>304</v>
+        <v>284</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="B20" s="22" t="b">
         <v>1</v>
       </c>
       <c r="C20" s="21" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
     </row>
     <row r="21" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>233</v>
-      </c>
-      <c r="B21" s="47" t="b">
+        <v>231</v>
+      </c>
+      <c r="B21" s="39" t="b">
         <v>0</v>
       </c>
       <c r="C21" s="21" t="s">
-        <v>301</v>
+        <v>281</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="23" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="B22" s="22" t="b">
         <v>1</v>
       </c>
       <c r="C22" s="21" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="23" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="B23" s="22" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C23" s="21" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
     </row>
     <row r="24" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A24" s="23" t="s">
-        <v>236</v>
-      </c>
-      <c r="B24" s="47" t="b">
+        <v>234</v>
+      </c>
+      <c r="B24" s="39" t="b">
         <v>0</v>
       </c>
       <c r="C24" s="21" t="s">
-        <v>305</v>
+        <v>285</v>
       </c>
     </row>
   </sheetData>
@@ -2552,7 +2517,7 @@
   <dimension ref="A1:D22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A19" sqref="A19"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2591,42 +2556,26 @@
         <v>289</v>
       </c>
       <c r="B5" s="34" t="s">
-        <v>295</v>
+        <v>290</v>
       </c>
       <c r="C5" s="34" t="s">
-        <v>283</v>
+        <v>291</v>
       </c>
       <c r="D5" s="34" t="s">
-        <v>284</v>
+        <v>292</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="3" t="s">
-        <v>296</v>
-      </c>
-      <c r="B6" s="34" t="s">
-        <v>295</v>
-      </c>
-      <c r="C6" s="34" t="s">
-        <v>283</v>
-      </c>
-      <c r="D6" s="34" t="s">
-        <v>297</v>
-      </c>
+      <c r="A6" s="3"/>
+      <c r="B6" s="34"/>
+      <c r="C6" s="34"/>
+      <c r="D6" s="34"/>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="3" t="s">
-        <v>298</v>
-      </c>
-      <c r="B7" s="34" t="s">
-        <v>299</v>
-      </c>
-      <c r="C7" s="34" t="s">
-        <v>283</v>
-      </c>
-      <c r="D7" s="34" t="s">
-        <v>284</v>
-      </c>
+      <c r="A7" s="3"/>
+      <c r="B7" s="34"/>
+      <c r="C7" s="34"/>
+      <c r="D7" s="34"/>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="3"/>
@@ -2731,7 +2680,7 @@
   <dimension ref="A1:AB165"/>
   <sheetViews>
     <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="E37" sqref="E37:E39"/>
+      <selection activeCell="A6" sqref="A6:G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2753,51 +2702,51 @@
     </row>
     <row r="2" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="3" spans="1:28" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="43" t="s">
+      <c r="B3" s="44" t="s">
         <v>10</v>
       </c>
-      <c r="C3" s="44"/>
-      <c r="D3" s="45"/>
-      <c r="E3" s="40" t="s">
+      <c r="C3" s="45"/>
+      <c r="D3" s="46"/>
+      <c r="E3" s="41" t="s">
         <v>11</v>
       </c>
-      <c r="F3" s="41"/>
-      <c r="G3" s="42"/>
-      <c r="H3" s="40" t="s">
+      <c r="F3" s="42"/>
+      <c r="G3" s="43"/>
+      <c r="H3" s="41" t="s">
         <v>12</v>
       </c>
-      <c r="I3" s="41"/>
-      <c r="J3" s="42"/>
-      <c r="K3" s="40" t="s">
+      <c r="I3" s="42"/>
+      <c r="J3" s="43"/>
+      <c r="K3" s="41" t="s">
         <v>13</v>
       </c>
-      <c r="L3" s="41"/>
-      <c r="M3" s="42"/>
-      <c r="N3" s="40" t="s">
+      <c r="L3" s="42"/>
+      <c r="M3" s="43"/>
+      <c r="N3" s="41" t="s">
         <v>14</v>
       </c>
-      <c r="O3" s="41"/>
-      <c r="P3" s="42"/>
-      <c r="Q3" s="40" t="s">
+      <c r="O3" s="42"/>
+      <c r="P3" s="43"/>
+      <c r="Q3" s="41" t="s">
         <v>15</v>
       </c>
-      <c r="R3" s="41"/>
-      <c r="S3" s="42"/>
-      <c r="T3" s="40" t="s">
+      <c r="R3" s="42"/>
+      <c r="S3" s="43"/>
+      <c r="T3" s="41" t="s">
         <v>16</v>
       </c>
-      <c r="U3" s="41"/>
-      <c r="V3" s="42"/>
-      <c r="W3" s="40" t="s">
+      <c r="U3" s="42"/>
+      <c r="V3" s="43"/>
+      <c r="W3" s="41" t="s">
         <v>17</v>
       </c>
-      <c r="X3" s="41"/>
-      <c r="Y3" s="42"/>
-      <c r="Z3" s="40" t="s">
+      <c r="X3" s="42"/>
+      <c r="Y3" s="43"/>
+      <c r="Z3" s="41" t="s">
         <v>18</v>
       </c>
-      <c r="AA3" s="41"/>
-      <c r="AB3" s="42"/>
+      <c r="AA3" s="42"/>
+      <c r="AB3" s="43"/>
     </row>
     <row r="4" spans="1:28" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="6" t="s">
@@ -2810,7 +2759,7 @@
         <v>20</v>
       </c>
       <c r="D4" s="9" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="E4" s="11" t="s">
         <v>19</v>
@@ -2819,7 +2768,7 @@
         <v>20</v>
       </c>
       <c r="G4" s="9" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="H4" s="11" t="s">
         <v>19</v>
@@ -2828,7 +2777,7 @@
         <v>20</v>
       </c>
       <c r="J4" s="9" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="K4" s="11" t="s">
         <v>19</v>
@@ -2837,7 +2786,7 @@
         <v>20</v>
       </c>
       <c r="M4" s="9" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="N4" s="11" t="s">
         <v>19</v>
@@ -2846,7 +2795,7 @@
         <v>20</v>
       </c>
       <c r="P4" s="9" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="Q4" s="11" t="s">
         <v>19</v>
@@ -2855,7 +2804,7 @@
         <v>20</v>
       </c>
       <c r="S4" s="9" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="T4" s="11" t="s">
         <v>19</v>
@@ -2864,7 +2813,7 @@
         <v>20</v>
       </c>
       <c r="V4" s="9" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="W4" s="11" t="s">
         <v>19</v>
@@ -2873,7 +2822,7 @@
         <v>20</v>
       </c>
       <c r="Y4" s="9" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="Z4" s="11" t="s">
         <v>19</v>
@@ -2882,12 +2831,12 @@
         <v>20</v>
       </c>
       <c r="AB4" s="9" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
     </row>
     <row r="5" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="B5" s="5">
         <v>0</v>
@@ -2920,27 +2869,13 @@
       <c r="AB5" s="3"/>
     </row>
     <row r="6" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A6" s="3" t="s">
-        <v>290</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>267</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>291</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>292</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>293</v>
-      </c>
-      <c r="F6" s="3" t="s">
-        <v>294</v>
-      </c>
-      <c r="G6" s="3" t="s">
-        <v>292</v>
-      </c>
+      <c r="A6" s="3"/>
+      <c r="B6" s="3"/>
+      <c r="C6" s="3"/>
+      <c r="D6" s="3"/>
+      <c r="E6" s="3"/>
+      <c r="F6" s="3"/>
+      <c r="G6" s="3"/>
       <c r="H6" s="28"/>
       <c r="I6" s="28"/>
       <c r="J6" s="28"/>
@@ -6343,7 +6278,7 @@
     </row>
   </sheetData>
   <autoFilter ref="A4:AB165" xr:uid="{00000000-0009-0000-0000-000003000000}"/>
-  <sortState ref="A53:J152">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A53:J152">
     <sortCondition ref="A53:A152"/>
   </sortState>
   <mergeCells count="9">
@@ -6371,8 +6306,8 @@
   <sheetPr codeName="Sheet5"/>
   <dimension ref="A1:D103"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I13" sqref="I13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6404,35 +6339,35 @@
         <v>21</v>
       </c>
       <c r="D4" s="36" t="s">
-        <v>268</v>
+        <v>264</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>285</v>
+        <v>295</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>286</v>
+        <v>295</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>287</v>
+        <v>262</v>
       </c>
       <c r="D5" s="3" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>266</v>
+        <v>296</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>267</v>
+        <v>296</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="D6" s="3" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -7019,7 +6954,7 @@
     </row>
   </sheetData>
   <autoFilter ref="A4:D103" xr:uid="{00000000-0009-0000-0000-000004000000}"/>
-  <sortState ref="A5:A8">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A5:A8">
     <sortCondition ref="A5:A8"/>
   </sortState>
   <conditionalFormatting sqref="A5:A103">
@@ -7055,17 +6990,17 @@
   <sheetData>
     <row r="1" spans="1:12" ht="21" x14ac:dyDescent="0.35">
       <c r="A1" s="7" t="s">
-        <v>273</v>
+        <v>269</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>275</v>
+        <v>271</v>
       </c>
     </row>
     <row r="4" spans="1:12" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A4" s="26" t="s">
-        <v>288</v>
+        <v>279</v>
       </c>
       <c r="B4" s="26" t="s">
         <v>19</v>
@@ -7074,31 +7009,31 @@
         <v>21</v>
       </c>
       <c r="D4" s="26" t="s">
+        <v>270</v>
+      </c>
+      <c r="E4" s="36" t="s">
+        <v>272</v>
+      </c>
+      <c r="F4" s="36" t="s">
+        <v>273</v>
+      </c>
+      <c r="G4" s="36" t="s">
+        <v>278</v>
+      </c>
+      <c r="H4" s="36" t="s">
         <v>274</v>
       </c>
-      <c r="E4" s="36" t="s">
+      <c r="I4" s="36" t="s">
+        <v>275</v>
+      </c>
+      <c r="J4" s="36" t="s">
+        <v>278</v>
+      </c>
+      <c r="K4" s="36" t="s">
         <v>276</v>
       </c>
-      <c r="F4" s="36" t="s">
+      <c r="L4" s="36" t="s">
         <v>277</v>
-      </c>
-      <c r="G4" s="36" t="s">
-        <v>282</v>
-      </c>
-      <c r="H4" s="36" t="s">
-        <v>278</v>
-      </c>
-      <c r="I4" s="36" t="s">
-        <v>279</v>
-      </c>
-      <c r="J4" s="36" t="s">
-        <v>282</v>
-      </c>
-      <c r="K4" s="36" t="s">
-        <v>280</v>
-      </c>
-      <c r="L4" s="36" t="s">
-        <v>281</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
@@ -8506,7 +8441,7 @@
   <dimension ref="A1:G59"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F25" sqref="F25"/>
+      <selection activeCell="I18" sqref="I18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8538,11 +8473,11 @@
       <c r="G4" s="1"/>
     </row>
     <row r="5" spans="1:7" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="46" t="s">
-        <v>152</v>
+      <c r="A5" s="47" t="s">
+        <v>151</v>
       </c>
       <c r="B5" s="12" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="C5" t="s">
         <v>45</v>
@@ -8552,7 +8487,7 @@
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="46"/>
+      <c r="A6" s="47"/>
       <c r="B6" s="12" t="s">
         <v>97</v>
       </c>
@@ -8564,7 +8499,7 @@
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="46"/>
+      <c r="A7" s="47"/>
       <c r="B7" s="12" t="s">
         <v>106</v>
       </c>
@@ -8576,7 +8511,7 @@
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="46"/>
+      <c r="A8" s="47"/>
       <c r="B8" s="12" t="s">
         <v>98</v>
       </c>
@@ -8584,11 +8519,11 @@
         <v>48</v>
       </c>
       <c r="D8">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="46"/>
+      <c r="A9" s="47"/>
       <c r="B9" s="12" t="s">
         <v>99</v>
       </c>
@@ -8596,11 +8531,11 @@
         <v>47</v>
       </c>
       <c r="D9">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A10" s="46"/>
+      <c r="A10" s="47"/>
       <c r="B10" s="12" t="s">
         <v>107</v>
       </c>
@@ -8612,7 +8547,7 @@
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="46"/>
+      <c r="A11" s="47"/>
       <c r="B11" s="12" t="s">
         <v>100</v>
       </c>
@@ -8624,7 +8559,7 @@
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="46"/>
+      <c r="A12" s="47"/>
       <c r="B12" s="12" t="s">
         <v>101</v>
       </c>
@@ -8636,7 +8571,7 @@
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" s="46"/>
+      <c r="A13" s="47"/>
       <c r="B13" s="12" t="s">
         <v>102</v>
       </c>
@@ -8648,7 +8583,7 @@
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" s="46"/>
+      <c r="A14" s="47"/>
       <c r="B14" s="12" t="s">
         <v>103</v>
       </c>
@@ -8660,8 +8595,8 @@
       </c>
     </row>
     <row r="15" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A15" s="46" t="s">
-        <v>153</v>
+      <c r="A15" s="47" t="s">
+        <v>152</v>
       </c>
       <c r="B15" s="12" t="s">
         <v>105</v>
@@ -8674,7 +8609,7 @@
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" s="46"/>
+      <c r="A16" s="47"/>
       <c r="B16" s="12" t="s">
         <v>108</v>
       </c>
@@ -8686,7 +8621,7 @@
       </c>
     </row>
     <row r="17" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A17" s="46"/>
+      <c r="A17" s="47"/>
       <c r="B17" s="12" t="s">
         <v>109</v>
       </c>
@@ -8698,21 +8633,21 @@
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="46"/>
+      <c r="A18" s="47"/>
       <c r="B18" s="16" t="s">
+        <v>294</v>
+      </c>
+      <c r="C18" s="19" t="s">
+        <v>159</v>
+      </c>
+      <c r="D18" s="18" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="47"/>
+      <c r="B19" s="12" t="s">
         <v>110</v>
-      </c>
-      <c r="C18" s="19" t="s">
-        <v>160</v>
-      </c>
-      <c r="D18" s="18" t="s">
-        <v>223</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="46"/>
-      <c r="B19" s="12" t="s">
-        <v>111</v>
       </c>
       <c r="C19" t="s">
         <v>57</v>
@@ -8722,11 +8657,11 @@
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="46" t="s">
-        <v>154</v>
+      <c r="A20" s="47" t="s">
+        <v>153</v>
       </c>
       <c r="B20" s="12" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C20" t="s">
         <v>58</v>
@@ -8736,9 +8671,9 @@
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="46"/>
+      <c r="A21" s="47"/>
       <c r="B21" s="12" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C21" t="s">
         <v>59</v>
@@ -8748,9 +8683,9 @@
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="46"/>
+      <c r="A22" s="47"/>
       <c r="B22" s="12" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C22" t="s">
         <v>60</v>
@@ -8760,9 +8695,9 @@
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" s="46"/>
+      <c r="A23" s="47"/>
       <c r="B23" s="12" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C23" t="s">
         <v>61</v>
@@ -8772,9 +8707,9 @@
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" s="46"/>
+      <c r="A24" s="47"/>
       <c r="B24" s="12" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C24" t="s">
         <v>62</v>
@@ -8784,9 +8719,9 @@
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" s="46"/>
+      <c r="A25" s="47"/>
       <c r="B25" s="12" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C25" t="s">
         <v>63</v>
@@ -8796,9 +8731,9 @@
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26" s="46"/>
+      <c r="A26" s="47"/>
       <c r="B26" s="12" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C26" t="s">
         <v>64</v>
@@ -8808,9 +8743,9 @@
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27" s="46"/>
+      <c r="A27" s="47"/>
       <c r="B27" s="12" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C27" t="s">
         <v>65</v>
@@ -8820,9 +8755,9 @@
       </c>
     </row>
     <row r="28" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A28" s="46"/>
+      <c r="A28" s="47"/>
       <c r="B28" s="12" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C28" t="s">
         <v>66</v>
@@ -8832,9 +8767,9 @@
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A29" s="46"/>
+      <c r="A29" s="47"/>
       <c r="B29" s="12" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C29" t="s">
         <v>67</v>
@@ -8844,9 +8779,9 @@
       </c>
     </row>
     <row r="30" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A30" s="46"/>
+      <c r="A30" s="47"/>
       <c r="B30" s="12" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C30" t="s">
         <v>68</v>
@@ -8856,11 +8791,11 @@
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31" s="46" t="s">
-        <v>155</v>
+      <c r="A31" s="47" t="s">
+        <v>154</v>
       </c>
       <c r="B31" s="12" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C31" t="s">
         <v>69</v>
@@ -8870,9 +8805,9 @@
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A32" s="46"/>
+      <c r="A32" s="47"/>
       <c r="B32" s="12" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C32" t="s">
         <v>70</v>
@@ -8882,9 +8817,9 @@
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A33" s="46"/>
+      <c r="A33" s="47"/>
       <c r="B33" s="12" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C33" t="s">
         <v>71</v>
@@ -8894,9 +8829,9 @@
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A34" s="46"/>
+      <c r="A34" s="47"/>
       <c r="B34" s="12" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C34" t="s">
         <v>72</v>
@@ -8906,9 +8841,9 @@
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A35" s="46"/>
+      <c r="A35" s="47"/>
       <c r="B35" s="12" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C35" t="s">
         <v>73</v>
@@ -8918,9 +8853,9 @@
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A36" s="46"/>
+      <c r="A36" s="47"/>
       <c r="B36" s="12" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C36" t="s">
         <v>74</v>
@@ -8930,9 +8865,9 @@
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A37" s="46"/>
+      <c r="A37" s="47"/>
       <c r="B37" s="12" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C37" t="s">
         <v>75</v>
@@ -8942,9 +8877,9 @@
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A38" s="46"/>
+      <c r="A38" s="47"/>
       <c r="B38" s="12" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C38" t="s">
         <v>76</v>
@@ -8954,11 +8889,11 @@
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A39" s="46" t="s">
-        <v>156</v>
+      <c r="A39" s="47" t="s">
+        <v>155</v>
       </c>
       <c r="B39" s="12" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C39" t="s">
         <v>77</v>
@@ -8968,9 +8903,9 @@
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A40" s="46"/>
+      <c r="A40" s="47"/>
       <c r="B40" s="12" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C40" t="s">
         <v>78</v>
@@ -8980,9 +8915,9 @@
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A41" s="46"/>
+      <c r="A41" s="47"/>
       <c r="B41" s="12" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C41" t="s">
         <v>79</v>
@@ -8992,9 +8927,9 @@
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A42" s="46"/>
+      <c r="A42" s="47"/>
       <c r="B42" s="12" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C42" t="s">
         <v>80</v>
@@ -9004,9 +8939,9 @@
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A43" s="46"/>
+      <c r="A43" s="47"/>
       <c r="B43" s="12" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C43" t="s">
         <v>81</v>
@@ -9016,9 +8951,9 @@
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A44" s="46"/>
+      <c r="A44" s="47"/>
       <c r="B44" s="12" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C44" t="s">
         <v>82</v>
@@ -9028,9 +8963,9 @@
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A45" s="46"/>
+      <c r="A45" s="47"/>
       <c r="B45" s="12" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C45" t="s">
         <v>83</v>
@@ -9040,21 +8975,21 @@
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A46" s="46"/>
+      <c r="A46" s="47"/>
       <c r="B46" s="16" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C46" s="19" t="s">
         <v>84</v>
       </c>
       <c r="D46" s="18" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A47" s="46"/>
+      <c r="A47" s="47"/>
       <c r="B47" s="12" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C47" t="s">
         <v>85</v>
@@ -9064,23 +8999,23 @@
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A48" s="46"/>
+      <c r="A48" s="47"/>
       <c r="B48" s="16" t="s">
+        <v>139</v>
+      </c>
+      <c r="C48" s="19" t="s">
+        <v>160</v>
+      </c>
+      <c r="D48" s="18" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A49" s="47" t="s">
+        <v>156</v>
+      </c>
+      <c r="B49" s="12" t="s">
         <v>140</v>
-      </c>
-      <c r="C48" s="19" t="s">
-        <v>161</v>
-      </c>
-      <c r="D48" s="18" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A49" s="46" t="s">
-        <v>157</v>
-      </c>
-      <c r="B49" s="12" t="s">
-        <v>141</v>
       </c>
       <c r="C49" t="s">
         <v>86</v>
@@ -9090,9 +9025,9 @@
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A50" s="46"/>
+      <c r="A50" s="47"/>
       <c r="B50" s="12" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C50" t="s">
         <v>87</v>
@@ -9102,9 +9037,9 @@
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A51" s="46"/>
+      <c r="A51" s="47"/>
       <c r="B51" s="12" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C51" t="s">
         <v>88</v>
@@ -9114,11 +9049,11 @@
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A52" s="46" t="s">
-        <v>158</v>
+      <c r="A52" s="47" t="s">
+        <v>157</v>
       </c>
       <c r="B52" s="12" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C52" t="s">
         <v>89</v>
@@ -9128,9 +9063,9 @@
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A53" s="46"/>
+      <c r="A53" s="47"/>
       <c r="B53" s="12" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C53" t="s">
         <v>90</v>
@@ -9140,9 +9075,9 @@
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A54" s="46"/>
+      <c r="A54" s="47"/>
       <c r="B54" s="12" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C54" t="s">
         <v>91</v>
@@ -9152,9 +9087,9 @@
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A55" s="46"/>
+      <c r="A55" s="47"/>
       <c r="B55" s="12" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C55" t="s">
         <v>92</v>
@@ -9164,9 +9099,9 @@
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A56" s="46"/>
+      <c r="A56" s="47"/>
       <c r="B56" s="12" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C56" t="s">
         <v>93</v>
@@ -9176,9 +9111,9 @@
       </c>
     </row>
     <row r="57" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A57" s="46"/>
+      <c r="A57" s="47"/>
       <c r="B57" s="12" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C57" t="s">
         <v>94</v>
@@ -9188,11 +9123,11 @@
       </c>
     </row>
     <row r="58" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A58" s="46" t="s">
-        <v>159</v>
+      <c r="A58" s="47" t="s">
+        <v>158</v>
       </c>
       <c r="B58" s="12" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C58" t="s">
         <v>95</v>
@@ -9202,9 +9137,9 @@
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A59" s="46"/>
+      <c r="A59" s="47"/>
       <c r="B59" s="12" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C59" t="s">
         <v>96</v>
@@ -9243,7 +9178,7 @@
   <dimension ref="A1:D20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9266,99 +9201,99 @@
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="46" t="s">
-        <v>162</v>
+      <c r="A5" s="47" t="s">
+        <v>161</v>
       </c>
       <c r="B5" s="12" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="C5" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="D5" s="14">
         <v>50</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="46"/>
+      <c r="A6" s="47"/>
       <c r="B6" s="12" t="s">
+        <v>198</v>
+      </c>
+      <c r="C6" t="s">
+        <v>164</v>
+      </c>
+      <c r="D6" s="14">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A7" s="47"/>
+      <c r="B7" s="12" t="s">
         <v>199</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C7" t="s">
         <v>165</v>
-      </c>
-      <c r="D6" s="14">
-        <v>1025</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A7" s="46"/>
-      <c r="B7" s="12" t="s">
-        <v>200</v>
-      </c>
-      <c r="C7" t="s">
-        <v>166</v>
       </c>
       <c r="D7">
         <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A8" s="46"/>
+      <c r="A8" s="47"/>
       <c r="B8" s="12" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C8" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="D8" s="14">
         <v>50</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="46"/>
+      <c r="A9" s="47"/>
       <c r="B9" s="12" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C9" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="D9">
         <f>D6</f>
-        <v>1025</v>
+        <v>500</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="46"/>
+      <c r="A10" s="47"/>
       <c r="B10" s="12" t="s">
+        <v>202</v>
+      </c>
+      <c r="C10" t="s">
+        <v>168</v>
+      </c>
+      <c r="D10">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="47"/>
+      <c r="B11" s="12" t="s">
         <v>203</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C11" t="s">
         <v>169</v>
-      </c>
-      <c r="D10">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="46"/>
-      <c r="B11" s="12" t="s">
-        <v>204</v>
-      </c>
-      <c r="C11" t="s">
-        <v>170</v>
       </c>
       <c r="D11">
         <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="46"/>
+      <c r="A12" s="47"/>
       <c r="B12" s="12" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="C12" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="D12">
         <f>D5</f>
@@ -9366,100 +9301,100 @@
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="46"/>
+      <c r="A13" s="47"/>
       <c r="B13" s="12" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="C13" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="D13">
         <f>D6</f>
-        <v>1025</v>
+        <v>500</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="46"/>
+      <c r="A14" s="47"/>
       <c r="B14" s="12" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="C14" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="D14">
         <f>D6/D5</f>
-        <v>20.5</v>
+        <v>10</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="46"/>
+      <c r="A15" s="47"/>
       <c r="B15" s="16" t="s">
+        <v>206</v>
+      </c>
+      <c r="C15" s="17" t="s">
+        <v>173</v>
+      </c>
+      <c r="D15" s="18" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="47"/>
+      <c r="B16" s="16" t="s">
         <v>207</v>
       </c>
-      <c r="C15" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="D15" s="18" t="s">
+      <c r="C16" s="17" t="s">
+        <v>179</v>
+      </c>
+      <c r="D16" s="18" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A17" s="47" t="s">
+        <v>162</v>
+      </c>
+      <c r="B17" s="12" t="s">
+        <v>208</v>
+      </c>
+      <c r="C17" t="s">
         <v>175</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="46"/>
-      <c r="B16" s="16" t="s">
-        <v>208</v>
-      </c>
-      <c r="C16" s="17" t="s">
-        <v>180</v>
-      </c>
-      <c r="D16" s="18" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A17" s="46" t="s">
-        <v>163</v>
-      </c>
-      <c r="B17" s="12" t="s">
-        <v>209</v>
-      </c>
-      <c r="C17" t="s">
-        <v>176</v>
       </c>
       <c r="D17">
         <v>0.01</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="46"/>
+      <c r="A18" s="47"/>
       <c r="B18" s="12" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="C18" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="D18">
         <v>5.0000000000000001E-3</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="46"/>
+      <c r="A19" s="47"/>
       <c r="B19" s="12" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C19" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D19">
         <v>10</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A20" s="46"/>
+      <c r="A20" s="47"/>
       <c r="B20" s="12" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C20" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="D20">
         <v>0</v>
@@ -9499,89 +9434,89 @@
   <sheetData>
     <row r="1" spans="1:4" ht="21" x14ac:dyDescent="0.35">
       <c r="A1" s="7" t="s">
-        <v>308</v>
+        <v>288</v>
       </c>
       <c r="B1" s="7"/>
     </row>
     <row r="5" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A5" s="46"/>
+      <c r="A5" s="47"/>
       <c r="B5" s="12" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="C5" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="D5">
         <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A6" s="46"/>
+      <c r="A6" s="47"/>
       <c r="B6" s="12" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="C6" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="D6" s="14">
         <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="46"/>
+      <c r="A7" s="47"/>
       <c r="B7" s="12" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="C7" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="D7">
         <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="46"/>
+      <c r="A8" s="47"/>
       <c r="B8" s="12" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="C8" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="D8">
         <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="46"/>
+      <c r="A9" s="47"/>
       <c r="B9" s="12" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="C9" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="D9" s="24">
         <v>50</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="46"/>
+      <c r="A10" s="47"/>
       <c r="B10" s="12" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="C10" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="D10" s="14">
         <v>150</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="46"/>
+      <c r="A11" s="47"/>
       <c r="B11" s="12" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="C11" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="D11">
         <f>D10/D9</f>
@@ -9589,100 +9524,100 @@
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="46"/>
+      <c r="A12" s="47"/>
       <c r="B12" s="16" t="s">
+        <v>206</v>
+      </c>
+      <c r="C12" s="19" t="s">
+        <v>187</v>
+      </c>
+      <c r="D12" s="18" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="47"/>
+      <c r="B13" s="16" t="s">
         <v>207</v>
       </c>
-      <c r="C12" s="19" t="s">
+      <c r="C13" s="19" t="s">
         <v>188</v>
       </c>
-      <c r="D12" s="18" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="46"/>
-      <c r="B13" s="16" t="s">
-        <v>208</v>
-      </c>
-      <c r="C13" s="19" t="s">
-        <v>189</v>
-      </c>
       <c r="D13" s="18" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A14" s="15" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B14" s="12" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C14" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="D14">
         <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A15" s="46" t="s">
-        <v>196</v>
+      <c r="A15" s="47" t="s">
+        <v>195</v>
       </c>
       <c r="B15" s="12" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C15" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="D15">
         <v>0</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A16" s="46"/>
+      <c r="A16" s="47"/>
       <c r="B16" s="12" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="C16" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="D16">
         <v>3</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="46"/>
+      <c r="A17" s="47"/>
       <c r="B17" s="12" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="C17" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="D17">
         <v>0</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A18" s="46"/>
+      <c r="A18" s="47"/>
       <c r="B18" s="12" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C18" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="D18">
         <v>0</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A19" s="46"/>
+      <c r="A19" s="47"/>
       <c r="B19" s="12" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="C19" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="D19">
         <v>1.6</v>
@@ -9855,15 +9790,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
   <documentManagement>
     <iab7cdb7554d4997ae876b11632fa575 xmlns="3cada6dc-2705-46ed-bab2-0b2cd6d935ca">
@@ -9872,6 +9798,15 @@
     <TaxCatchAll xmlns="3cada6dc-2705-46ed-bab2-0b2cd6d935ca"/>
   </documentManagement>
 </p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -9893,14 +9828,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7B5D7682-109C-47ED-9D9D-D061E76CCAD3}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FCC61AA8-C35E-4598-8617-08B80F018AC2}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
@@ -9914,4 +9841,12 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7B5D7682-109C-47ED-9D9D-D061E76CCAD3}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Added input to HAST for Phase Shifting Transformers with backwards compatibility by checking the number of entries in the load flow settings.
</commit_message>
<xml_diff>
--- a/HAST_Inputs.xlsx
+++ b/HAST_Inputs.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21328"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65E45D54-9CB5-46F8-B382-FCFF1BCD4C4E}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6D53376-F01B-4A08-B8C6-F015343378EE}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="868" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="868" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cover Sheet" sheetId="10" r:id="rId1"/>
@@ -424,7 +424,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="344" uniqueCount="297">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="346" uniqueCount="299">
   <si>
     <t>Name</t>
   </si>
@@ -1368,6 +1368,12 @@
   </si>
   <si>
     <t>Dunstown</t>
+  </si>
+  <si>
+    <t>Automatic Tap Adjustment of Phase Shifters</t>
+  </si>
+  <si>
+    <t>ldf.iPST_at</t>
   </si>
 </sst>
 </file>
@@ -6306,7 +6312,7 @@
   <sheetPr codeName="Sheet5"/>
   <dimension ref="A1:D103"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
@@ -8438,10 +8444,10 @@
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <sheetPr codeName="Sheet6"/>
-  <dimension ref="A1:G59"/>
+  <dimension ref="A1:G60"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I18" sqref="I18"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8513,58 +8519,58 @@
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="47"/>
       <c r="B8" s="12" t="s">
-        <v>98</v>
+        <v>297</v>
       </c>
       <c r="C8" t="s">
-        <v>48</v>
+        <v>298</v>
       </c>
       <c r="D8">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="47"/>
       <c r="B9" s="12" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C9" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="D9">
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="47"/>
       <c r="B10" s="12" t="s">
-        <v>107</v>
+        <v>99</v>
       </c>
       <c r="C10" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D10">
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="47"/>
       <c r="B11" s="12" t="s">
-        <v>100</v>
+        <v>107</v>
       </c>
       <c r="C11" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D11">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="47"/>
       <c r="B12" s="12" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C12" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D12">
         <v>1</v>
@@ -8573,110 +8579,110 @@
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="47"/>
       <c r="B13" s="12" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C13" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D13">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="47"/>
       <c r="B14" s="12" t="s">
+        <v>102</v>
+      </c>
+      <c r="C14" t="s">
+        <v>52</v>
+      </c>
+      <c r="D14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" s="47"/>
+      <c r="B15" s="12" t="s">
         <v>103</v>
       </c>
-      <c r="C14" t="s">
+      <c r="C15" t="s">
         <v>53</v>
       </c>
-      <c r="D14">
+      <c r="D15">
         <v>100</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A15" s="47" t="s">
+    <row r="16" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A16" s="47" t="s">
         <v>152</v>
       </c>
-      <c r="B15" s="12" t="s">
+      <c r="B16" s="12" t="s">
         <v>105</v>
       </c>
-      <c r="C15" t="s">
+      <c r="C16" t="s">
         <v>54</v>
-      </c>
-      <c r="D15">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" s="47"/>
-      <c r="B16" s="12" t="s">
-        <v>108</v>
-      </c>
-      <c r="C16" t="s">
-        <v>55</v>
       </c>
       <c r="D16">
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="47"/>
       <c r="B17" s="12" t="s">
+        <v>108</v>
+      </c>
+      <c r="C17" t="s">
+        <v>55</v>
+      </c>
+      <c r="D17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A18" s="47"/>
+      <c r="B18" s="12" t="s">
         <v>109</v>
       </c>
-      <c r="C17" t="s">
+      <c r="C18" t="s">
         <v>56</v>
       </c>
-      <c r="D17">
+      <c r="D18">
         <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="47"/>
-      <c r="B18" s="16" t="s">
-        <v>294</v>
-      </c>
-      <c r="C18" s="19" t="s">
-        <v>159</v>
-      </c>
-      <c r="D18" s="18" t="s">
-        <v>293</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="47"/>
-      <c r="B19" s="12" t="s">
+      <c r="B19" s="16" t="s">
+        <v>294</v>
+      </c>
+      <c r="C19" s="19" t="s">
+        <v>159</v>
+      </c>
+      <c r="D19" s="18" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" s="47"/>
+      <c r="B20" s="12" t="s">
         <v>110</v>
       </c>
-      <c r="C19" t="s">
+      <c r="C20" t="s">
         <v>57</v>
-      </c>
-      <c r="D19">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="47" t="s">
-        <v>153</v>
-      </c>
-      <c r="B20" s="12" t="s">
-        <v>111</v>
-      </c>
-      <c r="C20" t="s">
-        <v>58</v>
       </c>
       <c r="D20">
         <v>0</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="47"/>
+      <c r="A21" s="47" t="s">
+        <v>153</v>
+      </c>
       <c r="B21" s="12" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C21" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D21">
         <v>0</v>
@@ -8685,10 +8691,10 @@
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="47"/>
       <c r="B22" s="12" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C22" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D22">
         <v>0</v>
@@ -8697,180 +8703,180 @@
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="47"/>
       <c r="B23" s="12" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C23" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D23">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="47"/>
       <c r="B24" s="12" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C24" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D24">
-        <v>20</v>
+        <v>1</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="47"/>
       <c r="B25" s="12" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C25" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D25">
-        <v>0</v>
+        <v>20</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="47"/>
       <c r="B26" s="12" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C26" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D26">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="47"/>
       <c r="B27" s="12" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C27" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D27">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="47"/>
       <c r="B28" s="12" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C28" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D28">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A29" s="47"/>
       <c r="B29" s="12" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C29" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D29">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="47"/>
       <c r="B30" s="12" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C30" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D30">
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31" s="47" t="s">
+    <row r="31" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A31" s="47"/>
+      <c r="B31" s="12" t="s">
+        <v>121</v>
+      </c>
+      <c r="C31" t="s">
+        <v>68</v>
+      </c>
+      <c r="D31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32" s="47" t="s">
         <v>154</v>
       </c>
-      <c r="B31" s="12" t="s">
+      <c r="B32" s="12" t="s">
         <v>122</v>
       </c>
-      <c r="C31" t="s">
+      <c r="C32" t="s">
         <v>69</v>
       </c>
-      <c r="D31">
+      <c r="D32">
         <v>100</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A32" s="47"/>
-      <c r="B32" s="12" t="s">
-        <v>123</v>
-      </c>
-      <c r="C32" t="s">
-        <v>70</v>
-      </c>
-      <c r="D32">
-        <v>80</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="47"/>
       <c r="B33" s="12" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C33" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D33">
-        <v>5</v>
+        <v>80</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" s="47"/>
       <c r="B34" s="12" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C34" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D34">
-        <v>10000</v>
+        <v>5</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" s="47"/>
       <c r="B35" s="12" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C35" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D35">
-        <v>10</v>
+        <v>10000</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" s="47"/>
       <c r="B36" s="12" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C36" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D36">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" s="47"/>
       <c r="B37" s="12" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C37" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D37">
         <v>1</v>
@@ -8879,158 +8885,158 @@
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" s="47"/>
       <c r="B38" s="12" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C38" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D38">
         <v>1</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A39" s="47" t="s">
+      <c r="A39" s="47"/>
+      <c r="B39" s="12" t="s">
+        <v>129</v>
+      </c>
+      <c r="C39" t="s">
+        <v>76</v>
+      </c>
+      <c r="D39">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A40" s="47" t="s">
         <v>155</v>
       </c>
-      <c r="B39" s="12" t="s">
+      <c r="B40" s="12" t="s">
         <v>130</v>
       </c>
-      <c r="C39" t="s">
+      <c r="C40" t="s">
         <v>77</v>
       </c>
-      <c r="D39">
+      <c r="D40">
         <v>0</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A40" s="47"/>
-      <c r="B40" s="12" t="s">
-        <v>131</v>
-      </c>
-      <c r="C40" t="s">
-        <v>78</v>
-      </c>
-      <c r="D40">
-        <v>1</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" s="47"/>
       <c r="B41" s="12" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C41" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D41">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" s="47"/>
       <c r="B42" s="12" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C42" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D42">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" s="47"/>
       <c r="B43" s="12" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C43" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D43">
-        <v>110</v>
+        <v>1</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" s="47"/>
       <c r="B44" s="12" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C44" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D44">
-        <v>0.9</v>
+        <v>110</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" s="47"/>
       <c r="B45" s="12" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C45" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D45">
-        <v>1.1200000000000001</v>
+        <v>0.9</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" s="47"/>
-      <c r="B46" s="16" t="s">
-        <v>137</v>
-      </c>
-      <c r="C46" s="19" t="s">
-        <v>84</v>
-      </c>
-      <c r="D46" s="18" t="s">
-        <v>221</v>
+      <c r="B46" s="12" t="s">
+        <v>136</v>
+      </c>
+      <c r="C46" t="s">
+        <v>83</v>
+      </c>
+      <c r="D46">
+        <v>1.1200000000000001</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" s="47"/>
-      <c r="B47" s="12" t="s">
-        <v>138</v>
-      </c>
-      <c r="C47" t="s">
-        <v>85</v>
-      </c>
-      <c r="D47">
-        <v>1</v>
+      <c r="B47" s="16" t="s">
+        <v>137</v>
+      </c>
+      <c r="C47" s="19" t="s">
+        <v>84</v>
+      </c>
+      <c r="D47" s="18" t="s">
+        <v>221</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" s="47"/>
-      <c r="B48" s="16" t="s">
+      <c r="B48" s="12" t="s">
+        <v>138</v>
+      </c>
+      <c r="C48" t="s">
+        <v>85</v>
+      </c>
+      <c r="D48">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A49" s="47"/>
+      <c r="B49" s="16" t="s">
         <v>139</v>
       </c>
-      <c r="C48" s="19" t="s">
+      <c r="C49" s="19" t="s">
         <v>160</v>
       </c>
-      <c r="D48" s="18" t="s">
+      <c r="D49" s="18" t="s">
         <v>220</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A49" s="47" t="s">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A50" s="47" t="s">
         <v>156</v>
       </c>
-      <c r="B49" s="12" t="s">
+      <c r="B50" s="12" t="s">
         <v>140</v>
       </c>
-      <c r="C49" t="s">
+      <c r="C50" t="s">
         <v>86</v>
-      </c>
-      <c r="D49">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A50" s="47"/>
-      <c r="B50" s="12" t="s">
-        <v>141</v>
-      </c>
-      <c r="C50" t="s">
-        <v>87</v>
       </c>
       <c r="D50">
         <v>100</v>
@@ -9039,131 +9045,143 @@
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" s="47"/>
       <c r="B51" s="12" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C51" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D51">
         <v>100</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A52" s="47" t="s">
+      <c r="A52" s="47"/>
+      <c r="B52" s="12" t="s">
+        <v>142</v>
+      </c>
+      <c r="C52" t="s">
+        <v>88</v>
+      </c>
+      <c r="D52">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A53" s="47" t="s">
         <v>157</v>
       </c>
-      <c r="B52" s="12" t="s">
+      <c r="B53" s="12" t="s">
         <v>143</v>
       </c>
-      <c r="C52" t="s">
+      <c r="C53" t="s">
         <v>89</v>
       </c>
-      <c r="D52">
+      <c r="D53">
         <v>0</v>
-      </c>
-    </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A53" s="47"/>
-      <c r="B53" s="12" t="s">
-        <v>144</v>
-      </c>
-      <c r="C53" t="s">
-        <v>90</v>
-      </c>
-      <c r="D53">
-        <v>0.9</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" s="47"/>
       <c r="B54" s="12" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C54" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D54">
-        <v>12</v>
+        <v>0.9</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" s="47"/>
       <c r="B55" s="12" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C55" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D55">
-        <v>0.95</v>
+        <v>12</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" s="47"/>
       <c r="B56" s="12" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C56" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D56">
-        <v>0.1</v>
-      </c>
-    </row>
-    <row r="57" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+        <v>0.95</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" s="47"/>
       <c r="B57" s="12" t="s">
+        <v>147</v>
+      </c>
+      <c r="C57" t="s">
+        <v>93</v>
+      </c>
+      <c r="D57">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A58" s="47"/>
+      <c r="B58" s="12" t="s">
         <v>148</v>
       </c>
-      <c r="C57" t="s">
+      <c r="C58" t="s">
         <v>94</v>
-      </c>
-      <c r="D57">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="58" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A58" s="47" t="s">
-        <v>158</v>
-      </c>
-      <c r="B58" s="12" t="s">
-        <v>149</v>
-      </c>
-      <c r="C58" t="s">
-        <v>95</v>
       </c>
       <c r="D58">
         <v>1</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A59" s="47"/>
+    <row r="59" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A59" s="47" t="s">
+        <v>158</v>
+      </c>
       <c r="B59" s="12" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C59" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D59">
         <v>1</v>
       </c>
     </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A60" s="47"/>
+      <c r="B60" s="12" t="s">
+        <v>150</v>
+      </c>
+      <c r="C60" t="s">
+        <v>96</v>
+      </c>
+      <c r="D60">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="8">
-    <mergeCell ref="A52:A57"/>
-    <mergeCell ref="A58:A59"/>
-    <mergeCell ref="A5:A14"/>
-    <mergeCell ref="A15:A19"/>
-    <mergeCell ref="A20:A30"/>
-    <mergeCell ref="A31:A38"/>
-    <mergeCell ref="A39:A48"/>
-    <mergeCell ref="A49:A51"/>
+    <mergeCell ref="A53:A58"/>
+    <mergeCell ref="A59:A60"/>
+    <mergeCell ref="A5:A15"/>
+    <mergeCell ref="A16:A20"/>
+    <mergeCell ref="A21:A31"/>
+    <mergeCell ref="A32:A39"/>
+    <mergeCell ref="A40:A49"/>
+    <mergeCell ref="A50:A52"/>
   </mergeCells>
   <dataValidations count="2">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D5" xr:uid="{00000000-0002-0000-0500-000000000000}">
       <formula1>"0,1,2"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D6:D13 D16 D57:D59 D47 D42 D38:D40 D36 D29:D30 D25 D20:D23" xr:uid="{00000000-0002-0000-0500-000001000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D6:D14 D17 D58:D60 D48 D43 D39:D41 D37 D30:D31 D26 D21:D24" xr:uid="{00000000-0002-0000-0500-000001000000}">
       <formula1>"0,1"</formula1>
     </dataValidation>
   </dataValidations>
@@ -9790,6 +9808,15 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
   <documentManagement>
     <iab7cdb7554d4997ae876b11632fa575 xmlns="3cada6dc-2705-46ed-bab2-0b2cd6d935ca">
@@ -9798,15 +9825,6 @@
     <TaxCatchAll xmlns="3cada6dc-2705-46ed-bab2-0b2cd6d935ca"/>
   </documentManagement>
 </p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -9828,6 +9846,14 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7B5D7682-109C-47ED-9D9D-D061E76CCAD3}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FCC61AA8-C35E-4598-8617-08B80F018AC2}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
@@ -9841,12 +9867,4 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7B5D7682-109C-47ED-9D9D-D061E76CCAD3}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Version 2.1.3 - Updated Load Flow Settings so now the default load flow in PowerFactory can be used.
</commit_message>
<xml_diff>
--- a/HAST_Inputs.xlsx
+++ b/HAST_Inputs.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21328"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6D53376-F01B-4A08-B8C6-F015343378EE}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FBEF17A-7A0F-4B16-900F-BE6B392B1755}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="868" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -423,8 +423,42 @@
 </comments>
 </file>
 
+<file path=xl/comments5.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Author</author>
+  </authors>
+  <commentList>
+    <comment ref="D4" authorId="0" shapeId="0" xr:uid="{9F1654DB-B47D-4018-9D12-CF3B3E844655}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Author:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Either enter the name of the Load Flow command in the study case (typically "Load Flow Calculation.ComLdf") to use or set to False and populate the settings below.</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="346" uniqueCount="299">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="350" uniqueCount="303">
   <si>
     <t>Name</t>
   </si>
@@ -1375,12 +1409,24 @@
   <si>
     <t>ldf.iPST_at</t>
   </si>
+  <si>
+    <t>Study Case Load Flow Settings</t>
+  </si>
+  <si>
+    <t>.ComLdf</t>
+  </si>
+  <si>
+    <t>Load Flow Calculation</t>
+  </si>
+  <si>
+    <t>Name of load flow settings to be used for studycase (leave empty to use settings below)</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="13" x14ac:knownFonts="1">
+  <fonts count="15" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1473,6 +1519,19 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="4">
@@ -1663,7 +1722,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="48">
+  <cellXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1730,6 +1789,9 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1760,7 +1822,51 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
   </cellStyles>
-  <dxfs count="2">
+  <dxfs count="10">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0" tint="-0.499984740745262"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0" tint="-0.499984740745262"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0" tint="-0.499984740745262"/>
+      </font>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0" tint="-0.499984740745262"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0" tint="-0.499984740745262"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0" tint="-0.499984740745262"/>
+      </font>
+    </dxf>
     <dxf>
       <font>
         <color theme="6"/>
@@ -2265,11 +2371,11 @@
       <c r="A2" s="7"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="D3" s="40" t="s">
+      <c r="D3" s="41" t="s">
         <v>224</v>
       </c>
-      <c r="E3" s="40"/>
-      <c r="F3" s="40"/>
+      <c r="E3" s="41"/>
+      <c r="F3" s="41"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D4" t="s">
@@ -2708,51 +2814,51 @@
     </row>
     <row r="2" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="3" spans="1:28" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="44" t="s">
+      <c r="B3" s="45" t="s">
         <v>10</v>
       </c>
-      <c r="C3" s="45"/>
-      <c r="D3" s="46"/>
-      <c r="E3" s="41" t="s">
+      <c r="C3" s="46"/>
+      <c r="D3" s="47"/>
+      <c r="E3" s="42" t="s">
         <v>11</v>
       </c>
-      <c r="F3" s="42"/>
-      <c r="G3" s="43"/>
-      <c r="H3" s="41" t="s">
+      <c r="F3" s="43"/>
+      <c r="G3" s="44"/>
+      <c r="H3" s="42" t="s">
         <v>12</v>
       </c>
-      <c r="I3" s="42"/>
-      <c r="J3" s="43"/>
-      <c r="K3" s="41" t="s">
+      <c r="I3" s="43"/>
+      <c r="J3" s="44"/>
+      <c r="K3" s="42" t="s">
         <v>13</v>
       </c>
-      <c r="L3" s="42"/>
-      <c r="M3" s="43"/>
-      <c r="N3" s="41" t="s">
+      <c r="L3" s="43"/>
+      <c r="M3" s="44"/>
+      <c r="N3" s="42" t="s">
         <v>14</v>
       </c>
-      <c r="O3" s="42"/>
-      <c r="P3" s="43"/>
-      <c r="Q3" s="41" t="s">
+      <c r="O3" s="43"/>
+      <c r="P3" s="44"/>
+      <c r="Q3" s="42" t="s">
         <v>15</v>
       </c>
-      <c r="R3" s="42"/>
-      <c r="S3" s="43"/>
-      <c r="T3" s="41" t="s">
+      <c r="R3" s="43"/>
+      <c r="S3" s="44"/>
+      <c r="T3" s="42" t="s">
         <v>16</v>
       </c>
-      <c r="U3" s="42"/>
-      <c r="V3" s="43"/>
-      <c r="W3" s="41" t="s">
+      <c r="U3" s="43"/>
+      <c r="V3" s="44"/>
+      <c r="W3" s="42" t="s">
         <v>17</v>
       </c>
-      <c r="X3" s="42"/>
-      <c r="Y3" s="43"/>
-      <c r="Z3" s="41" t="s">
+      <c r="X3" s="43"/>
+      <c r="Y3" s="44"/>
+      <c r="Z3" s="42" t="s">
         <v>18</v>
       </c>
-      <c r="AA3" s="42"/>
-      <c r="AB3" s="43"/>
+      <c r="AA3" s="43"/>
+      <c r="AB3" s="44"/>
     </row>
     <row r="4" spans="1:28" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="6" t="s">
@@ -6964,12 +7070,12 @@
     <sortCondition ref="A5:A8"/>
   </sortState>
   <conditionalFormatting sqref="A5:A103">
-    <cfRule type="expression" dxfId="1" priority="3">
+    <cfRule type="expression" dxfId="9" priority="3">
       <formula>LEN(A5)&gt;19</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A3">
-    <cfRule type="expression" dxfId="0" priority="1">
+    <cfRule type="expression" dxfId="8" priority="1">
       <formula>A3="NAMES OKAY"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -8442,12 +8548,12 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <sheetPr codeName="Sheet6"/>
   <dimension ref="A1:G60"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8455,7 +8561,7 @@
     <col min="1" max="1" width="20" customWidth="1"/>
     <col min="2" max="2" width="55.5703125" style="12" customWidth="1"/>
     <col min="3" max="3" width="13.7109375" customWidth="1"/>
-    <col min="4" max="4" width="14.85546875" customWidth="1"/>
+    <col min="4" max="4" width="22.85546875" customWidth="1"/>
     <col min="5" max="5" width="13.140625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="17" customWidth="1"/>
     <col min="7" max="7" width="27.85546875" customWidth="1"/>
@@ -8472,14 +8578,28 @@
       </c>
       <c r="B1" s="13"/>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="D4" s="1"/>
-      <c r="E4" s="1"/>
+    <row r="4" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A4" s="40" t="s">
+        <v>299</v>
+      </c>
+      <c r="B4" s="12" t="s">
+        <v>302</v>
+      </c>
+      <c r="C4" t="s">
+        <v>300</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>301</v>
+      </c>
+      <c r="E4" s="1" t="str">
+        <f>IF($D$4="","&lt;--- Cannot be empty, please enter False","")</f>
+        <v/>
+      </c>
       <c r="F4" s="1"/>
       <c r="G4" s="1"/>
     </row>
     <row r="5" spans="1:7" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="47" t="s">
+      <c r="A5" s="48" t="s">
         <v>151</v>
       </c>
       <c r="B5" s="12" t="s">
@@ -8493,7 +8613,7 @@
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="47"/>
+      <c r="A6" s="48"/>
       <c r="B6" s="12" t="s">
         <v>97</v>
       </c>
@@ -8505,7 +8625,7 @@
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="47"/>
+      <c r="A7" s="48"/>
       <c r="B7" s="12" t="s">
         <v>106</v>
       </c>
@@ -8517,7 +8637,7 @@
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="47"/>
+      <c r="A8" s="48"/>
       <c r="B8" s="12" t="s">
         <v>297</v>
       </c>
@@ -8529,7 +8649,7 @@
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="47"/>
+      <c r="A9" s="48"/>
       <c r="B9" s="12" t="s">
         <v>98</v>
       </c>
@@ -8541,7 +8661,7 @@
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="47"/>
+      <c r="A10" s="48"/>
       <c r="B10" s="12" t="s">
         <v>99</v>
       </c>
@@ -8553,7 +8673,7 @@
       </c>
     </row>
     <row r="11" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A11" s="47"/>
+      <c r="A11" s="48"/>
       <c r="B11" s="12" t="s">
         <v>107</v>
       </c>
@@ -8565,7 +8685,7 @@
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="47"/>
+      <c r="A12" s="48"/>
       <c r="B12" s="12" t="s">
         <v>100</v>
       </c>
@@ -8577,7 +8697,7 @@
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" s="47"/>
+      <c r="A13" s="48"/>
       <c r="B13" s="12" t="s">
         <v>101</v>
       </c>
@@ -8589,7 +8709,7 @@
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" s="47"/>
+      <c r="A14" s="48"/>
       <c r="B14" s="12" t="s">
         <v>102</v>
       </c>
@@ -8601,7 +8721,7 @@
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" s="47"/>
+      <c r="A15" s="48"/>
       <c r="B15" s="12" t="s">
         <v>103</v>
       </c>
@@ -8613,7 +8733,7 @@
       </c>
     </row>
     <row r="16" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A16" s="47" t="s">
+      <c r="A16" s="48" t="s">
         <v>152</v>
       </c>
       <c r="B16" s="12" t="s">
@@ -8627,7 +8747,7 @@
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="47"/>
+      <c r="A17" s="48"/>
       <c r="B17" s="12" t="s">
         <v>108</v>
       </c>
@@ -8639,7 +8759,7 @@
       </c>
     </row>
     <row r="18" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A18" s="47"/>
+      <c r="A18" s="48"/>
       <c r="B18" s="12" t="s">
         <v>109</v>
       </c>
@@ -8651,7 +8771,7 @@
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="47"/>
+      <c r="A19" s="48"/>
       <c r="B19" s="16" t="s">
         <v>294</v>
       </c>
@@ -8663,7 +8783,7 @@
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="47"/>
+      <c r="A20" s="48"/>
       <c r="B20" s="12" t="s">
         <v>110</v>
       </c>
@@ -8675,7 +8795,7 @@
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="47" t="s">
+      <c r="A21" s="48" t="s">
         <v>153</v>
       </c>
       <c r="B21" s="12" t="s">
@@ -8689,7 +8809,7 @@
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="47"/>
+      <c r="A22" s="48"/>
       <c r="B22" s="12" t="s">
         <v>112</v>
       </c>
@@ -8701,7 +8821,7 @@
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" s="47"/>
+      <c r="A23" s="48"/>
       <c r="B23" s="12" t="s">
         <v>113</v>
       </c>
@@ -8713,7 +8833,7 @@
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" s="47"/>
+      <c r="A24" s="48"/>
       <c r="B24" s="12" t="s">
         <v>114</v>
       </c>
@@ -8725,7 +8845,7 @@
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" s="47"/>
+      <c r="A25" s="48"/>
       <c r="B25" s="12" t="s">
         <v>115</v>
       </c>
@@ -8737,7 +8857,7 @@
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26" s="47"/>
+      <c r="A26" s="48"/>
       <c r="B26" s="12" t="s">
         <v>116</v>
       </c>
@@ -8749,7 +8869,7 @@
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27" s="47"/>
+      <c r="A27" s="48"/>
       <c r="B27" s="12" t="s">
         <v>117</v>
       </c>
@@ -8761,7 +8881,7 @@
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A28" s="47"/>
+      <c r="A28" s="48"/>
       <c r="B28" s="12" t="s">
         <v>118</v>
       </c>
@@ -8773,7 +8893,7 @@
       </c>
     </row>
     <row r="29" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A29" s="47"/>
+      <c r="A29" s="48"/>
       <c r="B29" s="12" t="s">
         <v>119</v>
       </c>
@@ -8785,7 +8905,7 @@
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30" s="47"/>
+      <c r="A30" s="48"/>
       <c r="B30" s="12" t="s">
         <v>120</v>
       </c>
@@ -8797,7 +8917,7 @@
       </c>
     </row>
     <row r="31" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A31" s="47"/>
+      <c r="A31" s="48"/>
       <c r="B31" s="12" t="s">
         <v>121</v>
       </c>
@@ -8809,7 +8929,7 @@
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A32" s="47" t="s">
+      <c r="A32" s="48" t="s">
         <v>154</v>
       </c>
       <c r="B32" s="12" t="s">
@@ -8823,7 +8943,7 @@
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A33" s="47"/>
+      <c r="A33" s="48"/>
       <c r="B33" s="12" t="s">
         <v>123</v>
       </c>
@@ -8835,7 +8955,7 @@
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A34" s="47"/>
+      <c r="A34" s="48"/>
       <c r="B34" s="12" t="s">
         <v>124</v>
       </c>
@@ -8847,7 +8967,7 @@
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A35" s="47"/>
+      <c r="A35" s="48"/>
       <c r="B35" s="12" t="s">
         <v>125</v>
       </c>
@@ -8859,7 +8979,7 @@
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A36" s="47"/>
+      <c r="A36" s="48"/>
       <c r="B36" s="12" t="s">
         <v>126</v>
       </c>
@@ -8871,7 +8991,7 @@
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A37" s="47"/>
+      <c r="A37" s="48"/>
       <c r="B37" s="12" t="s">
         <v>127</v>
       </c>
@@ -8883,7 +9003,7 @@
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A38" s="47"/>
+      <c r="A38" s="48"/>
       <c r="B38" s="12" t="s">
         <v>128</v>
       </c>
@@ -8895,7 +9015,7 @@
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A39" s="47"/>
+      <c r="A39" s="48"/>
       <c r="B39" s="12" t="s">
         <v>129</v>
       </c>
@@ -8907,7 +9027,7 @@
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A40" s="47" t="s">
+      <c r="A40" s="48" t="s">
         <v>155</v>
       </c>
       <c r="B40" s="12" t="s">
@@ -8921,7 +9041,7 @@
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A41" s="47"/>
+      <c r="A41" s="48"/>
       <c r="B41" s="12" t="s">
         <v>131</v>
       </c>
@@ -8933,7 +9053,7 @@
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A42" s="47"/>
+      <c r="A42" s="48"/>
       <c r="B42" s="12" t="s">
         <v>132</v>
       </c>
@@ -8945,7 +9065,7 @@
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A43" s="47"/>
+      <c r="A43" s="48"/>
       <c r="B43" s="12" t="s">
         <v>133</v>
       </c>
@@ -8957,7 +9077,7 @@
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A44" s="47"/>
+      <c r="A44" s="48"/>
       <c r="B44" s="12" t="s">
         <v>134</v>
       </c>
@@ -8969,7 +9089,7 @@
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A45" s="47"/>
+      <c r="A45" s="48"/>
       <c r="B45" s="12" t="s">
         <v>135</v>
       </c>
@@ -8981,7 +9101,7 @@
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A46" s="47"/>
+      <c r="A46" s="48"/>
       <c r="B46" s="12" t="s">
         <v>136</v>
       </c>
@@ -8993,7 +9113,7 @@
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A47" s="47"/>
+      <c r="A47" s="48"/>
       <c r="B47" s="16" t="s">
         <v>137</v>
       </c>
@@ -9005,7 +9125,7 @@
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A48" s="47"/>
+      <c r="A48" s="48"/>
       <c r="B48" s="12" t="s">
         <v>138</v>
       </c>
@@ -9017,7 +9137,7 @@
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A49" s="47"/>
+      <c r="A49" s="48"/>
       <c r="B49" s="16" t="s">
         <v>139</v>
       </c>
@@ -9029,7 +9149,7 @@
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A50" s="47" t="s">
+      <c r="A50" s="48" t="s">
         <v>156</v>
       </c>
       <c r="B50" s="12" t="s">
@@ -9043,7 +9163,7 @@
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A51" s="47"/>
+      <c r="A51" s="48"/>
       <c r="B51" s="12" t="s">
         <v>141</v>
       </c>
@@ -9055,7 +9175,7 @@
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A52" s="47"/>
+      <c r="A52" s="48"/>
       <c r="B52" s="12" t="s">
         <v>142</v>
       </c>
@@ -9067,7 +9187,7 @@
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A53" s="47" t="s">
+      <c r="A53" s="48" t="s">
         <v>157</v>
       </c>
       <c r="B53" s="12" t="s">
@@ -9081,7 +9201,7 @@
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A54" s="47"/>
+      <c r="A54" s="48"/>
       <c r="B54" s="12" t="s">
         <v>144</v>
       </c>
@@ -9093,7 +9213,7 @@
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A55" s="47"/>
+      <c r="A55" s="48"/>
       <c r="B55" s="12" t="s">
         <v>145</v>
       </c>
@@ -9105,7 +9225,7 @@
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A56" s="47"/>
+      <c r="A56" s="48"/>
       <c r="B56" s="12" t="s">
         <v>146</v>
       </c>
@@ -9117,7 +9237,7 @@
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A57" s="47"/>
+      <c r="A57" s="48"/>
       <c r="B57" s="12" t="s">
         <v>147</v>
       </c>
@@ -9129,7 +9249,7 @@
       </c>
     </row>
     <row r="58" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A58" s="47"/>
+      <c r="A58" s="48"/>
       <c r="B58" s="12" t="s">
         <v>148</v>
       </c>
@@ -9141,7 +9261,7 @@
       </c>
     </row>
     <row r="59" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A59" s="47" t="s">
+      <c r="A59" s="48" t="s">
         <v>158</v>
       </c>
       <c r="B59" s="12" t="s">
@@ -9155,7 +9275,7 @@
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A60" s="47"/>
+      <c r="A60" s="48"/>
       <c r="B60" s="12" t="s">
         <v>150</v>
       </c>
@@ -9177,16 +9297,33 @@
     <mergeCell ref="A40:A49"/>
     <mergeCell ref="A50:A52"/>
   </mergeCells>
-  <dataValidations count="2">
+  <conditionalFormatting sqref="A5:D60">
+    <cfRule type="expression" dxfId="3" priority="3">
+      <formula>$D$4&lt;&gt;FALSE</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A4:D4">
+    <cfRule type="expression" dxfId="5" priority="2">
+      <formula>$D$4=FALSE</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D4">
+    <cfRule type="expression" dxfId="4" priority="1">
+      <formula>$D$4=""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <dataValidations count="3">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D5" xr:uid="{00000000-0002-0000-0500-000000000000}">
       <formula1>"0,1,2"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D6:D14 D17 D58:D60 D48 D43 D39:D41 D37 D30:D31 D26 D21:D24" xr:uid="{00000000-0002-0000-0500-000001000000}">
       <formula1>"0,1"</formula1>
     </dataValidation>
+    <dataValidation errorStyle="warning" showInputMessage="1" showErrorMessage="1" errorTitle="Cannot be Empty" error="Cannot be empty, please enter either False or the name of an existing Load Flow Command to use (i.e. Load Flow Calculation.ComLdf)" sqref="D4" xr:uid="{A6D47467-2239-459C-B9B4-99D08878A811}"/>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -9219,7 +9356,7 @@
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="47" t="s">
+      <c r="A5" s="48" t="s">
         <v>161</v>
       </c>
       <c r="B5" s="12" t="s">
@@ -9233,7 +9370,7 @@
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="47"/>
+      <c r="A6" s="48"/>
       <c r="B6" s="12" t="s">
         <v>198</v>
       </c>
@@ -9245,7 +9382,7 @@
       </c>
     </row>
     <row r="7" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A7" s="47"/>
+      <c r="A7" s="48"/>
       <c r="B7" s="12" t="s">
         <v>199</v>
       </c>
@@ -9257,7 +9394,7 @@
       </c>
     </row>
     <row r="8" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A8" s="47"/>
+      <c r="A8" s="48"/>
       <c r="B8" s="12" t="s">
         <v>200</v>
       </c>
@@ -9269,7 +9406,7 @@
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="47"/>
+      <c r="A9" s="48"/>
       <c r="B9" s="12" t="s">
         <v>201</v>
       </c>
@@ -9282,7 +9419,7 @@
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="47"/>
+      <c r="A10" s="48"/>
       <c r="B10" s="12" t="s">
         <v>202</v>
       </c>
@@ -9294,7 +9431,7 @@
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="47"/>
+      <c r="A11" s="48"/>
       <c r="B11" s="12" t="s">
         <v>203</v>
       </c>
@@ -9306,7 +9443,7 @@
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="47"/>
+      <c r="A12" s="48"/>
       <c r="B12" s="12" t="s">
         <v>197</v>
       </c>
@@ -9319,7 +9456,7 @@
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="47"/>
+      <c r="A13" s="48"/>
       <c r="B13" s="12" t="s">
         <v>204</v>
       </c>
@@ -9332,7 +9469,7 @@
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="47"/>
+      <c r="A14" s="48"/>
       <c r="B14" s="12" t="s">
         <v>205</v>
       </c>
@@ -9345,7 +9482,7 @@
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="47"/>
+      <c r="A15" s="48"/>
       <c r="B15" s="16" t="s">
         <v>206</v>
       </c>
@@ -9357,7 +9494,7 @@
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="47"/>
+      <c r="A16" s="48"/>
       <c r="B16" s="16" t="s">
         <v>207</v>
       </c>
@@ -9369,7 +9506,7 @@
       </c>
     </row>
     <row r="17" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A17" s="47" t="s">
+      <c r="A17" s="48" t="s">
         <v>162</v>
       </c>
       <c r="B17" s="12" t="s">
@@ -9383,7 +9520,7 @@
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="47"/>
+      <c r="A18" s="48"/>
       <c r="B18" s="12" t="s">
         <v>209</v>
       </c>
@@ -9395,7 +9532,7 @@
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="47"/>
+      <c r="A19" s="48"/>
       <c r="B19" s="12" t="s">
         <v>210</v>
       </c>
@@ -9407,7 +9544,7 @@
       </c>
     </row>
     <row r="20" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A20" s="47"/>
+      <c r="A20" s="48"/>
       <c r="B20" s="12" t="s">
         <v>211</v>
       </c>
@@ -9457,7 +9594,7 @@
       <c r="B1" s="7"/>
     </row>
     <row r="5" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A5" s="47"/>
+      <c r="A5" s="48"/>
       <c r="B5" s="12" t="s">
         <v>244</v>
       </c>
@@ -9469,7 +9606,7 @@
       </c>
     </row>
     <row r="6" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A6" s="47"/>
+      <c r="A6" s="48"/>
       <c r="B6" s="12" t="s">
         <v>212</v>
       </c>
@@ -9481,7 +9618,7 @@
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="47"/>
+      <c r="A7" s="48"/>
       <c r="B7" s="12" t="s">
         <v>213</v>
       </c>
@@ -9493,7 +9630,7 @@
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="47"/>
+      <c r="A8" s="48"/>
       <c r="B8" s="12" t="s">
         <v>214</v>
       </c>
@@ -9505,7 +9642,7 @@
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="47"/>
+      <c r="A9" s="48"/>
       <c r="B9" s="12" t="s">
         <v>197</v>
       </c>
@@ -9517,7 +9654,7 @@
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="47"/>
+      <c r="A10" s="48"/>
       <c r="B10" s="12" t="s">
         <v>204</v>
       </c>
@@ -9529,7 +9666,7 @@
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="47"/>
+      <c r="A11" s="48"/>
       <c r="B11" s="12" t="s">
         <v>205</v>
       </c>
@@ -9542,7 +9679,7 @@
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="47"/>
+      <c r="A12" s="48"/>
       <c r="B12" s="16" t="s">
         <v>206</v>
       </c>
@@ -9554,7 +9691,7 @@
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="47"/>
+      <c r="A13" s="48"/>
       <c r="B13" s="16" t="s">
         <v>207</v>
       </c>
@@ -9580,7 +9717,7 @@
       </c>
     </row>
     <row r="15" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A15" s="47" t="s">
+      <c r="A15" s="48" t="s">
         <v>195</v>
       </c>
       <c r="B15" s="12" t="s">
@@ -9594,7 +9731,7 @@
       </c>
     </row>
     <row r="16" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A16" s="47"/>
+      <c r="A16" s="48"/>
       <c r="B16" s="12" t="s">
         <v>217</v>
       </c>
@@ -9606,7 +9743,7 @@
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="47"/>
+      <c r="A17" s="48"/>
       <c r="B17" s="12" t="s">
         <v>218</v>
       </c>
@@ -9618,7 +9755,7 @@
       </c>
     </row>
     <row r="18" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A18" s="47"/>
+      <c r="A18" s="48"/>
       <c r="B18" s="12" t="s">
         <v>211</v>
       </c>
@@ -9630,7 +9767,7 @@
       </c>
     </row>
     <row r="19" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A19" s="47"/>
+      <c r="A19" s="48"/>
       <c r="B19" s="12" t="s">
         <v>219</v>
       </c>
@@ -9808,15 +9945,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
   <documentManagement>
     <iab7cdb7554d4997ae876b11632fa575 xmlns="3cada6dc-2705-46ed-bab2-0b2cd6d935ca">
@@ -9825,6 +9953,15 @@
     <TaxCatchAll xmlns="3cada6dc-2705-46ed-bab2-0b2cd6d935ca"/>
   </documentManagement>
 </p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -9846,14 +9983,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7B5D7682-109C-47ED-9D9D-D061E76CCAD3}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FCC61AA8-C35E-4598-8617-08B80F018AC2}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
@@ -9867,4 +9996,12 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7B5D7682-109C-47ED-9D9D-D061E76CCAD3}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Version 2.1.5 - Version number update in HAST_Inputs.xlsx Updated Load Flow Settings so now the default load flow in PowerFactory can be used.
</commit_message>
<xml_diff>
--- a/HAST_Inputs.xlsx
+++ b/HAST_Inputs.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21328"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FBEF17A-7A0F-4B16-900F-BE6B392B1755}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CE578DF-FC0E-4EE0-9A80-1B5433B92400}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="868" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="868" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cover Sheet" sheetId="10" r:id="rId1"/>
@@ -458,7 +458,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="350" uniqueCount="303">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="353" uniqueCount="305">
   <si>
     <t>Name</t>
   </si>
@@ -1420,6 +1420,12 @@
   </si>
   <si>
     <t>Name of load flow settings to be used for studycase (leave empty to use settings below)</t>
+  </si>
+  <si>
+    <t>V2.1.5</t>
+  </si>
+  <si>
+    <t>1) Added in changes to use Load Flow Command that already exists in PowerFactory rather than inputting settings</t>
   </si>
 </sst>
 </file>
@@ -1822,40 +1828,13 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
   </cellStyles>
-  <dxfs count="10">
+  <dxfs count="5">
     <dxf>
       <fill>
         <patternFill>
           <bgColor rgb="FFFF0000"/>
         </patternFill>
       </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0" tint="-0.499984740745262"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0" tint="-0.499984740745262"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0" tint="-0.499984740745262"/>
-      </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0" tint="-0.499984740745262"/>
-      </font>
     </dxf>
     <dxf>
       <font>
@@ -2223,8 +2202,8 @@
   </sheetPr>
   <dimension ref="A1:D12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A17" sqref="A17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2334,12 +2313,24 @@
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C12" s="4"/>
+      <c r="A12" t="s">
+        <v>304</v>
+      </c>
+      <c r="B12" s="35" t="s">
+        <v>266</v>
+      </c>
+      <c r="C12" s="4">
+        <v>43788</v>
+      </c>
+      <c r="D12" t="s">
+        <v>303</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B10" r:id="rId1" xr:uid="{CC8536B1-0BA0-4FAD-8288-D1AF894BCD4C}"/>
     <hyperlink ref="B11" r:id="rId2" xr:uid="{F4137E57-A552-4C8E-8A40-95C82D83748B}"/>
+    <hyperlink ref="B12" r:id="rId3" xr:uid="{004A820E-03E5-43D2-895B-AC5991D002C3}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -7070,12 +7061,12 @@
     <sortCondition ref="A5:A8"/>
   </sortState>
   <conditionalFormatting sqref="A5:A103">
-    <cfRule type="expression" dxfId="9" priority="3">
+    <cfRule type="expression" dxfId="4" priority="3">
       <formula>LEN(A5)&gt;19</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A3">
-    <cfRule type="expression" dxfId="8" priority="1">
+    <cfRule type="expression" dxfId="3" priority="1">
       <formula>A3="NAMES OKAY"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -8552,7 +8543,7 @@
   <sheetPr codeName="Sheet6"/>
   <dimension ref="A1:G60"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
@@ -9298,17 +9289,17 @@
     <mergeCell ref="A50:A52"/>
   </mergeCells>
   <conditionalFormatting sqref="A5:D60">
-    <cfRule type="expression" dxfId="3" priority="3">
+    <cfRule type="expression" dxfId="2" priority="3">
       <formula>$D$4&lt;&gt;FALSE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A4:D4">
-    <cfRule type="expression" dxfId="5" priority="2">
+    <cfRule type="expression" dxfId="1" priority="2">
       <formula>$D$4=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D4">
-    <cfRule type="expression" dxfId="4" priority="1">
+    <cfRule type="expression" dxfId="0" priority="1">
       <formula>$D$4=""</formula>
     </cfRule>
   </conditionalFormatting>
@@ -9945,6 +9936,15 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
   <documentManagement>
     <iab7cdb7554d4997ae876b11632fa575 xmlns="3cada6dc-2705-46ed-bab2-0b2cd6d935ca">
@@ -9953,15 +9953,6 @@
     <TaxCatchAll xmlns="3cada6dc-2705-46ed-bab2-0b2cd6d935ca"/>
   </documentManagement>
 </p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -9983,6 +9974,14 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7B5D7682-109C-47ED-9D9D-D061E76CCAD3}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FCC61AA8-C35E-4598-8617-08B80F018AC2}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
@@ -9996,12 +9995,4 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7B5D7682-109C-47ED-9D9D-D061E76CCAD3}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>